<commit_message>
removed inflation adjustment in pws cost
Former-commit-id: b3f712eb9b54f2820f1db65e30617642dee84f56
Former-commit-id: 78aec4a48bc58722d974b2b824be05e9aac95b5f
</commit_message>
<xml_diff>
--- a/data/tech-economic-data.xlsx
+++ b/data/tech-economic-data.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\github\i2cner\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9CFC483F-DDB2-439C-BF7F-541D900FC956}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DA6D562A-15C1-491C-82F4-4C862618E513}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" firstSheet="8" activeTab="17" xr2:uid="{ECBC9880-2B97-44EA-9887-629A306A84A1}"/>
   </bookViews>
@@ -23,14 +23,14 @@
     <sheet name="Keipi_SMR" sheetId="5" r:id="rId8"/>
     <sheet name="GARBAGE_KEIPI_CCSSMR" sheetId="9" r:id="rId9"/>
     <sheet name="Keipi_electrolysis" sheetId="8" r:id="rId10"/>
-    <sheet name="Photoconversion" sheetId="16" r:id="rId11"/>
-    <sheet name="AEC" sheetId="21" r:id="rId12"/>
-    <sheet name="PEMEC" sheetId="20" r:id="rId13"/>
-    <sheet name="PEMFC" sheetId="19" r:id="rId14"/>
-    <sheet name="EIA_LCOE_WND_SOLAR" sheetId="11" r:id="rId15"/>
-    <sheet name="SOFC" sheetId="17" r:id="rId16"/>
-    <sheet name="Li-ion" sheetId="12" r:id="rId17"/>
-    <sheet name="SOEC" sheetId="18" r:id="rId18"/>
+    <sheet name="AEC" sheetId="21" r:id="rId11"/>
+    <sheet name="PEMEC" sheetId="20" r:id="rId12"/>
+    <sheet name="PEMFC" sheetId="19" r:id="rId13"/>
+    <sheet name="EIA_LCOE_WND_SOLAR" sheetId="11" r:id="rId14"/>
+    <sheet name="SOFC" sheetId="17" r:id="rId15"/>
+    <sheet name="Li-ion" sheetId="12" r:id="rId16"/>
+    <sheet name="SOEC" sheetId="18" r:id="rId17"/>
+    <sheet name="Photoconversion" sheetId="16" r:id="rId18"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -1300,13 +1300,13 @@
     <xf numFmtId="0" fontId="8" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="1" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="3">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -1679,15 +1679,15 @@
       <c r="C3" t="s">
         <v>176</v>
       </c>
-      <c r="J3" s="26" t="s">
+      <c r="J3" s="27" t="s">
         <v>204</v>
       </c>
-      <c r="K3" s="26"/>
-      <c r="L3" s="26"/>
-      <c r="M3" s="26"/>
-      <c r="N3" s="26"/>
-      <c r="O3" s="26"/>
-      <c r="P3" s="26"/>
+      <c r="K3" s="27"/>
+      <c r="L3" s="27"/>
+      <c r="M3" s="27"/>
+      <c r="N3" s="27"/>
+      <c r="O3" s="27"/>
+      <c r="P3" s="27"/>
     </row>
     <row r="4" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
@@ -2177,15 +2177,15 @@
       <c r="C17" t="s">
         <v>237</v>
       </c>
-      <c r="J17" s="26" t="s">
+      <c r="J17" s="27" t="s">
         <v>209</v>
       </c>
-      <c r="K17" s="26"/>
-      <c r="L17" s="26"/>
-      <c r="M17" s="26"/>
-      <c r="N17" s="26"/>
-      <c r="O17" s="26"/>
-      <c r="P17" s="26"/>
+      <c r="K17" s="27"/>
+      <c r="L17" s="27"/>
+      <c r="M17" s="27"/>
+      <c r="N17" s="27"/>
+      <c r="O17" s="27"/>
+      <c r="P17" s="27"/>
     </row>
     <row r="18" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A18" s="2" t="s">
@@ -2647,15 +2647,15 @@
       <c r="E31">
         <v>0.7</v>
       </c>
-      <c r="J31" s="26" t="s">
+      <c r="J31" s="27" t="s">
         <v>210</v>
       </c>
-      <c r="K31" s="26"/>
-      <c r="L31" s="26"/>
-      <c r="M31" s="26"/>
-      <c r="N31" s="26"/>
-      <c r="O31" s="26"/>
-      <c r="P31" s="26"/>
+      <c r="K31" s="27"/>
+      <c r="L31" s="27"/>
+      <c r="M31" s="27"/>
+      <c r="N31" s="27"/>
+      <c r="O31" s="27"/>
+      <c r="P31" s="27"/>
     </row>
     <row r="32" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A32" s="2" t="s">
@@ -3421,302 +3421,6 @@
 </file>
 
 <file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{403B81F9-D657-42BD-96F8-D40A873BAE34}">
-  <dimension ref="A1:J23"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B9" sqref="B9"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
-  <cols>
-    <col min="1" max="1" width="15.33203125" customWidth="1"/>
-    <col min="2" max="2" width="13.88671875" customWidth="1"/>
-    <col min="4" max="4" width="10" bestFit="1" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A1" t="s">
-        <v>244</v>
-      </c>
-      <c r="B1">
-        <v>377970</v>
-      </c>
-      <c r="C1" t="s">
-        <v>245</v>
-      </c>
-    </row>
-    <row r="2" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A2" t="s">
-        <v>246</v>
-      </c>
-      <c r="B2">
-        <v>251000</v>
-      </c>
-      <c r="C2" t="s">
-        <v>245</v>
-      </c>
-    </row>
-    <row r="3" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A3" t="s">
-        <v>247</v>
-      </c>
-      <c r="B3">
-        <v>7.5</v>
-      </c>
-      <c r="C3" t="s">
-        <v>248</v>
-      </c>
-      <c r="I3">
-        <v>4.0468600000000002E-3</v>
-      </c>
-      <c r="J3" t="s">
-        <v>249</v>
-      </c>
-    </row>
-    <row r="4" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="B4">
-        <f>B3*I3*1000</f>
-        <v>30.351450000000003</v>
-      </c>
-      <c r="C4" t="s">
-        <v>250</v>
-      </c>
-    </row>
-    <row r="5" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A5" t="s">
-        <v>251</v>
-      </c>
-      <c r="B5">
-        <f>300*B4</f>
-        <v>9105.4350000000013</v>
-      </c>
-      <c r="C5" t="s">
-        <v>245</v>
-      </c>
-      <c r="D5">
-        <f>B5*100/B2</f>
-        <v>3.6276633466135464</v>
-      </c>
-      <c r="E5" t="s">
-        <v>258</v>
-      </c>
-    </row>
-    <row r="6" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A6" t="s">
-        <v>261</v>
-      </c>
-      <c r="B6">
-        <f>D6*B2/100</f>
-        <v>12550</v>
-      </c>
-      <c r="D6">
-        <v>5</v>
-      </c>
-      <c r="E6" t="s">
-        <v>258</v>
-      </c>
-    </row>
-    <row r="8" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A8" t="s">
-        <v>263</v>
-      </c>
-      <c r="B8">
-        <v>0.28999999999999998</v>
-      </c>
-    </row>
-    <row r="9" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A9" t="s">
-        <v>176</v>
-      </c>
-      <c r="B9">
-        <v>0.9</v>
-      </c>
-    </row>
-    <row r="10" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A10" t="s">
-        <v>36</v>
-      </c>
-      <c r="B10">
-        <v>20</v>
-      </c>
-      <c r="C10" t="s">
-        <v>145</v>
-      </c>
-    </row>
-    <row r="11" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A11" t="s">
-        <v>252</v>
-      </c>
-      <c r="B11">
-        <v>1000</v>
-      </c>
-      <c r="C11" t="s">
-        <v>253</v>
-      </c>
-      <c r="D11">
-        <f>365.25*B11*B9*B8</f>
-        <v>95330.25</v>
-      </c>
-      <c r="E11" t="s">
-        <v>254</v>
-      </c>
-      <c r="F11">
-        <f>D11*B10</f>
-        <v>1906605</v>
-      </c>
-      <c r="G11" t="s">
-        <v>255</v>
-      </c>
-    </row>
-    <row r="12" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="B12">
-        <f>30*D11/1000000</f>
-        <v>2.8599074999999998</v>
-      </c>
-      <c r="C12" t="s">
-        <v>264</v>
-      </c>
-      <c r="D12">
-        <f>B12*B10</f>
-        <v>57.198149999999998</v>
-      </c>
-      <c r="E12" t="s">
-        <v>265</v>
-      </c>
-    </row>
-    <row r="13" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A13" t="s">
-        <v>256</v>
-      </c>
-      <c r="B13">
-        <f>222881/1000000</f>
-        <v>0.222881</v>
-      </c>
-      <c r="C13" t="s">
-        <v>257</v>
-      </c>
-    </row>
-    <row r="14" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A14" t="s">
-        <v>259</v>
-      </c>
-      <c r="B14">
-        <f>B12/8760</f>
-        <v>3.2647345890410957E-4</v>
-      </c>
-      <c r="C14" t="s">
-        <v>139</v>
-      </c>
-    </row>
-    <row r="15" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A15" t="s">
-        <v>260</v>
-      </c>
-      <c r="B15">
-        <f>B13/B14</f>
-        <v>682.69255561587227</v>
-      </c>
-      <c r="C15" t="s">
-        <v>250</v>
-      </c>
-    </row>
-    <row r="16" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A16" t="s">
-        <v>266</v>
-      </c>
-      <c r="B16">
-        <f>B6/B15</f>
-        <v>18.383091915625716</v>
-      </c>
-      <c r="C16" t="s">
-        <v>139</v>
-      </c>
-    </row>
-    <row r="17" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A17" t="s">
-        <v>87</v>
-      </c>
-      <c r="B17">
-        <f>4.291722*1.3445</f>
-        <v>5.7702202290000004</v>
-      </c>
-      <c r="C17" t="s">
-        <v>52</v>
-      </c>
-    </row>
-    <row r="18" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A18" t="s">
-        <v>124</v>
-      </c>
-      <c r="B18">
-        <f>B17/B14</f>
-        <v>17674.393037551043</v>
-      </c>
-      <c r="C18" t="s">
-        <v>140</v>
-      </c>
-    </row>
-    <row r="19" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A19" t="s">
-        <v>262</v>
-      </c>
-      <c r="B19">
-        <f>(B17*1000000)/F11</f>
-        <v>3.0264371639642191</v>
-      </c>
-      <c r="C19" t="s">
-        <v>113</v>
-      </c>
-      <c r="E19" t="s">
-        <v>267</v>
-      </c>
-      <c r="F19">
-        <v>3</v>
-      </c>
-      <c r="G19" t="s">
-        <v>268</v>
-      </c>
-    </row>
-    <row r="20" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A20" t="s">
-        <v>156</v>
-      </c>
-      <c r="B20">
-        <f>F11*F20/(1000000*B10)</f>
-        <v>9.5330250000000005E-2</v>
-      </c>
-      <c r="C20" t="s">
-        <v>269</v>
-      </c>
-      <c r="E20" t="s">
-        <v>267</v>
-      </c>
-      <c r="F20">
-        <v>1</v>
-      </c>
-      <c r="G20" t="s">
-        <v>268</v>
-      </c>
-    </row>
-    <row r="22" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A22" s="12" t="s">
-        <v>283</v>
-      </c>
-    </row>
-    <row r="23" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="B23" s="12"/>
-    </row>
-  </sheetData>
-  <hyperlinks>
-    <hyperlink ref="A22" r:id="rId1" location="!divAbstract" display="https://pubs.rsc.org/en/content/articlelanding/2013/ee/c3ee40831k - !divAbstract" xr:uid="{92883294-6EE4-4414-BC11-4CB1313D14CB}"/>
-  </hyperlinks>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId2"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9B6BC44C-C965-493C-907E-B5E15FE8A950}">
   <dimension ref="A1:D4"/>
   <sheetViews>
@@ -3772,7 +3476,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet13.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BFB7227C-A1DE-45C0-910C-0F614B128A68}">
   <dimension ref="A1:D9"/>
   <sheetViews>
@@ -3882,7 +3586,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet14.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet13.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FDE08F1C-1E3B-4C4E-8A6D-24A9BDA23FF2}">
   <dimension ref="A1:G15"/>
   <sheetViews>
@@ -4059,7 +3763,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet15.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet14.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{23AAF198-3247-41A0-820F-167859A4EE2B}">
   <dimension ref="A1:R25"/>
   <sheetViews>
@@ -4093,10 +3797,10 @@
         <v>2025</v>
       </c>
       <c r="D3" s="18"/>
-      <c r="E3" s="26">
+      <c r="E3" s="27">
         <v>2040</v>
       </c>
-      <c r="F3" s="26"/>
+      <c r="F3" s="27"/>
       <c r="G3" t="s">
         <v>297</v>
       </c>
@@ -4441,7 +4145,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet16.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet15.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BF0E9B4C-54AC-49FD-862E-E12FD7004C39}">
   <dimension ref="A1:O10"/>
   <sheetViews>
@@ -4582,7 +4286,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet17.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet16.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2E6C6BEB-6091-4743-A766-86BDD24D0263}">
   <dimension ref="A1:J18"/>
   <sheetViews>
@@ -4827,11 +4531,11 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet18.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet17.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5A029AF6-CB84-4D91-9DA5-CC90BF5892BA}">
   <dimension ref="A1:P36"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="P10" sqref="P10"/>
     </sheetView>
   </sheetViews>
@@ -4846,7 +4550,7 @@
       </c>
     </row>
     <row r="2" spans="1:16" x14ac:dyDescent="0.3">
-      <c r="H2" s="28">
+      <c r="H2" s="26">
         <v>0.27779999999999999</v>
       </c>
       <c r="I2" t="s">
@@ -5328,6 +5032,302 @@
     <hyperlink ref="P9" r:id="rId2" xr:uid="{83FB7102-FA60-4FF6-B48E-F6D3561360A3}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet18.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{403B81F9-D657-42BD-96F8-D40A873BAE34}">
+  <dimension ref="A1:J23"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B18" sqref="B18"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="15.33203125" customWidth="1"/>
+    <col min="2" max="2" width="13.88671875" customWidth="1"/>
+    <col min="4" max="4" width="10" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A1" t="s">
+        <v>244</v>
+      </c>
+      <c r="B1">
+        <v>377970</v>
+      </c>
+      <c r="C1" t="s">
+        <v>245</v>
+      </c>
+    </row>
+    <row r="2" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A2" t="s">
+        <v>246</v>
+      </c>
+      <c r="B2">
+        <v>251000</v>
+      </c>
+      <c r="C2" t="s">
+        <v>245</v>
+      </c>
+    </row>
+    <row r="3" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A3" t="s">
+        <v>247</v>
+      </c>
+      <c r="B3">
+        <v>7.5</v>
+      </c>
+      <c r="C3" t="s">
+        <v>248</v>
+      </c>
+      <c r="I3">
+        <v>4.0468600000000002E-3</v>
+      </c>
+      <c r="J3" t="s">
+        <v>249</v>
+      </c>
+    </row>
+    <row r="4" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="B4">
+        <f>B3*I3*1000</f>
+        <v>30.351450000000003</v>
+      </c>
+      <c r="C4" t="s">
+        <v>250</v>
+      </c>
+    </row>
+    <row r="5" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A5" t="s">
+        <v>251</v>
+      </c>
+      <c r="B5">
+        <f>300*B4</f>
+        <v>9105.4350000000013</v>
+      </c>
+      <c r="C5" t="s">
+        <v>245</v>
+      </c>
+      <c r="D5">
+        <f>B5*100/B2</f>
+        <v>3.6276633466135464</v>
+      </c>
+      <c r="E5" t="s">
+        <v>258</v>
+      </c>
+    </row>
+    <row r="6" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A6" t="s">
+        <v>261</v>
+      </c>
+      <c r="B6">
+        <f>D6*B2/100</f>
+        <v>12550</v>
+      </c>
+      <c r="D6">
+        <v>5</v>
+      </c>
+      <c r="E6" t="s">
+        <v>258</v>
+      </c>
+    </row>
+    <row r="8" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A8" t="s">
+        <v>263</v>
+      </c>
+      <c r="B8">
+        <v>0.28999999999999998</v>
+      </c>
+    </row>
+    <row r="9" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A9" t="s">
+        <v>176</v>
+      </c>
+      <c r="B9">
+        <v>0.9</v>
+      </c>
+    </row>
+    <row r="10" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A10" t="s">
+        <v>36</v>
+      </c>
+      <c r="B10">
+        <v>20</v>
+      </c>
+      <c r="C10" t="s">
+        <v>145</v>
+      </c>
+    </row>
+    <row r="11" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A11" t="s">
+        <v>252</v>
+      </c>
+      <c r="B11">
+        <v>1000</v>
+      </c>
+      <c r="C11" t="s">
+        <v>253</v>
+      </c>
+      <c r="D11">
+        <f>365.25*B11*B9*B8</f>
+        <v>95330.25</v>
+      </c>
+      <c r="E11" t="s">
+        <v>254</v>
+      </c>
+      <c r="F11">
+        <f>D11*B10</f>
+        <v>1906605</v>
+      </c>
+      <c r="G11" t="s">
+        <v>255</v>
+      </c>
+    </row>
+    <row r="12" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="B12">
+        <f>30*D11/1000000</f>
+        <v>2.8599074999999998</v>
+      </c>
+      <c r="C12" t="s">
+        <v>264</v>
+      </c>
+      <c r="D12">
+        <f>B12*B10</f>
+        <v>57.198149999999998</v>
+      </c>
+      <c r="E12" t="s">
+        <v>265</v>
+      </c>
+    </row>
+    <row r="13" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A13" t="s">
+        <v>256</v>
+      </c>
+      <c r="B13">
+        <f>222881/1000000</f>
+        <v>0.222881</v>
+      </c>
+      <c r="C13" t="s">
+        <v>257</v>
+      </c>
+    </row>
+    <row r="14" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A14" t="s">
+        <v>259</v>
+      </c>
+      <c r="B14">
+        <f>B12/8760</f>
+        <v>3.2647345890410957E-4</v>
+      </c>
+      <c r="C14" t="s">
+        <v>139</v>
+      </c>
+    </row>
+    <row r="15" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A15" t="s">
+        <v>260</v>
+      </c>
+      <c r="B15">
+        <f>B13/B14</f>
+        <v>682.69255561587227</v>
+      </c>
+      <c r="C15" t="s">
+        <v>250</v>
+      </c>
+    </row>
+    <row r="16" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A16" t="s">
+        <v>266</v>
+      </c>
+      <c r="B16">
+        <f>B6/B15</f>
+        <v>18.383091915625716</v>
+      </c>
+      <c r="C16" t="s">
+        <v>139</v>
+      </c>
+    </row>
+    <row r="17" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A17" t="s">
+        <v>87</v>
+      </c>
+      <c r="B17">
+        <f>4.291722</f>
+        <v>4.291722</v>
+      </c>
+      <c r="C17" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="18" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A18" t="s">
+        <v>124</v>
+      </c>
+      <c r="B18">
+        <f>B17/B14</f>
+        <v>13145.699544478275</v>
+      </c>
+      <c r="C18" t="s">
+        <v>140</v>
+      </c>
+    </row>
+    <row r="19" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A19" t="s">
+        <v>262</v>
+      </c>
+      <c r="B19">
+        <f>(B17*1000000)/F11</f>
+        <v>2.2509759493969645</v>
+      </c>
+      <c r="C19" t="s">
+        <v>113</v>
+      </c>
+      <c r="E19" t="s">
+        <v>267</v>
+      </c>
+      <c r="F19">
+        <v>3</v>
+      </c>
+      <c r="G19" t="s">
+        <v>268</v>
+      </c>
+    </row>
+    <row r="20" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A20" t="s">
+        <v>156</v>
+      </c>
+      <c r="B20">
+        <f>F11*F20/(1000000*B10)</f>
+        <v>9.5330250000000005E-2</v>
+      </c>
+      <c r="C20" t="s">
+        <v>269</v>
+      </c>
+      <c r="E20" t="s">
+        <v>267</v>
+      </c>
+      <c r="F20">
+        <v>1</v>
+      </c>
+      <c r="G20" t="s">
+        <v>268</v>
+      </c>
+    </row>
+    <row r="22" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A22" s="12" t="s">
+        <v>283</v>
+      </c>
+    </row>
+    <row r="23" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="B23" s="12"/>
+    </row>
+  </sheetData>
+  <hyperlinks>
+    <hyperlink ref="A22" r:id="rId1" location="!divAbstract" display="https://pubs.rsc.org/en/content/articlelanding/2013/ee/c3ee40831k - !divAbstract" xr:uid="{92883294-6EE4-4414-BC11-4CB1313D14CB}"/>
+  </hyperlinks>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId2"/>
 </worksheet>
 </file>
 
@@ -5389,15 +5389,15 @@
       <c r="C3" t="s">
         <v>176</v>
       </c>
-      <c r="J3" s="26" t="s">
+      <c r="J3" s="27" t="s">
         <v>204</v>
       </c>
-      <c r="K3" s="26"/>
-      <c r="L3" s="26"/>
-      <c r="M3" s="26"/>
-      <c r="N3" s="26"/>
-      <c r="O3" s="26"/>
-      <c r="P3" s="26"/>
+      <c r="K3" s="27"/>
+      <c r="L3" s="27"/>
+      <c r="M3" s="27"/>
+      <c r="N3" s="27"/>
+      <c r="O3" s="27"/>
+      <c r="P3" s="27"/>
     </row>
     <row r="4" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
@@ -5887,15 +5887,15 @@
       <c r="C17" t="s">
         <v>237</v>
       </c>
-      <c r="J17" s="26" t="s">
+      <c r="J17" s="27" t="s">
         <v>209</v>
       </c>
-      <c r="K17" s="26"/>
-      <c r="L17" s="26"/>
-      <c r="M17" s="26"/>
-      <c r="N17" s="26"/>
-      <c r="O17" s="26"/>
-      <c r="P17" s="26"/>
+      <c r="K17" s="27"/>
+      <c r="L17" s="27"/>
+      <c r="M17" s="27"/>
+      <c r="N17" s="27"/>
+      <c r="O17" s="27"/>
+      <c r="P17" s="27"/>
     </row>
     <row r="18" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A18" s="2" t="s">
@@ -6357,15 +6357,15 @@
       <c r="E31">
         <v>0.7</v>
       </c>
-      <c r="J31" s="26" t="s">
+      <c r="J31" s="27" t="s">
         <v>210</v>
       </c>
-      <c r="K31" s="26"/>
-      <c r="L31" s="26"/>
-      <c r="M31" s="26"/>
-      <c r="N31" s="26"/>
-      <c r="O31" s="26"/>
-      <c r="P31" s="26"/>
+      <c r="K31" s="27"/>
+      <c r="L31" s="27"/>
+      <c r="M31" s="27"/>
+      <c r="N31" s="27"/>
+      <c r="O31" s="27"/>
+      <c r="P31" s="27"/>
     </row>
     <row r="32" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A32" s="2" t="s">
@@ -7009,10 +7009,10 @@
       <c r="G10" t="s">
         <v>92</v>
       </c>
-      <c r="J10" s="27" t="s">
+      <c r="J10" s="28" t="s">
         <v>81</v>
       </c>
-      <c r="K10" s="27"/>
+      <c r="K10" s="28"/>
       <c r="L10" s="11">
         <f>L9/G5</f>
         <v>122583.35123523093</v>
@@ -7022,10 +7022,10 @@
       </c>
     </row>
     <row r="11" spans="1:16" x14ac:dyDescent="0.3">
-      <c r="J11" s="27" t="s">
+      <c r="J11" s="28" t="s">
         <v>82</v>
       </c>
-      <c r="K11" s="27"/>
+      <c r="K11" s="28"/>
       <c r="L11" s="11">
         <f>M4*L10</f>
         <v>4086438.5967776584</v>

</xml_diff>

<commit_message>
added utility scale aec
Former-commit-id: e752a798901455fabfa5c110a2a484f0e48c724d
Former-commit-id: d1908d6f76f3649735c938d313df5e442a7ee36b
</commit_message>
<xml_diff>
--- a/data/tech-economic-data.xlsx
+++ b/data/tech-economic-data.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\github\i2cner\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DA6D562A-15C1-491C-82F4-4C862618E513}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DC608377-38B6-4517-8450-01182D2B8ED4}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" firstSheet="8" activeTab="17" xr2:uid="{ECBC9880-2B97-44EA-9887-629A306A84A1}"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" firstSheet="8" activeTab="11" xr2:uid="{ECBC9880-2B97-44EA-9887-629A306A84A1}"/>
   </bookViews>
   <sheets>
     <sheet name="CCS_Costs_Early" sheetId="14" r:id="rId1"/>
@@ -25,11 +25,11 @@
     <sheet name="Keipi_electrolysis" sheetId="8" r:id="rId10"/>
     <sheet name="AEC" sheetId="21" r:id="rId11"/>
     <sheet name="PEMEC" sheetId="20" r:id="rId12"/>
-    <sheet name="PEMFC" sheetId="19" r:id="rId13"/>
-    <sheet name="EIA_LCOE_WND_SOLAR" sheetId="11" r:id="rId14"/>
-    <sheet name="SOFC" sheetId="17" r:id="rId15"/>
-    <sheet name="Li-ion" sheetId="12" r:id="rId16"/>
-    <sheet name="SOEC" sheetId="18" r:id="rId17"/>
+    <sheet name="SOEC" sheetId="18" r:id="rId13"/>
+    <sheet name="PEMFC" sheetId="19" r:id="rId14"/>
+    <sheet name="EIA_LCOE_WND_SOLAR" sheetId="11" r:id="rId15"/>
+    <sheet name="SOFC" sheetId="17" r:id="rId16"/>
+    <sheet name="Li-ion" sheetId="12" r:id="rId17"/>
     <sheet name="Photoconversion" sheetId="16" r:id="rId18"/>
   </sheets>
   <calcPr calcId="191029"/>
@@ -48,7 +48,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="752" uniqueCount="353">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="756" uniqueCount="356">
   <si>
     <t>H2 Method</t>
   </si>
@@ -1107,6 +1107,15 @@
   </si>
   <si>
     <t>https://doi.org/10.1016/j.ijhydene.2017.10.045</t>
+  </si>
+  <si>
+    <t>https://doi.org/10.1016/j.jclepro.2013.07.048</t>
+  </si>
+  <si>
+    <t>FCV BASED</t>
+  </si>
+  <si>
+    <t>https://doi.org/10.1016/j.ijhydene.2011.10.064</t>
   </si>
 </sst>
 </file>
@@ -3422,10 +3431,10 @@
 
 <file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9B6BC44C-C965-493C-907E-B5E15FE8A950}">
-  <dimension ref="A1:D4"/>
+  <dimension ref="A1:I9"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="I41" sqref="I41"/>
+      <selection activeCell="D6" sqref="D6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -3433,7 +3442,7 @@
     <col min="2" max="2" width="12.33203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.3">
       <c r="B1" t="s">
         <v>308</v>
       </c>
@@ -3443,8 +3452,11 @@
       <c r="D1" s="12" t="s">
         <v>307</v>
       </c>
-    </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="I1" t="s">
+        <v>354</v>
+      </c>
+    </row>
+    <row r="2" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A2">
         <v>2017</v>
       </c>
@@ -3459,18 +3471,51 @@
         <v>316</v>
       </c>
     </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>317</v>
       </c>
       <c r="D4" s="12" t="s">
         <v>315</v>
+      </c>
+    </row>
+    <row r="6" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="B6">
+        <v>43</v>
+      </c>
+      <c r="C6">
+        <f>B6/30</f>
+        <v>1.4333333333333333</v>
+      </c>
+      <c r="D6" s="12" t="s">
+        <v>353</v>
+      </c>
+    </row>
+    <row r="7" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="D7" s="12" t="s">
+        <v>355</v>
+      </c>
+    </row>
+    <row r="9" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="B9">
+        <f>0.04*970</f>
+        <v>38.800000000000004</v>
+      </c>
+      <c r="C9">
+        <f>B9/30</f>
+        <v>1.2933333333333334</v>
+      </c>
+      <c r="D9" s="12" t="s">
+        <v>353</v>
       </c>
     </row>
   </sheetData>
   <hyperlinks>
     <hyperlink ref="D1" r:id="rId1" display="https://urldefense.proofpoint.com/v2/url?u=https-3A__doi.org_10.1016_j.apenergy.2016.07.104&amp;d=DwMFaQ&amp;c=OCIEmEwdEq_aNlsP4fF3gFqSN-E3mlr2t9JcDdfOZag&amp;r=79oVBkpSJ8jc8Mw2l8LuV83qCNXLl72NkphdMlliukM&amp;m=u5UoiluATJYcC_3uLl3rnf_fVd77gqqgvry4u-DXIg4&amp;s=jOLHdWx_MPUn4VVadr0XEHCZPzHvqbpb3Ry75DeUYTw&amp;e=" xr:uid="{3122AE31-A0FC-4B8D-8284-BA98C897AEC6}"/>
     <hyperlink ref="D4" r:id="rId2" tooltip="Persistent link using digital object identifier" xr:uid="{579337F0-0E30-4944-9B30-489BBD332DB7}"/>
+    <hyperlink ref="D6" r:id="rId3" tooltip="Persistent link using digital object identifier" xr:uid="{64767E0B-4603-4888-AC84-3F51EA7C938D}"/>
+    <hyperlink ref="D7" r:id="rId4" tooltip="Persistent link using digital object identifier" display="https://doi-org.proxy2.library.illinois.edu/10.1016/j.ijhydene.2011.10.064" xr:uid="{BDE805AE-877E-4545-BDBE-4D38A75176FA}"/>
+    <hyperlink ref="D9" r:id="rId5" tooltip="Persistent link using digital object identifier" xr:uid="{80D8A260-46EB-4685-A28A-7C308844320C}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -3480,8 +3525,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BFB7227C-A1DE-45C0-910C-0F614B128A68}">
   <dimension ref="A1:D9"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B8" sqref="B8"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D9" sqref="D9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -3502,12 +3547,12 @@
         <v>2017</v>
       </c>
       <c r="B2">
-        <f>29*4/100</f>
-        <v>1.1599999999999999</v>
+        <f>29*1/100</f>
+        <v>0.28999999999999998</v>
       </c>
       <c r="C2">
         <f>B2*1000/33.33</f>
-        <v>34.803480348034803</v>
+        <v>8.7008700870087008</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.3">
@@ -3515,12 +3560,12 @@
         <v>2050</v>
       </c>
       <c r="B3">
-        <f>4*4/100</f>
-        <v>0.16</v>
+        <f>4*1/100</f>
+        <v>0.04</v>
       </c>
       <c r="C3">
         <f>B3*1000/33.33</f>
-        <v>4.8004800480048004</v>
+        <v>1.2001200120012001</v>
       </c>
       <c r="D3" s="12" t="s">
         <v>304</v>
@@ -3541,7 +3586,7 @@
       </c>
       <c r="B6">
         <f>B5*C3</f>
-        <v>144014.40144014402</v>
+        <v>36003.600360036005</v>
       </c>
       <c r="C6" t="s">
         <v>311</v>
@@ -3553,7 +3598,7 @@
       </c>
       <c r="B7">
         <f>B6/(8760*0.9*7)</f>
-        <v>2.609523835619048</v>
+        <v>0.652380958904762</v>
       </c>
       <c r="C7" t="s">
         <v>313</v>
@@ -3565,7 +3610,7 @@
       </c>
       <c r="B8">
         <f>B6/(8760*0.9*10)</f>
-        <v>1.8266666849333335</v>
+        <v>0.45666667123333338</v>
       </c>
       <c r="C8" t="s">
         <v>314</v>
@@ -3587,11 +3632,513 @@
 </file>
 
 <file path=xl/worksheets/sheet13.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5A029AF6-CB84-4D91-9DA5-CC90BF5892BA}">
+  <dimension ref="A1:P36"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="6" max="6" width="11" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="A1" s="12" t="s">
+        <v>322</v>
+      </c>
+    </row>
+    <row r="2" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="H2" s="26">
+        <v>0.27779999999999999</v>
+      </c>
+      <c r="I2" t="s">
+        <v>66</v>
+      </c>
+      <c r="K2" t="s">
+        <v>328</v>
+      </c>
+      <c r="L2">
+        <v>5000</v>
+      </c>
+      <c r="M2" t="s">
+        <v>325</v>
+      </c>
+    </row>
+    <row r="3" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="A3" t="s">
+        <v>36</v>
+      </c>
+      <c r="B3" s="10">
+        <v>20000</v>
+      </c>
+      <c r="C3" t="s">
+        <v>325</v>
+      </c>
+      <c r="D3">
+        <f>B3/(8760*0.9)</f>
+        <v>2.5367833587011668</v>
+      </c>
+      <c r="E3" t="s">
+        <v>145</v>
+      </c>
+      <c r="F3" t="s">
+        <v>348</v>
+      </c>
+      <c r="K3" t="s">
+        <v>331</v>
+      </c>
+      <c r="L3">
+        <v>20000</v>
+      </c>
+      <c r="M3" t="s">
+        <v>325</v>
+      </c>
+    </row>
+    <row r="4" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="B4">
+        <v>60000</v>
+      </c>
+      <c r="C4" t="s">
+        <v>325</v>
+      </c>
+      <c r="D4">
+        <f t="shared" ref="D4:D5" si="0">B4/(8760*0.9)</f>
+        <v>7.6103500761035008</v>
+      </c>
+      <c r="F4">
+        <v>2050</v>
+      </c>
+    </row>
+    <row r="5" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="B5">
+        <v>90000</v>
+      </c>
+      <c r="C5" t="s">
+        <v>325</v>
+      </c>
+      <c r="D5">
+        <f t="shared" si="0"/>
+        <v>11.415525114155251</v>
+      </c>
+      <c r="F5">
+        <v>2070</v>
+      </c>
+    </row>
+    <row r="9" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="A9" t="s">
+        <v>323</v>
+      </c>
+      <c r="J9" t="s">
+        <v>349</v>
+      </c>
+      <c r="P9" s="12" t="s">
+        <v>352</v>
+      </c>
+    </row>
+    <row r="10" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="A10" t="s">
+        <v>324</v>
+      </c>
+      <c r="J10">
+        <v>2017</v>
+      </c>
+      <c r="K10">
+        <v>8000</v>
+      </c>
+      <c r="L10" t="s">
+        <v>350</v>
+      </c>
+      <c r="M10">
+        <f>1.11*K10</f>
+        <v>8880</v>
+      </c>
+      <c r="N10" t="s">
+        <v>351</v>
+      </c>
+    </row>
+    <row r="11" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="A11">
+        <v>2030</v>
+      </c>
+      <c r="B11">
+        <f>(107.7+107.8+108.8)/3</f>
+        <v>108.10000000000001</v>
+      </c>
+      <c r="C11" t="s">
+        <v>326</v>
+      </c>
+      <c r="D11">
+        <f>B11*1000/(B3)</f>
+        <v>5.4050000000000011</v>
+      </c>
+      <c r="E11" t="s">
+        <v>119</v>
+      </c>
+      <c r="J11">
+        <v>2030</v>
+      </c>
+      <c r="K11">
+        <v>5500</v>
+      </c>
+      <c r="L11" t="s">
+        <v>350</v>
+      </c>
+      <c r="M11">
+        <f t="shared" ref="M11:M13" si="1">1.11*K11</f>
+        <v>6105.0000000000009</v>
+      </c>
+      <c r="N11" t="s">
+        <v>351</v>
+      </c>
+    </row>
+    <row r="12" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="A12">
+        <v>2040</v>
+      </c>
+      <c r="B12">
+        <f>0.6*B11</f>
+        <v>64.86</v>
+      </c>
+      <c r="C12" t="s">
+        <v>326</v>
+      </c>
+      <c r="D12">
+        <f>B12*1000/(B3)</f>
+        <v>3.2429999999999999</v>
+      </c>
+      <c r="E12" t="s">
+        <v>119</v>
+      </c>
+      <c r="J12">
+        <v>2050</v>
+      </c>
+      <c r="K12">
+        <v>1000</v>
+      </c>
+      <c r="L12" t="s">
+        <v>350</v>
+      </c>
+      <c r="M12">
+        <f t="shared" si="1"/>
+        <v>1110</v>
+      </c>
+      <c r="N12" t="s">
+        <v>351</v>
+      </c>
+    </row>
+    <row r="13" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="A13">
+        <v>2050</v>
+      </c>
+      <c r="B13">
+        <v>64.86</v>
+      </c>
+      <c r="D13">
+        <f>B13*1000/B4</f>
+        <v>1.081</v>
+      </c>
+      <c r="E13" t="s">
+        <v>119</v>
+      </c>
+      <c r="J13">
+        <v>2070</v>
+      </c>
+      <c r="K13">
+        <v>400</v>
+      </c>
+      <c r="L13" t="s">
+        <v>350</v>
+      </c>
+      <c r="M13">
+        <f t="shared" si="1"/>
+        <v>444.00000000000006</v>
+      </c>
+      <c r="N13" t="s">
+        <v>351</v>
+      </c>
+    </row>
+    <row r="14" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="A14">
+        <v>2070</v>
+      </c>
+      <c r="B14">
+        <v>64.86</v>
+      </c>
+      <c r="D14">
+        <f>B14*1000/B5</f>
+        <v>0.72066666666666668</v>
+      </c>
+      <c r="E14" t="s">
+        <v>119</v>
+      </c>
+    </row>
+    <row r="24" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A24" t="s">
+        <v>327</v>
+      </c>
+    </row>
+    <row r="25" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A25" t="s">
+        <v>328</v>
+      </c>
+      <c r="B25">
+        <v>52.2</v>
+      </c>
+      <c r="C25" t="s">
+        <v>118</v>
+      </c>
+      <c r="D25">
+        <f>B25/$H$2</f>
+        <v>187.9049676025918</v>
+      </c>
+      <c r="E25" t="s">
+        <v>119</v>
+      </c>
+      <c r="F25">
+        <f>D25*L2/1000</f>
+        <v>939.52483801295898</v>
+      </c>
+    </row>
+    <row r="26" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A26" t="s">
+        <v>329</v>
+      </c>
+      <c r="B26">
+        <v>46.7</v>
+      </c>
+      <c r="C26" t="s">
+        <v>118</v>
+      </c>
+      <c r="D26">
+        <f t="shared" ref="D26:D27" si="2">B26/$H$2</f>
+        <v>168.10655147588196</v>
+      </c>
+      <c r="E26" t="s">
+        <v>119</v>
+      </c>
+      <c r="F26">
+        <f>D26*L3/1000</f>
+        <v>3362.131029517639</v>
+      </c>
+    </row>
+    <row r="27" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A27" t="s">
+        <v>330</v>
+      </c>
+      <c r="B27">
+        <v>41.6</v>
+      </c>
+      <c r="C27" t="s">
+        <v>118</v>
+      </c>
+      <c r="D27">
+        <f t="shared" si="2"/>
+        <v>149.74802015838733</v>
+      </c>
+      <c r="E27" t="s">
+        <v>119</v>
+      </c>
+      <c r="F27">
+        <f>D27*L3/1000</f>
+        <v>2994.9604031677463</v>
+      </c>
+    </row>
+    <row r="29" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A29" t="s">
+        <v>332</v>
+      </c>
+    </row>
+    <row r="30" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A30" t="s">
+        <v>17</v>
+      </c>
+      <c r="B30">
+        <v>5881</v>
+      </c>
+      <c r="C30" t="s">
+        <v>333</v>
+      </c>
+      <c r="D30">
+        <f>B30*H2</f>
+        <v>1633.7418</v>
+      </c>
+      <c r="E30" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="31" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A31" t="s">
+        <v>93</v>
+      </c>
+      <c r="K31" s="2"/>
+      <c r="L31" t="s">
+        <v>346</v>
+      </c>
+    </row>
+    <row r="32" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A32" t="s">
+        <v>339</v>
+      </c>
+      <c r="B32" t="s">
+        <v>334</v>
+      </c>
+      <c r="C32" t="s">
+        <v>335</v>
+      </c>
+      <c r="D32" t="s">
+        <v>338</v>
+      </c>
+      <c r="E32" t="s">
+        <v>336</v>
+      </c>
+      <c r="F32" t="s">
+        <v>337</v>
+      </c>
+      <c r="I32" t="s">
+        <v>342</v>
+      </c>
+      <c r="K32">
+        <f>4.08/(4.08+3.69+0.58)</f>
+        <v>0.488622754491018</v>
+      </c>
+      <c r="L32">
+        <v>943</v>
+      </c>
+    </row>
+    <row r="33" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A33" t="s">
+        <v>340</v>
+      </c>
+      <c r="B33">
+        <f>6*H2</f>
+        <v>1.6667999999999998</v>
+      </c>
+      <c r="C33">
+        <f>283*H2</f>
+        <v>78.617400000000004</v>
+      </c>
+      <c r="D33">
+        <f>38*H2</f>
+        <v>10.5564</v>
+      </c>
+      <c r="E33">
+        <f>1230*H2</f>
+        <v>341.69400000000002</v>
+      </c>
+      <c r="F33">
+        <f>4323*H2</f>
+        <v>1200.9294</v>
+      </c>
+      <c r="G33" t="s">
+        <v>74</v>
+      </c>
+      <c r="I33" t="s">
+        <v>343</v>
+      </c>
+      <c r="K33">
+        <f>3.69/(4.08+3.69+0.58)</f>
+        <v>0.44191616766467068</v>
+      </c>
+      <c r="L33">
+        <v>599</v>
+      </c>
+    </row>
+    <row r="34" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A34" t="s">
+        <v>341</v>
+      </c>
+      <c r="B34">
+        <f>11.5</f>
+        <v>11.5</v>
+      </c>
+      <c r="C34">
+        <v>24</v>
+      </c>
+      <c r="D34">
+        <v>230</v>
+      </c>
+      <c r="E34">
+        <v>777.43592814371266</v>
+      </c>
+      <c r="F34">
+        <v>12</v>
+      </c>
+      <c r="G34" t="s">
+        <v>119</v>
+      </c>
+      <c r="I34" t="s">
+        <v>344</v>
+      </c>
+      <c r="K34">
+        <f>0.58/(4.08+3.69+0.58)</f>
+        <v>6.9461077844311381E-2</v>
+      </c>
+      <c r="L34">
+        <v>748</v>
+      </c>
+    </row>
+    <row r="35" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A35" t="s">
+        <v>346</v>
+      </c>
+      <c r="B35">
+        <f>B34*B33</f>
+        <v>19.168199999999999</v>
+      </c>
+      <c r="C35">
+        <f t="shared" ref="C35:F35" si="3">C34*C33</f>
+        <v>1886.8176000000001</v>
+      </c>
+      <c r="D35">
+        <f t="shared" si="3"/>
+        <v>2427.9720000000002</v>
+      </c>
+      <c r="E35">
+        <f t="shared" si="3"/>
+        <v>265645.19203113776</v>
+      </c>
+      <c r="F35">
+        <f t="shared" si="3"/>
+        <v>14411.1528</v>
+      </c>
+      <c r="G35" t="s">
+        <v>347</v>
+      </c>
+      <c r="I35" t="s">
+        <v>345</v>
+      </c>
+      <c r="L35">
+        <f>(K32*L32)+(K33*L33)+(K34*L34)</f>
+        <v>777.43592814371266</v>
+      </c>
+    </row>
+    <row r="36" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A36" t="s">
+        <v>17</v>
+      </c>
+      <c r="F36">
+        <f>SUM(B35:F35)/1000</f>
+        <v>284.39030263113773</v>
+      </c>
+      <c r="G36" t="s">
+        <v>73</v>
+      </c>
+    </row>
+  </sheetData>
+  <hyperlinks>
+    <hyperlink ref="A1" r:id="rId1" tooltip="Persistent link using digital object identifier" xr:uid="{02408BA4-1641-4ED4-B210-4315E996BE1B}"/>
+    <hyperlink ref="P9" r:id="rId2" xr:uid="{83FB7102-FA60-4FF6-B48E-F6D3561360A3}"/>
+  </hyperlinks>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet14.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FDE08F1C-1E3B-4C4E-8A6D-24A9BDA23FF2}">
   <dimension ref="A1:G15"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D30" sqref="D30"/>
+      <selection activeCell="F24" sqref="F24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -3763,7 +4310,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet14.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet15.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{23AAF198-3247-41A0-820F-167859A4EE2B}">
   <dimension ref="A1:R25"/>
   <sheetViews>
@@ -4145,7 +4692,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet15.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet16.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BF0E9B4C-54AC-49FD-862E-E12FD7004C39}">
   <dimension ref="A1:O10"/>
   <sheetViews>
@@ -4286,7 +4833,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet16.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet17.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2E6C6BEB-6091-4743-A766-86BDD24D0263}">
   <dimension ref="A1:J18"/>
   <sheetViews>
@@ -4531,515 +5078,11 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet17.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5A029AF6-CB84-4D91-9DA5-CC90BF5892BA}">
-  <dimension ref="A1:P36"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="P10" sqref="P10"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
-  <cols>
-    <col min="6" max="6" width="11" bestFit="1" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:16" x14ac:dyDescent="0.3">
-      <c r="A1" s="12" t="s">
-        <v>322</v>
-      </c>
-    </row>
-    <row r="2" spans="1:16" x14ac:dyDescent="0.3">
-      <c r="H2" s="26">
-        <v>0.27779999999999999</v>
-      </c>
-      <c r="I2" t="s">
-        <v>66</v>
-      </c>
-      <c r="K2" t="s">
-        <v>328</v>
-      </c>
-      <c r="L2">
-        <v>5000</v>
-      </c>
-      <c r="M2" t="s">
-        <v>325</v>
-      </c>
-    </row>
-    <row r="3" spans="1:16" x14ac:dyDescent="0.3">
-      <c r="A3" t="s">
-        <v>36</v>
-      </c>
-      <c r="B3" s="10">
-        <v>20000</v>
-      </c>
-      <c r="C3" t="s">
-        <v>325</v>
-      </c>
-      <c r="D3">
-        <f>B3/(8760*0.9)</f>
-        <v>2.5367833587011668</v>
-      </c>
-      <c r="E3" t="s">
-        <v>145</v>
-      </c>
-      <c r="F3" t="s">
-        <v>348</v>
-      </c>
-      <c r="K3" t="s">
-        <v>331</v>
-      </c>
-      <c r="L3">
-        <v>20000</v>
-      </c>
-      <c r="M3" t="s">
-        <v>325</v>
-      </c>
-    </row>
-    <row r="4" spans="1:16" x14ac:dyDescent="0.3">
-      <c r="B4">
-        <v>60000</v>
-      </c>
-      <c r="C4" t="s">
-        <v>325</v>
-      </c>
-      <c r="D4">
-        <f t="shared" ref="D4:D5" si="0">B4/(8760*0.9)</f>
-        <v>7.6103500761035008</v>
-      </c>
-      <c r="F4">
-        <v>2050</v>
-      </c>
-    </row>
-    <row r="5" spans="1:16" x14ac:dyDescent="0.3">
-      <c r="B5">
-        <v>90000</v>
-      </c>
-      <c r="C5" t="s">
-        <v>325</v>
-      </c>
-      <c r="D5">
-        <f t="shared" si="0"/>
-        <v>11.415525114155251</v>
-      </c>
-      <c r="F5">
-        <v>2070</v>
-      </c>
-    </row>
-    <row r="9" spans="1:16" x14ac:dyDescent="0.3">
-      <c r="A9" t="s">
-        <v>323</v>
-      </c>
-      <c r="J9" t="s">
-        <v>349</v>
-      </c>
-      <c r="P9" s="12" t="s">
-        <v>352</v>
-      </c>
-    </row>
-    <row r="10" spans="1:16" x14ac:dyDescent="0.3">
-      <c r="A10" t="s">
-        <v>324</v>
-      </c>
-      <c r="J10">
-        <v>2017</v>
-      </c>
-      <c r="K10">
-        <v>8000</v>
-      </c>
-      <c r="L10" t="s">
-        <v>350</v>
-      </c>
-      <c r="M10">
-        <f>1.11*K10</f>
-        <v>8880</v>
-      </c>
-      <c r="N10" t="s">
-        <v>351</v>
-      </c>
-    </row>
-    <row r="11" spans="1:16" x14ac:dyDescent="0.3">
-      <c r="A11">
-        <v>2030</v>
-      </c>
-      <c r="B11">
-        <f>(107.7+107.8+108.8)/3</f>
-        <v>108.10000000000001</v>
-      </c>
-      <c r="C11" t="s">
-        <v>326</v>
-      </c>
-      <c r="D11">
-        <f>B11*1000/(B3)</f>
-        <v>5.4050000000000011</v>
-      </c>
-      <c r="E11" t="s">
-        <v>119</v>
-      </c>
-      <c r="J11">
-        <v>2030</v>
-      </c>
-      <c r="K11">
-        <v>5500</v>
-      </c>
-      <c r="L11" t="s">
-        <v>350</v>
-      </c>
-      <c r="M11">
-        <f t="shared" ref="M11:M13" si="1">1.11*K11</f>
-        <v>6105.0000000000009</v>
-      </c>
-      <c r="N11" t="s">
-        <v>351</v>
-      </c>
-    </row>
-    <row r="12" spans="1:16" x14ac:dyDescent="0.3">
-      <c r="A12">
-        <v>2040</v>
-      </c>
-      <c r="B12">
-        <f>0.6*B11</f>
-        <v>64.86</v>
-      </c>
-      <c r="C12" t="s">
-        <v>326</v>
-      </c>
-      <c r="D12">
-        <f>B12*1000/(B3)</f>
-        <v>3.2429999999999999</v>
-      </c>
-      <c r="E12" t="s">
-        <v>119</v>
-      </c>
-      <c r="J12">
-        <v>2050</v>
-      </c>
-      <c r="K12">
-        <v>1000</v>
-      </c>
-      <c r="L12" t="s">
-        <v>350</v>
-      </c>
-      <c r="M12">
-        <f t="shared" si="1"/>
-        <v>1110</v>
-      </c>
-      <c r="N12" t="s">
-        <v>351</v>
-      </c>
-    </row>
-    <row r="13" spans="1:16" x14ac:dyDescent="0.3">
-      <c r="A13">
-        <v>2050</v>
-      </c>
-      <c r="B13">
-        <v>64.86</v>
-      </c>
-      <c r="D13">
-        <f>B13*1000/B4</f>
-        <v>1.081</v>
-      </c>
-      <c r="E13" t="s">
-        <v>119</v>
-      </c>
-      <c r="J13">
-        <v>2070</v>
-      </c>
-      <c r="K13">
-        <v>400</v>
-      </c>
-      <c r="L13" t="s">
-        <v>350</v>
-      </c>
-      <c r="M13">
-        <f t="shared" si="1"/>
-        <v>444.00000000000006</v>
-      </c>
-      <c r="N13" t="s">
-        <v>351</v>
-      </c>
-    </row>
-    <row r="14" spans="1:16" x14ac:dyDescent="0.3">
-      <c r="A14">
-        <v>2070</v>
-      </c>
-      <c r="B14">
-        <v>64.86</v>
-      </c>
-      <c r="D14">
-        <f>B14*1000/B5</f>
-        <v>0.72066666666666668</v>
-      </c>
-      <c r="E14" t="s">
-        <v>119</v>
-      </c>
-    </row>
-    <row r="24" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A24" t="s">
-        <v>327</v>
-      </c>
-    </row>
-    <row r="25" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A25" t="s">
-        <v>328</v>
-      </c>
-      <c r="B25">
-        <v>52.2</v>
-      </c>
-      <c r="C25" t="s">
-        <v>118</v>
-      </c>
-      <c r="D25">
-        <f>B25/$H$2</f>
-        <v>187.9049676025918</v>
-      </c>
-      <c r="E25" t="s">
-        <v>119</v>
-      </c>
-      <c r="F25">
-        <f>D25*L2/1000</f>
-        <v>939.52483801295898</v>
-      </c>
-    </row>
-    <row r="26" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A26" t="s">
-        <v>329</v>
-      </c>
-      <c r="B26">
-        <v>46.7</v>
-      </c>
-      <c r="C26" t="s">
-        <v>118</v>
-      </c>
-      <c r="D26">
-        <f t="shared" ref="D26:D27" si="2">B26/$H$2</f>
-        <v>168.10655147588196</v>
-      </c>
-      <c r="E26" t="s">
-        <v>119</v>
-      </c>
-      <c r="F26">
-        <f>D26*L3/1000</f>
-        <v>3362.131029517639</v>
-      </c>
-    </row>
-    <row r="27" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A27" t="s">
-        <v>330</v>
-      </c>
-      <c r="B27">
-        <v>41.6</v>
-      </c>
-      <c r="C27" t="s">
-        <v>118</v>
-      </c>
-      <c r="D27">
-        <f t="shared" si="2"/>
-        <v>149.74802015838733</v>
-      </c>
-      <c r="E27" t="s">
-        <v>119</v>
-      </c>
-      <c r="F27">
-        <f>D27*L3/1000</f>
-        <v>2994.9604031677463</v>
-      </c>
-    </row>
-    <row r="29" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A29" t="s">
-        <v>332</v>
-      </c>
-    </row>
-    <row r="30" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A30" t="s">
-        <v>17</v>
-      </c>
-      <c r="B30">
-        <v>5881</v>
-      </c>
-      <c r="C30" t="s">
-        <v>333</v>
-      </c>
-      <c r="D30">
-        <f>B30*H2</f>
-        <v>1633.7418</v>
-      </c>
-      <c r="E30" t="s">
-        <v>74</v>
-      </c>
-    </row>
-    <row r="31" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A31" t="s">
-        <v>93</v>
-      </c>
-      <c r="K31" s="2"/>
-      <c r="L31" t="s">
-        <v>346</v>
-      </c>
-    </row>
-    <row r="32" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A32" t="s">
-        <v>339</v>
-      </c>
-      <c r="B32" t="s">
-        <v>334</v>
-      </c>
-      <c r="C32" t="s">
-        <v>335</v>
-      </c>
-      <c r="D32" t="s">
-        <v>338</v>
-      </c>
-      <c r="E32" t="s">
-        <v>336</v>
-      </c>
-      <c r="F32" t="s">
-        <v>337</v>
-      </c>
-      <c r="I32" t="s">
-        <v>342</v>
-      </c>
-      <c r="K32">
-        <f>4.08/(4.08+3.69+0.58)</f>
-        <v>0.488622754491018</v>
-      </c>
-      <c r="L32">
-        <v>943</v>
-      </c>
-    </row>
-    <row r="33" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A33" t="s">
-        <v>340</v>
-      </c>
-      <c r="B33">
-        <f>6*H2</f>
-        <v>1.6667999999999998</v>
-      </c>
-      <c r="C33">
-        <f>283*H2</f>
-        <v>78.617400000000004</v>
-      </c>
-      <c r="D33">
-        <f>38*H2</f>
-        <v>10.5564</v>
-      </c>
-      <c r="E33">
-        <f>1230*H2</f>
-        <v>341.69400000000002</v>
-      </c>
-      <c r="F33">
-        <f>4323*H2</f>
-        <v>1200.9294</v>
-      </c>
-      <c r="G33" t="s">
-        <v>74</v>
-      </c>
-      <c r="I33" t="s">
-        <v>343</v>
-      </c>
-      <c r="K33">
-        <f>3.69/(4.08+3.69+0.58)</f>
-        <v>0.44191616766467068</v>
-      </c>
-      <c r="L33">
-        <v>599</v>
-      </c>
-    </row>
-    <row r="34" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A34" t="s">
-        <v>341</v>
-      </c>
-      <c r="B34">
-        <f>11.5</f>
-        <v>11.5</v>
-      </c>
-      <c r="C34">
-        <v>24</v>
-      </c>
-      <c r="D34">
-        <v>230</v>
-      </c>
-      <c r="E34">
-        <v>777.43592814371266</v>
-      </c>
-      <c r="F34">
-        <v>12</v>
-      </c>
-      <c r="G34" t="s">
-        <v>119</v>
-      </c>
-      <c r="I34" t="s">
-        <v>344</v>
-      </c>
-      <c r="K34">
-        <f>0.58/(4.08+3.69+0.58)</f>
-        <v>6.9461077844311381E-2</v>
-      </c>
-      <c r="L34">
-        <v>748</v>
-      </c>
-    </row>
-    <row r="35" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A35" t="s">
-        <v>346</v>
-      </c>
-      <c r="B35">
-        <f>B34*B33</f>
-        <v>19.168199999999999</v>
-      </c>
-      <c r="C35">
-        <f t="shared" ref="C35:F35" si="3">C34*C33</f>
-        <v>1886.8176000000001</v>
-      </c>
-      <c r="D35">
-        <f t="shared" si="3"/>
-        <v>2427.9720000000002</v>
-      </c>
-      <c r="E35">
-        <f t="shared" si="3"/>
-        <v>265645.19203113776</v>
-      </c>
-      <c r="F35">
-        <f t="shared" si="3"/>
-        <v>14411.1528</v>
-      </c>
-      <c r="G35" t="s">
-        <v>347</v>
-      </c>
-      <c r="I35" t="s">
-        <v>345</v>
-      </c>
-      <c r="L35">
-        <f>(K32*L32)+(K33*L33)+(K34*L34)</f>
-        <v>777.43592814371266</v>
-      </c>
-    </row>
-    <row r="36" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A36" t="s">
-        <v>17</v>
-      </c>
-      <c r="F36">
-        <f>SUM(B35:F35)/1000</f>
-        <v>284.39030263113773</v>
-      </c>
-      <c r="G36" t="s">
-        <v>73</v>
-      </c>
-    </row>
-  </sheetData>
-  <hyperlinks>
-    <hyperlink ref="A1" r:id="rId1" tooltip="Persistent link using digital object identifier" xr:uid="{02408BA4-1641-4ED4-B210-4315E996BE1B}"/>
-    <hyperlink ref="P9" r:id="rId2" xr:uid="{83FB7102-FA60-4FF6-B48E-F6D3561360A3}"/>
-  </hyperlinks>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
 <file path=xl/worksheets/sheet18.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{403B81F9-D657-42BD-96F8-D40A873BAE34}">
   <dimension ref="A1:J23"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="B18" sqref="B18"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
added ccs lifecycle emissions
Former-commit-id: 56b5d9172b37cf64a13fbcc80652f57bff9a985d
Former-commit-id: 359488cfa9d96e1f7b3cf386ef39c04ab7db0d62
</commit_message>
<xml_diff>
--- a/data/tech-economic-data.xlsx
+++ b/data/tech-economic-data.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\github\i2cner\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5BF2E3F7-64AD-4462-B65B-0AA5B51C2F7E}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{88371D5E-61CC-4AB5-BE31-95A64361A5F6}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" firstSheet="7" activeTab="15" xr2:uid="{ECBC9880-2B97-44EA-9887-629A306A84A1}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{ECBC9880-2B97-44EA-9887-629A306A84A1}"/>
   </bookViews>
   <sheets>
     <sheet name="CCS_Costs_Early" sheetId="14" r:id="rId1"/>
@@ -21,10 +21,10 @@
     <sheet name="Keipi_SMR" sheetId="5" r:id="rId6"/>
     <sheet name="Keipi_SMR+CCS" sheetId="9" r:id="rId7"/>
     <sheet name="Keipi_electrolysis" sheetId="8" r:id="rId8"/>
-    <sheet name="PEMEC" sheetId="20" r:id="rId9"/>
-    <sheet name="AEC" sheetId="21" r:id="rId10"/>
-    <sheet name="SOEC" sheetId="18" r:id="rId11"/>
-    <sheet name="Li-ion" sheetId="12" r:id="rId12"/>
+    <sheet name="Li-ion" sheetId="12" r:id="rId9"/>
+    <sheet name="PEMEC" sheetId="20" r:id="rId10"/>
+    <sheet name="AEC" sheetId="21" r:id="rId11"/>
+    <sheet name="SOEC" sheetId="18" r:id="rId12"/>
     <sheet name="SOFC" sheetId="17" r:id="rId13"/>
     <sheet name="PEMFC" sheetId="19" r:id="rId14"/>
     <sheet name="EIA_LCOE_WND_SOLAR" sheetId="11" r:id="rId15"/>
@@ -46,7 +46,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="748" uniqueCount="375">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="762" uniqueCount="387">
   <si>
     <t>H2 Method</t>
   </si>
@@ -1171,6 +1171,42 @@
   </si>
   <si>
     <t>neglected</t>
+  </si>
+  <si>
+    <t>https://doi.org/10.1017/CBO9781107415416</t>
+  </si>
+  <si>
+    <t>Life Cycle Emissions</t>
+  </si>
+  <si>
+    <t>CCS PC</t>
+  </si>
+  <si>
+    <t>Total Emi</t>
+  </si>
+  <si>
+    <t>Direct Emi</t>
+  </si>
+  <si>
+    <t>CCS Gas CC</t>
+  </si>
+  <si>
+    <t>https://www.energy.gov/sites/prod/files/2014/03/f12/27637.pdf</t>
+  </si>
+  <si>
+    <t>Steam reforming+CCS</t>
+  </si>
+  <si>
+    <t>PC</t>
+  </si>
+  <si>
+    <t>Gas CC</t>
+  </si>
+  <si>
+    <t>CO2 Cap</t>
+  </si>
+  <si>
+    <t>Emi build</t>
   </si>
 </sst>
 </file>
@@ -1181,7 +1217,7 @@
     <numFmt numFmtId="164" formatCode="0.000E+00"/>
     <numFmt numFmtId="165" formatCode="0.00000000E+00"/>
   </numFmts>
-  <fonts count="15" x14ac:knownFonts="1">
+  <fonts count="16" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -1285,6 +1321,12 @@
       <name val="Arial"/>
       <family val="2"/>
     </font>
+    <font>
+      <sz val="8"/>
+      <color rgb="FF006FCA"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
   </fonts>
   <fills count="7">
     <fill>
@@ -1353,7 +1395,7 @@
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="10" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="31">
+  <cellXfs count="32">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -1388,15 +1430,16 @@
     <xf numFmtId="0" fontId="1" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="13" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="2" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="11" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="2" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="11" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="3">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -1713,10 +1756,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DA3B25EB-4023-477D-80C4-74718858ACC8}">
-  <dimension ref="A1:P44"/>
+  <dimension ref="A1:P50"/>
   <sheetViews>
-    <sheetView topLeftCell="B16" workbookViewId="0">
-      <selection activeCell="J33" sqref="J33"/>
+    <sheetView tabSelected="1" topLeftCell="A31" workbookViewId="0">
+      <selection activeCell="B47" sqref="B47"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1769,15 +1812,15 @@
       <c r="C3" t="s">
         <v>161</v>
       </c>
-      <c r="J3" s="26" t="s">
+      <c r="J3" s="29" t="s">
         <v>188</v>
       </c>
-      <c r="K3" s="26"/>
-      <c r="L3" s="26"/>
-      <c r="M3" s="26"/>
-      <c r="N3" s="26"/>
-      <c r="O3" s="26"/>
-      <c r="P3" s="26"/>
+      <c r="K3" s="29"/>
+      <c r="L3" s="29"/>
+      <c r="M3" s="29"/>
+      <c r="N3" s="29"/>
+      <c r="O3" s="29"/>
+      <c r="P3" s="29"/>
     </row>
     <row r="4" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
@@ -1825,27 +1868,27 @@
       </c>
       <c r="K5">
         <f t="shared" ref="K5:K15" si="0">$B$36*J5</f>
-        <v>3.4000000000000002E-4</v>
+        <v>3.145E-4</v>
       </c>
       <c r="L5">
         <f>K5*$B$12</f>
-        <v>0.23388222246400001</v>
+        <v>0.2290910557792</v>
       </c>
       <c r="M5">
         <f>K5*$B$21</f>
-        <v>4.4472000000000005E-2</v>
+        <v>4.1136600000000002E-2</v>
       </c>
       <c r="N5">
         <f t="shared" ref="N5:N15" si="1">L5/$L$10</f>
-        <v>0.94444444444444453</v>
+        <v>0.94444444444444442</v>
       </c>
       <c r="O5">
         <f t="shared" ref="O5:O15" si="2">$B$15/N5</f>
-        <v>0.42211529395200004</v>
+        <v>0.42539782337618831</v>
       </c>
       <c r="P5">
         <f t="shared" ref="P5:P15" si="3">$D$30+M5</f>
-        <v>5.0292000000000003E-2</v>
+        <v>4.6956600000000001E-2</v>
       </c>
     </row>
     <row r="6" spans="1:16" x14ac:dyDescent="0.3">
@@ -1866,15 +1909,15 @@
       </c>
       <c r="K6">
         <f t="shared" si="0"/>
-        <v>3.4400000000000001E-4</v>
+        <v>3.1819999999999998E-4</v>
       </c>
       <c r="L6">
         <f t="shared" ref="L6:L15" si="4">K6*$B$12</f>
-        <v>0.23663377802239999</v>
+        <v>0.23178624467071998</v>
       </c>
       <c r="M6">
         <f t="shared" ref="M6:M15" si="5">K6*$B$21</f>
-        <v>4.4995200000000006E-2</v>
+        <v>4.1620560000000001E-2</v>
       </c>
       <c r="N6">
         <f t="shared" si="1"/>
@@ -1882,21 +1925,21 @@
       </c>
       <c r="O6">
         <f t="shared" si="2"/>
-        <v>0.41720697658046524</v>
+        <v>0.42045133705786053</v>
       </c>
       <c r="P6">
         <f t="shared" si="3"/>
-        <v>5.0815200000000005E-2</v>
+        <v>4.744056E-2</v>
       </c>
     </row>
     <row r="7" spans="1:16" x14ac:dyDescent="0.3">
       <c r="B7">
         <f>B36*0.9</f>
-        <v>3.6000000000000002E-4</v>
+        <v>3.3300000000000002E-4</v>
       </c>
       <c r="C7">
         <f>0.9*B35</f>
-        <v>8.4780000000000001E-4</v>
+        <v>6.8400000000000004E-4</v>
       </c>
       <c r="E7" t="s">
         <v>201</v>
@@ -1906,15 +1949,15 @@
       </c>
       <c r="K7">
         <f t="shared" si="0"/>
-        <v>3.48E-4</v>
+        <v>3.2190000000000002E-4</v>
       </c>
       <c r="L7">
         <f t="shared" si="4"/>
-        <v>0.2393853335808</v>
+        <v>0.23448143356223999</v>
       </c>
       <c r="M7">
         <f t="shared" si="5"/>
-        <v>4.5518400000000007E-2</v>
+        <v>4.2104520000000006E-2</v>
       </c>
       <c r="N7">
         <f t="shared" si="1"/>
@@ -1922,21 +1965,21 @@
       </c>
       <c r="O7">
         <f t="shared" si="2"/>
-        <v>0.41241149409103456</v>
+        <v>0.41561856306868972</v>
       </c>
       <c r="P7">
         <f t="shared" si="3"/>
-        <v>5.1338400000000006E-2</v>
+        <v>4.7924520000000005E-2</v>
       </c>
     </row>
     <row r="8" spans="1:16" x14ac:dyDescent="0.3">
       <c r="B8">
         <f>B6/B7</f>
-        <v>499.99999999999994</v>
+        <v>540.54054054054052</v>
       </c>
       <c r="C8">
         <f>C6/C7</f>
-        <v>294.88086812927577</v>
+        <v>365.4970760233918</v>
       </c>
       <c r="E8" t="s">
         <v>202</v>
@@ -1946,27 +1989,27 @@
       </c>
       <c r="K8">
         <f t="shared" si="0"/>
-        <v>3.5200000000000005E-4</v>
+        <v>3.256E-4</v>
       </c>
       <c r="L8">
         <f t="shared" si="4"/>
-        <v>0.24213688913920003</v>
+        <v>0.23717662245375998</v>
       </c>
       <c r="M8">
         <f t="shared" si="5"/>
-        <v>4.6041600000000009E-2</v>
+        <v>4.2588480000000005E-2</v>
       </c>
       <c r="N8">
         <f t="shared" si="1"/>
-        <v>0.97777777777777797</v>
+        <v>0.97777777777777763</v>
       </c>
       <c r="O8">
         <f t="shared" si="2"/>
-        <v>0.40772499983999999</v>
+        <v>0.4108956248520001</v>
       </c>
       <c r="P8">
         <f t="shared" si="3"/>
-        <v>5.1861600000000008E-2</v>
+        <v>4.8408480000000004E-2</v>
       </c>
     </row>
     <row r="9" spans="1:16" x14ac:dyDescent="0.3">
@@ -1987,27 +2030,27 @@
       </c>
       <c r="K9">
         <f t="shared" si="0"/>
-        <v>3.5600000000000003E-4</v>
+        <v>3.2929999999999998E-4</v>
       </c>
       <c r="L9">
         <f t="shared" si="4"/>
-        <v>0.24488844469760002</v>
+        <v>0.23987181134527996</v>
       </c>
       <c r="M9">
         <f t="shared" si="5"/>
-        <v>4.656480000000001E-2</v>
+        <v>4.3072440000000004E-2</v>
       </c>
       <c r="N9">
         <f t="shared" si="1"/>
-        <v>0.98888888888888893</v>
+        <v>0.98888888888888871</v>
       </c>
       <c r="O9">
         <f t="shared" si="2"/>
-        <v>0.40314382006651689</v>
+        <v>0.40627882007838212</v>
       </c>
       <c r="P9">
         <f t="shared" si="3"/>
-        <v>5.2384800000000009E-2</v>
+        <v>4.8892440000000002E-2</v>
       </c>
     </row>
     <row r="10" spans="1:16" x14ac:dyDescent="0.3">
@@ -2028,15 +2071,15 @@
       </c>
       <c r="K10">
         <f t="shared" si="0"/>
-        <v>3.6000000000000002E-4</v>
+        <v>3.3300000000000002E-4</v>
       </c>
       <c r="L10">
         <f t="shared" si="4"/>
-        <v>0.247640000256</v>
+        <v>0.2425670002368</v>
       </c>
       <c r="M10">
         <f t="shared" si="5"/>
-        <v>4.7088000000000005E-2</v>
+        <v>4.3556400000000009E-2</v>
       </c>
       <c r="N10">
         <f t="shared" si="1"/>
@@ -2044,11 +2087,11 @@
       </c>
       <c r="O10">
         <f t="shared" si="2"/>
-        <v>0.39866444428800007</v>
+        <v>0.40176461096640004</v>
       </c>
       <c r="P10">
         <f>$D$30+M10</f>
-        <v>5.2908000000000004E-2</v>
+        <v>4.9376400000000008E-2</v>
       </c>
     </row>
     <row r="11" spans="1:16" x14ac:dyDescent="0.3">
@@ -2071,15 +2114,15 @@
       </c>
       <c r="K11">
         <f t="shared" si="0"/>
-        <v>3.6400000000000001E-4</v>
+        <v>3.367E-4</v>
       </c>
       <c r="L11">
         <f t="shared" si="4"/>
-        <v>0.25039155581439998</v>
+        <v>0.24526218912831999</v>
       </c>
       <c r="M11">
         <f t="shared" si="5"/>
-        <v>4.7611200000000006E-2</v>
+        <v>4.4040360000000001E-2</v>
       </c>
       <c r="N11">
         <f t="shared" si="1"/>
@@ -2087,11 +2130,11 @@
       </c>
       <c r="O11">
         <f t="shared" si="2"/>
-        <v>0.39428351632879127</v>
+        <v>0.39734961524149454</v>
       </c>
       <c r="P11">
         <f t="shared" si="3"/>
-        <v>5.3431200000000005E-2</v>
+        <v>4.9860359999999999E-2</v>
       </c>
     </row>
     <row r="12" spans="1:16" x14ac:dyDescent="0.3">
@@ -2100,11 +2143,11 @@
       </c>
       <c r="B12">
         <f>SUM(B8:B11)</f>
-        <v>687.88888959999997</v>
+        <v>728.42943014054049</v>
       </c>
       <c r="C12">
         <f>SUM(C8:C11)</f>
-        <v>482.76975772927574</v>
+        <v>553.38596562339183</v>
       </c>
       <c r="E12" t="s">
         <v>18</v>
@@ -2114,27 +2157,27 @@
       </c>
       <c r="K12">
         <f t="shared" si="0"/>
-        <v>3.6800000000000005E-4</v>
+        <v>3.4040000000000003E-4</v>
       </c>
       <c r="L12">
         <f>K12*$B$12</f>
-        <v>0.25314311137280004</v>
+        <v>0.24795737801984</v>
       </c>
       <c r="M12">
         <f t="shared" si="5"/>
-        <v>4.8134400000000015E-2</v>
+        <v>4.4524320000000006E-2</v>
       </c>
       <c r="N12">
         <f t="shared" si="1"/>
-        <v>1.0222222222222224</v>
+        <v>1.0222222222222221</v>
       </c>
       <c r="O12">
         <f t="shared" si="2"/>
-        <v>0.38999782593391308</v>
+        <v>0.39303059768452181</v>
       </c>
       <c r="P12">
         <f t="shared" si="3"/>
-        <v>5.3954400000000013E-2</v>
+        <v>5.0344320000000005E-2</v>
       </c>
     </row>
     <row r="13" spans="1:16" x14ac:dyDescent="0.3">
@@ -2143,11 +2186,11 @@
       </c>
       <c r="B13">
         <f>1/B36</f>
-        <v>2500</v>
+        <v>2702.7027027027029</v>
       </c>
       <c r="C13">
         <f>1/B35</f>
-        <v>1061.5711252653928</v>
+        <v>1315.7894736842104</v>
       </c>
       <c r="E13" t="s">
         <v>198</v>
@@ -2157,15 +2200,15 @@
       </c>
       <c r="K13">
         <f t="shared" si="0"/>
-        <v>3.7200000000000004E-4</v>
+        <v>3.4410000000000002E-4</v>
       </c>
       <c r="L13">
         <f t="shared" si="4"/>
-        <v>0.2558946669312</v>
+        <v>0.25065256691136001</v>
       </c>
       <c r="M13">
         <f t="shared" si="5"/>
-        <v>4.8657600000000009E-2</v>
+        <v>4.5008280000000005E-2</v>
       </c>
       <c r="N13">
         <f t="shared" si="1"/>
@@ -2173,11 +2216,11 @@
       </c>
       <c r="O13">
         <f t="shared" si="2"/>
-        <v>0.38580430092387102</v>
+        <v>0.38880446222554838</v>
       </c>
       <c r="P13">
         <f t="shared" si="3"/>
-        <v>5.4477600000000008E-2</v>
+        <v>5.0828280000000003E-2</v>
       </c>
     </row>
     <row r="14" spans="1:16" x14ac:dyDescent="0.3">
@@ -2186,38 +2229,38 @@
       </c>
       <c r="B14">
         <f>(B13-B12)/B13</f>
-        <v>0.72484444416000005</v>
+        <v>0.73048111084800005</v>
       </c>
       <c r="C14">
         <f>(C13-C12)/C13</f>
-        <v>0.54523088821902221</v>
+        <v>0.57942666612622218</v>
       </c>
       <c r="J14">
         <v>0.94</v>
       </c>
       <c r="K14">
         <f t="shared" si="0"/>
-        <v>3.7599999999999998E-4</v>
+        <v>3.478E-4</v>
       </c>
       <c r="L14">
         <f t="shared" si="4"/>
-        <v>0.25864622248959995</v>
+        <v>0.25334775580287999</v>
       </c>
       <c r="M14">
         <f t="shared" si="5"/>
-        <v>4.9180800000000004E-2</v>
+        <v>4.5492240000000003E-2</v>
       </c>
       <c r="N14">
         <f t="shared" si="1"/>
-        <v>1.0444444444444443</v>
+        <v>1.0444444444444445</v>
       </c>
       <c r="O14">
         <f t="shared" si="2"/>
-        <v>0.38169999985021291</v>
+        <v>0.38466824454229787</v>
       </c>
       <c r="P14">
         <f t="shared" si="3"/>
-        <v>5.5000800000000002E-2</v>
+        <v>5.1312240000000002E-2</v>
       </c>
     </row>
     <row r="15" spans="1:16" x14ac:dyDescent="0.3">
@@ -2226,38 +2269,38 @@
       </c>
       <c r="B15">
         <f>0.55*B14</f>
-        <v>0.39866444428800007</v>
+        <v>0.40176461096640004</v>
       </c>
       <c r="C15">
         <f>0.55*C14</f>
-        <v>0.29987698852046224</v>
+        <v>0.31868466636942222</v>
       </c>
       <c r="J15">
         <v>0.95</v>
       </c>
       <c r="K15">
         <f t="shared" si="0"/>
-        <v>3.8000000000000002E-4</v>
+        <v>3.5149999999999998E-4</v>
       </c>
       <c r="L15">
         <f t="shared" si="4"/>
-        <v>0.26139777804800002</v>
+        <v>0.25604294469439998</v>
       </c>
       <c r="M15">
         <f t="shared" si="5"/>
-        <v>4.9704000000000005E-2</v>
+        <v>4.5976200000000002E-2</v>
       </c>
       <c r="N15">
         <f t="shared" si="1"/>
-        <v>1.0555555555555556</v>
+        <v>1.0555555555555554</v>
       </c>
       <c r="O15">
         <f t="shared" si="2"/>
-        <v>0.37768210511494743</v>
+        <v>0.38061910512606328</v>
       </c>
       <c r="P15">
         <f t="shared" si="3"/>
-        <v>5.5524000000000004E-2</v>
+        <v>5.1796200000000001E-2</v>
       </c>
     </row>
     <row r="17" spans="1:16" x14ac:dyDescent="0.3">
@@ -2267,15 +2310,15 @@
       <c r="C17" t="s">
         <v>214</v>
       </c>
-      <c r="J17" s="26" t="s">
+      <c r="J17" s="29" t="s">
         <v>193</v>
       </c>
-      <c r="K17" s="26"/>
-      <c r="L17" s="26"/>
-      <c r="M17" s="26"/>
-      <c r="N17" s="26"/>
-      <c r="O17" s="26"/>
-      <c r="P17" s="26"/>
+      <c r="K17" s="29"/>
+      <c r="L17" s="29"/>
+      <c r="M17" s="29"/>
+      <c r="N17" s="29"/>
+      <c r="O17" s="29"/>
+      <c r="P17" s="29"/>
     </row>
     <row r="18" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A18" s="2" t="s">
@@ -2333,27 +2376,27 @@
       </c>
       <c r="K19">
         <f t="shared" ref="K19:K29" si="6">$B$35*J19</f>
-        <v>8.007E-4</v>
+        <v>6.4599999999999998E-4</v>
       </c>
       <c r="L19">
         <f>K19*$C$12</f>
-        <v>0.38655374501383111</v>
+        <v>0.35748733379271108</v>
       </c>
       <c r="M19">
         <f>L19/$L$24</f>
-        <v>0.94444444444444453</v>
+        <v>0.9444444444444442</v>
       </c>
       <c r="N19">
         <f t="shared" ref="N19:N29" si="7">$C$15/M19</f>
-        <v>0.31751681137460702</v>
+        <v>0.33743082321468243</v>
       </c>
       <c r="O19">
         <f>K19*$C$21</f>
-        <v>7.8308459999999996E-2</v>
+        <v>6.3178799999999993E-2</v>
       </c>
       <c r="P19">
         <f>$D$29+O19</f>
-        <v>8.9238459999999992E-2</v>
+        <v>7.4108799999999989E-2</v>
       </c>
     </row>
     <row r="20" spans="1:16" x14ac:dyDescent="0.3">
@@ -2374,11 +2417,11 @@
       </c>
       <c r="K20">
         <f t="shared" si="6"/>
-        <v>8.1012E-4</v>
+        <v>6.5360000000000006E-4</v>
       </c>
       <c r="L20">
         <f t="shared" ref="L20:L29" si="8">K20*$C$12</f>
-        <v>0.39110143613164089</v>
+        <v>0.36169306713144894</v>
       </c>
       <c r="M20">
         <f t="shared" ref="M20:M29" si="9">L20/$L$24</f>
@@ -2386,15 +2429,15 @@
       </c>
       <c r="N20">
         <f t="shared" si="7"/>
-        <v>0.31382475542839072</v>
+        <v>0.3335072089912558</v>
       </c>
       <c r="O20">
         <f t="shared" ref="O20:O29" si="10">K20*$C$21</f>
-        <v>7.9229735999999995E-2</v>
+        <v>6.3922080000000006E-2</v>
       </c>
       <c r="P20">
         <f>$D$29+O20</f>
-        <v>9.015973599999999E-2</v>
+        <v>7.4852080000000001E-2</v>
       </c>
     </row>
     <row r="21" spans="1:16" x14ac:dyDescent="0.3">
@@ -2417,27 +2460,27 @@
       </c>
       <c r="K21">
         <f t="shared" si="6"/>
-        <v>8.1954E-4</v>
+        <v>6.6120000000000003E-4</v>
       </c>
       <c r="L21">
         <f t="shared" si="8"/>
-        <v>0.39564912724945062</v>
+        <v>0.36589880047018669</v>
       </c>
       <c r="M21">
         <f t="shared" si="9"/>
-        <v>0.96666666666666667</v>
+        <v>0.96666666666666656</v>
       </c>
       <c r="N21">
         <f t="shared" si="7"/>
-        <v>0.31021757433151265</v>
+        <v>0.32967379279595405</v>
       </c>
       <c r="O21">
         <f t="shared" si="10"/>
-        <v>8.0151011999999994E-2</v>
+        <v>6.4665360000000005E-2</v>
       </c>
       <c r="P21">
         <f t="shared" ref="P21:P29" si="11">$D$29+O21</f>
-        <v>9.1081011999999989E-2</v>
+        <v>7.559536E-2</v>
       </c>
     </row>
     <row r="22" spans="1:16" x14ac:dyDescent="0.3">
@@ -2450,27 +2493,27 @@
       </c>
       <c r="K22">
         <f t="shared" si="6"/>
-        <v>8.2896000000000001E-4</v>
+        <v>6.6879999999999999E-4</v>
       </c>
       <c r="L22">
         <f t="shared" si="8"/>
-        <v>0.4001968183672604</v>
+        <v>0.37010453380892444</v>
       </c>
       <c r="M22">
         <f t="shared" si="9"/>
-        <v>0.97777777777777775</v>
+        <v>0.97777777777777763</v>
       </c>
       <c r="N22">
         <f t="shared" si="7"/>
-        <v>0.30669237462320004</v>
+        <v>0.32592749969600004</v>
       </c>
       <c r="O22">
         <f t="shared" si="10"/>
-        <v>8.1072287999999992E-2</v>
+        <v>6.5408640000000004E-2</v>
       </c>
       <c r="P22">
         <f t="shared" si="11"/>
-        <v>9.2002287999999988E-2</v>
+        <v>7.6338639999999999E-2</v>
       </c>
     </row>
     <row r="23" spans="1:16" x14ac:dyDescent="0.3">
@@ -2479,27 +2522,27 @@
       </c>
       <c r="K23">
         <f t="shared" si="6"/>
-        <v>8.3838000000000001E-4</v>
+        <v>6.7640000000000007E-4</v>
       </c>
       <c r="L23">
         <f t="shared" si="8"/>
-        <v>0.40474450948507018</v>
+        <v>0.37431026714766225</v>
       </c>
       <c r="M23">
         <f t="shared" si="9"/>
-        <v>0.98888888888888893</v>
+        <v>0.98888888888888882</v>
       </c>
       <c r="N23">
         <f t="shared" si="7"/>
-        <v>0.30324639288586069</v>
+        <v>0.32226539295784273</v>
       </c>
       <c r="O23">
         <f t="shared" si="10"/>
-        <v>8.1993564000000005E-2</v>
+        <v>6.6151920000000003E-2</v>
       </c>
       <c r="P23">
         <f t="shared" si="11"/>
-        <v>9.2923564E-2</v>
+        <v>7.7081919999999998E-2</v>
       </c>
     </row>
     <row r="24" spans="1:16" x14ac:dyDescent="0.3">
@@ -2509,11 +2552,11 @@
       </c>
       <c r="K24">
         <f t="shared" si="6"/>
-        <v>8.4780000000000001E-4</v>
+        <v>6.8400000000000004E-4</v>
       </c>
       <c r="L24">
         <f t="shared" si="8"/>
-        <v>0.40929220060287996</v>
+        <v>0.37851600048640005</v>
       </c>
       <c r="M24">
         <f t="shared" si="9"/>
@@ -2521,15 +2564,15 @@
       </c>
       <c r="N24">
         <f t="shared" si="7"/>
-        <v>0.29987698852046224</v>
+        <v>0.31868466636942222</v>
       </c>
       <c r="O24">
         <f t="shared" si="10"/>
-        <v>8.2914840000000004E-2</v>
+        <v>6.6895200000000002E-2</v>
       </c>
       <c r="P24">
         <f t="shared" si="11"/>
-        <v>9.3844839999999999E-2</v>
+        <v>7.7825199999999997E-2</v>
       </c>
     </row>
     <row r="25" spans="1:16" x14ac:dyDescent="0.3">
@@ -2538,11 +2581,11 @@
       </c>
       <c r="K25">
         <f t="shared" si="6"/>
-        <v>8.5722000000000001E-4</v>
+        <v>6.9160000000000011E-4</v>
       </c>
       <c r="L25">
         <f t="shared" si="8"/>
-        <v>0.41383989172068975</v>
+        <v>0.38272173382513786</v>
       </c>
       <c r="M25">
         <f t="shared" si="9"/>
@@ -2550,15 +2593,15 @@
       </c>
       <c r="N25">
         <f t="shared" si="7"/>
-        <v>0.29658163699825935</v>
+        <v>0.31518263706865934</v>
       </c>
       <c r="O25">
         <f t="shared" si="10"/>
-        <v>8.3836116000000002E-2</v>
+        <v>6.7638480000000015E-2</v>
       </c>
       <c r="P25">
         <f t="shared" si="11"/>
-        <v>9.4766115999999997E-2</v>
+        <v>7.856848000000001E-2</v>
       </c>
     </row>
     <row r="26" spans="1:16" x14ac:dyDescent="0.3">
@@ -2567,11 +2610,11 @@
       </c>
       <c r="K26">
         <f t="shared" si="6"/>
-        <v>8.6664000000000001E-4</v>
+        <v>6.9920000000000008E-4</v>
       </c>
       <c r="L26">
         <f t="shared" si="8"/>
-        <v>0.41838758283849953</v>
+        <v>0.3869274671638756</v>
       </c>
       <c r="M26">
         <f t="shared" si="9"/>
@@ -2579,15 +2622,15 @@
       </c>
       <c r="N26">
         <f t="shared" si="7"/>
-        <v>0.29335792355262613</v>
+        <v>0.31175673883965221</v>
       </c>
       <c r="O26">
         <f t="shared" si="10"/>
-        <v>8.4757392000000001E-2</v>
+        <v>6.838176E-2</v>
       </c>
       <c r="P26">
         <f t="shared" si="11"/>
-        <v>9.5687391999999996E-2</v>
+        <v>7.9311759999999995E-2</v>
       </c>
     </row>
     <row r="27" spans="1:16" x14ac:dyDescent="0.3">
@@ -2597,27 +2640,27 @@
       </c>
       <c r="K27">
         <f t="shared" si="6"/>
-        <v>8.7606000000000001E-4</v>
+        <v>7.0680000000000005E-4</v>
       </c>
       <c r="L27">
         <f t="shared" si="8"/>
-        <v>0.42293527395630931</v>
+        <v>0.39113320050261335</v>
       </c>
       <c r="M27">
         <f t="shared" si="9"/>
-        <v>1.0333333333333334</v>
+        <v>1.0333333333333332</v>
       </c>
       <c r="N27">
         <f t="shared" si="7"/>
-        <v>0.29020353727786663</v>
+        <v>0.3084045158413764</v>
       </c>
       <c r="O27">
         <f t="shared" si="10"/>
-        <v>8.5678667999999999E-2</v>
+        <v>6.9125039999999999E-2</v>
       </c>
       <c r="P27">
         <f t="shared" si="11"/>
-        <v>9.6608667999999995E-2</v>
+        <v>8.0055039999999994E-2</v>
       </c>
     </row>
     <row r="28" spans="1:16" x14ac:dyDescent="0.3">
@@ -2641,27 +2684,27 @@
       </c>
       <c r="K28">
         <f t="shared" si="6"/>
-        <v>8.8548000000000001E-4</v>
+        <v>7.1440000000000002E-4</v>
       </c>
       <c r="L28">
         <f t="shared" si="8"/>
-        <v>0.42748296507411909</v>
+        <v>0.3953389338413511</v>
       </c>
       <c r="M28">
         <f t="shared" si="9"/>
-        <v>1.0444444444444445</v>
+        <v>1.0444444444444443</v>
       </c>
       <c r="N28">
         <f t="shared" si="7"/>
-        <v>0.28711626560469788</v>
+        <v>0.30512361673668087</v>
       </c>
       <c r="O28">
         <f t="shared" si="10"/>
-        <v>8.6599943999999998E-2</v>
+        <v>6.9868319999999998E-2</v>
       </c>
       <c r="P28">
         <f t="shared" si="11"/>
-        <v>9.7529943999999993E-2</v>
+        <v>8.0798319999999993E-2</v>
       </c>
     </row>
     <row r="29" spans="1:16" x14ac:dyDescent="0.3">
@@ -2683,27 +2726,27 @@
       </c>
       <c r="K29">
         <f t="shared" si="6"/>
-        <v>8.9490000000000001E-4</v>
+        <v>7.2199999999999999E-4</v>
       </c>
       <c r="L29">
         <f t="shared" si="8"/>
-        <v>0.43203065619192887</v>
+        <v>0.39954466718008891</v>
       </c>
       <c r="M29">
         <f t="shared" si="9"/>
-        <v>1.0555555555555556</v>
+        <v>1.0555555555555554</v>
       </c>
       <c r="N29">
         <f t="shared" si="7"/>
-        <v>0.28409398912464845</v>
+        <v>0.30191178919208428</v>
       </c>
       <c r="O29">
         <f t="shared" si="10"/>
-        <v>8.7521219999999997E-2</v>
+        <v>7.0611599999999997E-2</v>
       </c>
       <c r="P29">
         <f t="shared" si="11"/>
-        <v>9.8451219999999992E-2</v>
+        <v>8.1541599999999992E-2</v>
       </c>
     </row>
     <row r="30" spans="1:16" x14ac:dyDescent="0.3">
@@ -2737,15 +2780,15 @@
       <c r="E31">
         <v>0.7</v>
       </c>
-      <c r="J31" s="26" t="s">
+      <c r="J31" s="29" t="s">
         <v>194</v>
       </c>
-      <c r="K31" s="26"/>
-      <c r="L31" s="26"/>
-      <c r="M31" s="26"/>
-      <c r="N31" s="26"/>
-      <c r="O31" s="26"/>
-      <c r="P31" s="26"/>
+      <c r="K31" s="29"/>
+      <c r="L31" s="29"/>
+      <c r="M31" s="29"/>
+      <c r="N31" s="29"/>
+      <c r="O31" s="29"/>
+      <c r="P31" s="29"/>
     </row>
     <row r="32" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A32" s="2" t="s">
@@ -2784,23 +2827,23 @@
       </c>
       <c r="K33" s="3">
         <f t="shared" ref="K33:K44" si="12">$B$37*J33</f>
-        <v>2.7999999999999998E-4</v>
+        <v>1.8722199999999996E-4</v>
       </c>
       <c r="L33" s="3">
         <f t="shared" ref="L33:L44" si="13">K33*$B$12</f>
-        <v>0.19260888908799997</v>
+        <v>0.13637801476977224</v>
       </c>
       <c r="N33" s="3">
         <f t="shared" ref="N33:N44" si="14">$E$31-L33</f>
-        <v>0.50739111091199995</v>
+        <v>0.56362198523022777</v>
       </c>
       <c r="O33" s="3">
         <f t="shared" ref="O33:O44" si="15">K33*$B$21</f>
-        <v>3.6623999999999997E-2</v>
+        <v>2.4488637599999998E-2</v>
       </c>
       <c r="P33" s="3">
         <f>$D$31+O33</f>
-        <v>7.7464307511999314E-2</v>
+        <v>6.5328945111999312E-2</v>
       </c>
     </row>
     <row r="34" spans="1:16" x14ac:dyDescent="0.3">
@@ -2812,24 +2855,24 @@
       </c>
       <c r="K34" s="3">
         <f t="shared" si="12"/>
-        <v>3.4000000000000002E-4</v>
+        <v>2.2734099999999996E-4</v>
       </c>
       <c r="L34" s="3">
         <f>K34*$B$12</f>
-        <v>0.23388222246400001</v>
+        <v>0.16560187507758059</v>
       </c>
       <c r="M34" s="3"/>
       <c r="N34" s="3">
         <f>$E$31-L34</f>
-        <v>0.46611777753599992</v>
+        <v>0.53439812492241934</v>
       </c>
       <c r="O34" s="3">
         <f>K34*$B$21</f>
-        <v>4.4472000000000005E-2</v>
+        <v>2.9736202799999997E-2</v>
       </c>
       <c r="P34" s="3">
         <f t="shared" ref="P34:P44" si="16">$D$31+O34</f>
-        <v>8.5312307511999308E-2</v>
+        <v>7.057651031199931E-2</v>
       </c>
     </row>
     <row r="35" spans="1:16" x14ac:dyDescent="0.3">
@@ -2837,8 +2880,8 @@
         <v>185</v>
       </c>
       <c r="B35" s="21">
-        <f>942/1000000</f>
-        <v>9.4200000000000002E-4</v>
+        <f>760/1000000</f>
+        <v>7.6000000000000004E-4</v>
       </c>
       <c r="C35" t="s">
         <v>62</v>
@@ -2848,24 +2891,24 @@
       </c>
       <c r="K35" s="3">
         <f t="shared" si="12"/>
-        <v>3.4400000000000001E-4</v>
+        <v>2.3001559999999996E-4</v>
       </c>
       <c r="L35" s="3">
         <f t="shared" si="13"/>
-        <v>0.23663377802239999</v>
+        <v>0.16755013243143446</v>
       </c>
       <c r="M35" s="3"/>
       <c r="N35" s="3">
         <f t="shared" si="14"/>
-        <v>0.46336622197759997</v>
+        <v>0.53244986756856549</v>
       </c>
       <c r="O35" s="3">
         <f t="shared" si="15"/>
-        <v>4.4995200000000006E-2</v>
+        <v>3.0086040479999996E-2</v>
       </c>
       <c r="P35" s="3">
         <f t="shared" si="16"/>
-        <v>8.5835507511999309E-2</v>
+        <v>7.0926347991999303E-2</v>
       </c>
     </row>
     <row r="36" spans="1:16" x14ac:dyDescent="0.3">
@@ -2873,8 +2916,8 @@
         <v>61</v>
       </c>
       <c r="B36" s="21">
-        <f>400/1000000</f>
-        <v>4.0000000000000002E-4</v>
+        <f>370/1000000</f>
+        <v>3.6999999999999999E-4</v>
       </c>
       <c r="C36" t="s">
         <v>62</v>
@@ -2884,24 +2927,24 @@
       </c>
       <c r="K36" s="3">
         <f t="shared" si="12"/>
-        <v>3.48E-4</v>
+        <v>2.3269019999999996E-4</v>
       </c>
       <c r="L36" s="3">
         <f t="shared" si="13"/>
-        <v>0.2393853335808</v>
+        <v>0.16949838978528836</v>
       </c>
       <c r="M36" s="3"/>
       <c r="N36" s="3">
         <f t="shared" si="14"/>
-        <v>0.46061466641919996</v>
+        <v>0.53050161021471154</v>
       </c>
       <c r="O36" s="3">
         <f t="shared" si="15"/>
-        <v>4.5518400000000007E-2</v>
+        <v>3.0435878159999995E-2</v>
       </c>
       <c r="P36" s="3">
         <f t="shared" si="16"/>
-        <v>8.6358707511999311E-2</v>
+        <v>7.1276185671999309E-2</v>
       </c>
     </row>
     <row r="37" spans="1:16" x14ac:dyDescent="0.3">
@@ -2909,35 +2952,38 @@
         <v>111</v>
       </c>
       <c r="B37" s="21">
-        <f>400/1000000</f>
-        <v>4.0000000000000002E-4</v>
+        <f>267.46/1000000</f>
+        <v>2.6745999999999996E-4</v>
       </c>
       <c r="C37" t="s">
         <v>62</v>
       </c>
+      <c r="D37" t="s">
+        <v>381</v>
+      </c>
       <c r="J37" s="3">
         <v>0.88</v>
       </c>
       <c r="K37" s="3">
         <f t="shared" si="12"/>
-        <v>3.5200000000000005E-4</v>
+        <v>2.3536479999999998E-4</v>
       </c>
       <c r="L37" s="3">
         <f t="shared" si="13"/>
-        <v>0.24213688913920003</v>
+        <v>0.17144664713914226</v>
       </c>
       <c r="M37" s="3"/>
       <c r="N37" s="3">
         <f t="shared" si="14"/>
-        <v>0.45786311086079989</v>
+        <v>0.52855335286085769</v>
       </c>
       <c r="O37" s="3">
         <f t="shared" si="15"/>
-        <v>4.6041600000000009E-2</v>
+        <v>3.0785715839999998E-2</v>
       </c>
       <c r="P37" s="3">
         <f t="shared" si="16"/>
-        <v>8.6881907511999312E-2</v>
+        <v>7.1626023351999302E-2</v>
       </c>
     </row>
     <row r="38" spans="1:16" x14ac:dyDescent="0.3">
@@ -2946,24 +2992,24 @@
       </c>
       <c r="K38" s="3">
         <f t="shared" si="12"/>
-        <v>3.5600000000000003E-4</v>
+        <v>2.3803939999999998E-4</v>
       </c>
       <c r="L38" s="3">
         <f t="shared" si="13"/>
-        <v>0.24488844469760002</v>
+        <v>0.17339490449299616</v>
       </c>
       <c r="M38" s="3"/>
       <c r="N38" s="3">
         <f t="shared" si="14"/>
-        <v>0.45511155530239994</v>
+        <v>0.52660509550700385</v>
       </c>
       <c r="O38" s="3">
         <f t="shared" si="15"/>
-        <v>4.656480000000001E-2</v>
+        <v>3.1135553520000001E-2</v>
       </c>
       <c r="P38" s="3">
         <f t="shared" si="16"/>
-        <v>8.7405107511999314E-2</v>
+        <v>7.1975861031999308E-2</v>
       </c>
     </row>
     <row r="39" spans="1:16" x14ac:dyDescent="0.3">
@@ -2972,24 +3018,24 @@
       </c>
       <c r="K39" s="3">
         <f t="shared" si="12"/>
-        <v>3.6000000000000002E-4</v>
+        <v>2.4071399999999997E-4</v>
       </c>
       <c r="L39" s="3">
         <f t="shared" si="13"/>
-        <v>0.247640000256</v>
+        <v>0.17534316184685003</v>
       </c>
       <c r="M39" s="3"/>
       <c r="N39" s="3">
         <f t="shared" si="14"/>
-        <v>0.45235999974399999</v>
+        <v>0.5246568381531499</v>
       </c>
       <c r="O39" s="3">
         <f t="shared" si="15"/>
-        <v>4.7088000000000005E-2</v>
+        <v>3.1485391199999997E-2</v>
       </c>
       <c r="P39" s="3">
         <f t="shared" si="16"/>
-        <v>8.7928307511999315E-2</v>
+        <v>7.2325698711999314E-2</v>
       </c>
     </row>
     <row r="40" spans="1:16" x14ac:dyDescent="0.3">
@@ -3001,24 +3047,24 @@
       </c>
       <c r="K40" s="3">
         <f t="shared" si="12"/>
-        <v>3.6400000000000001E-4</v>
+        <v>2.4338859999999997E-4</v>
       </c>
       <c r="L40" s="3">
         <f t="shared" si="13"/>
-        <v>0.25039155581439998</v>
+        <v>0.17729141920070393</v>
       </c>
       <c r="M40" s="3"/>
       <c r="N40" s="3">
         <f t="shared" si="14"/>
-        <v>0.44960844418559998</v>
+        <v>0.52270858079929605</v>
       </c>
       <c r="O40" s="3">
         <f t="shared" si="15"/>
-        <v>4.7611200000000006E-2</v>
+        <v>3.1835228879999997E-2</v>
       </c>
       <c r="P40" s="3">
         <f t="shared" si="16"/>
-        <v>8.8451507511999317E-2</v>
+        <v>7.2675536391999307E-2</v>
       </c>
     </row>
     <row r="41" spans="1:16" x14ac:dyDescent="0.3">
@@ -3030,102 +3076,240 @@
       </c>
       <c r="K41" s="3">
         <f t="shared" si="12"/>
-        <v>3.6800000000000005E-4</v>
+        <v>2.4606319999999999E-4</v>
       </c>
       <c r="L41" s="3">
         <f t="shared" si="13"/>
-        <v>0.25314311137280004</v>
+        <v>0.17923967655455783</v>
       </c>
       <c r="M41" s="3"/>
       <c r="N41" s="3">
         <f t="shared" si="14"/>
-        <v>0.44685688862719991</v>
+        <v>0.5207603234454421</v>
       </c>
       <c r="O41" s="3">
         <f t="shared" si="15"/>
-        <v>4.8134400000000015E-2</v>
+        <v>3.2185066560000003E-2</v>
       </c>
       <c r="P41" s="3">
         <f t="shared" si="16"/>
-        <v>8.8974707511999318E-2</v>
+        <v>7.3025374071999313E-2</v>
       </c>
     </row>
     <row r="42" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="A42" s="31" t="s">
+        <v>375</v>
+      </c>
       <c r="J42" s="3">
         <v>0.93</v>
       </c>
       <c r="K42" s="3">
         <f t="shared" si="12"/>
-        <v>3.7200000000000004E-4</v>
+        <v>2.4873779999999996E-4</v>
       </c>
       <c r="L42" s="3">
         <f t="shared" si="13"/>
-        <v>0.2558946669312</v>
+        <v>0.1811879339084117</v>
       </c>
       <c r="M42" s="3"/>
       <c r="N42" s="3">
         <f t="shared" si="14"/>
-        <v>0.44410533306879996</v>
+        <v>0.51881206609158825</v>
       </c>
       <c r="O42" s="3">
         <f t="shared" si="15"/>
-        <v>4.8657600000000009E-2</v>
+        <v>3.2534904239999995E-2</v>
       </c>
       <c r="P42" s="3">
         <f t="shared" si="16"/>
-        <v>8.9497907511999319E-2</v>
+        <v>7.3375211751999306E-2</v>
       </c>
     </row>
     <row r="43" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="B43" t="s">
+        <v>114</v>
+      </c>
       <c r="J43" s="3">
         <v>0.94</v>
       </c>
       <c r="K43" s="3">
         <f t="shared" si="12"/>
-        <v>3.7599999999999998E-4</v>
+        <v>2.5141239999999993E-4</v>
       </c>
       <c r="L43" s="3">
         <f t="shared" si="13"/>
-        <v>0.25864622248959995</v>
+        <v>0.18313619126226557</v>
       </c>
       <c r="M43" s="3"/>
       <c r="N43" s="3">
         <f t="shared" si="14"/>
-        <v>0.4413537775104</v>
+        <v>0.51686380873773441</v>
       </c>
       <c r="O43" s="3">
         <f t="shared" si="15"/>
-        <v>4.9180800000000004E-2</v>
+        <v>3.2884741919999995E-2</v>
       </c>
       <c r="P43" s="3">
         <f t="shared" si="16"/>
-        <v>9.0021107511999321E-2</v>
+        <v>7.3725049431999312E-2</v>
       </c>
     </row>
     <row r="44" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="A44" t="s">
+        <v>376</v>
+      </c>
+      <c r="B44" t="s">
+        <v>378</v>
+      </c>
+      <c r="C44" t="s">
+        <v>379</v>
+      </c>
+      <c r="D44" t="s">
+        <v>386</v>
+      </c>
+      <c r="E44" t="s">
+        <v>385</v>
+      </c>
       <c r="J44" s="3">
         <v>0.95</v>
       </c>
       <c r="K44" s="3">
         <f t="shared" si="12"/>
-        <v>3.8000000000000002E-4</v>
+        <v>2.5408699999999995E-4</v>
       </c>
       <c r="L44" s="3">
         <f t="shared" si="13"/>
-        <v>0.26139777804800002</v>
+        <v>0.18508444861611947</v>
       </c>
       <c r="M44" s="3"/>
       <c r="N44" s="3">
         <f t="shared" si="14"/>
-        <v>0.43860222195199994</v>
+        <v>0.51491555138388045</v>
       </c>
       <c r="O44" s="3">
         <f t="shared" si="15"/>
-        <v>4.9704000000000005E-2</v>
+        <v>3.3234579599999994E-2</v>
       </c>
       <c r="P44" s="3">
         <f t="shared" si="16"/>
-        <v>9.0544307511999322E-2</v>
+        <v>7.4074887111999305E-2</v>
+      </c>
+    </row>
+    <row r="45" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="A45" t="s">
+        <v>383</v>
+      </c>
+      <c r="B45">
+        <v>820</v>
+      </c>
+      <c r="C45">
+        <v>760</v>
+      </c>
+      <c r="D45">
+        <f>B45-C45</f>
+        <v>60</v>
+      </c>
+      <c r="E45">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="46" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="A46" t="s">
+        <v>384</v>
+      </c>
+      <c r="B46">
+        <v>490</v>
+      </c>
+      <c r="C46">
+        <v>370</v>
+      </c>
+      <c r="D46">
+        <f>B46-C46</f>
+        <v>120</v>
+      </c>
+      <c r="E46">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="47" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="A47" t="s">
+        <v>377</v>
+      </c>
+      <c r="B47">
+        <v>220</v>
+      </c>
+      <c r="C47">
+        <f>0.1*760</f>
+        <v>76</v>
+      </c>
+      <c r="D47">
+        <f>B47-C47</f>
+        <v>144</v>
+      </c>
+      <c r="E47">
+        <f>C45-C47</f>
+        <v>684</v>
+      </c>
+    </row>
+    <row r="48" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="A48" t="s">
+        <v>380</v>
+      </c>
+      <c r="B48">
+        <v>170</v>
+      </c>
+      <c r="C48">
+        <f>0.1*370</f>
+        <v>37</v>
+      </c>
+      <c r="D48">
+        <f>B48-C48</f>
+        <v>133</v>
+      </c>
+      <c r="E48">
+        <f>C46-C48</f>
+        <v>333</v>
+      </c>
+    </row>
+    <row r="49" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A49" t="s">
+        <v>13</v>
+      </c>
+      <c r="B49">
+        <f>11888/33.336</f>
+        <v>356.61147108231341</v>
+      </c>
+      <c r="C49">
+        <f>B49*0.75</f>
+        <v>267.45860331173503</v>
+      </c>
+      <c r="D49">
+        <f>0.25*B49</f>
+        <v>89.152867770578354</v>
+      </c>
+      <c r="E49">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="50" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A50" t="s">
+        <v>382</v>
+      </c>
+      <c r="B50">
+        <f>C50+D50</f>
+        <v>179.04867610591151</v>
+      </c>
+      <c r="C50">
+        <f>0.3*C49</f>
+        <v>80.23758099352051</v>
+      </c>
+      <c r="D50">
+        <f>D48*D49/D46</f>
+        <v>98.811095112391016</v>
+      </c>
+      <c r="E50">
+        <f>C49-C50</f>
+        <v>187.22102231821452</v>
       </c>
     </row>
   </sheetData>
@@ -3144,6 +3328,195 @@
 </file>
 
 <file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BFB7227C-A1DE-45C0-910C-0F614B128A68}">
+  <dimension ref="A1:K19"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="O21" sqref="O21"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="15.21875" customWidth="1"/>
+    <col min="2" max="2" width="10.88671875" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="B1" t="s">
+        <v>281</v>
+      </c>
+      <c r="C1" t="s">
+        <v>114</v>
+      </c>
+      <c r="J1">
+        <v>33.335999999999999</v>
+      </c>
+      <c r="K1" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="2" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A2">
+        <v>2017</v>
+      </c>
+      <c r="B2">
+        <f>29*1/100</f>
+        <v>0.28999999999999998</v>
+      </c>
+      <c r="C2">
+        <f>B2*1000/J1</f>
+        <v>8.6993040556755457</v>
+      </c>
+    </row>
+    <row r="3" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A3">
+        <v>2050</v>
+      </c>
+      <c r="B3">
+        <f>4*1/100</f>
+        <v>0.04</v>
+      </c>
+      <c r="C3">
+        <f>B3*1000/J1</f>
+        <v>1.1999040076793857</v>
+      </c>
+      <c r="D3" s="12" t="s">
+        <v>279</v>
+      </c>
+    </row>
+    <row r="5" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A5" t="s">
+        <v>284</v>
+      </c>
+      <c r="B5">
+        <f>3000*10</f>
+        <v>30000</v>
+      </c>
+      <c r="D5" t="s">
+        <v>329</v>
+      </c>
+    </row>
+    <row r="6" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A6" t="s">
+        <v>285</v>
+      </c>
+      <c r="B6">
+        <f>B5*C3</f>
+        <v>35997.120230381566</v>
+      </c>
+      <c r="C6" t="s">
+        <v>286</v>
+      </c>
+    </row>
+    <row r="7" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A7" t="s">
+        <v>287</v>
+      </c>
+      <c r="B7">
+        <f>B6/(8760*0.9*7)</f>
+        <v>0.6522635397256934</v>
+      </c>
+      <c r="C7" t="s">
+        <v>330</v>
+      </c>
+    </row>
+    <row r="8" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A8" t="s">
+        <v>287</v>
+      </c>
+      <c r="B8">
+        <f>B6/(8760*0.9*10)</f>
+        <v>0.45658447780798539</v>
+      </c>
+      <c r="C8" t="s">
+        <v>331</v>
+      </c>
+    </row>
+    <row r="9" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="D9" s="12" t="s">
+        <v>280</v>
+      </c>
+    </row>
+    <row r="11" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="H11" s="12" t="s">
+        <v>345</v>
+      </c>
+    </row>
+    <row r="12" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A12" s="20">
+        <v>2022</v>
+      </c>
+      <c r="B12" s="20">
+        <v>3800</v>
+      </c>
+      <c r="H12" s="12" t="s">
+        <v>344</v>
+      </c>
+    </row>
+    <row r="13" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A13" s="20">
+        <v>2030</v>
+      </c>
+      <c r="B13" s="20">
+        <v>1500</v>
+      </c>
+      <c r="H13" s="12" t="s">
+        <v>324</v>
+      </c>
+    </row>
+    <row r="14" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A14">
+        <v>2050</v>
+      </c>
+      <c r="B14">
+        <v>400</v>
+      </c>
+    </row>
+    <row r="17" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A17" t="s">
+        <v>4</v>
+      </c>
+      <c r="B17">
+        <v>82</v>
+      </c>
+      <c r="C17" s="20"/>
+      <c r="D17" s="26" t="s">
+        <v>349</v>
+      </c>
+      <c r="H17" t="s">
+        <v>351</v>
+      </c>
+    </row>
+    <row r="18" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="C18" s="20"/>
+      <c r="D18" s="12" t="s">
+        <v>350</v>
+      </c>
+      <c r="H18" t="s">
+        <v>354</v>
+      </c>
+    </row>
+    <row r="19" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="D19" s="12" t="s">
+        <v>352</v>
+      </c>
+    </row>
+  </sheetData>
+  <hyperlinks>
+    <hyperlink ref="D3" r:id="rId1" xr:uid="{73261102-8930-4034-AFBD-8AF2404129E0}"/>
+    <hyperlink ref="D9" r:id="rId2" display="https://urldefense.proofpoint.com/v2/url?u=https-3A__doi.org_10.3390_environments5020024&amp;d=DwMFaQ&amp;c=OCIEmEwdEq_aNlsP4fF3gFqSN-E3mlr2t9JcDdfOZag&amp;r=79oVBkpSJ8jc8Mw2l8LuV83qCNXLl72NkphdMlliukM&amp;m=NGWcOQO2qa2PKM1ngjeYDCH3rElV-XSihhWPcRPvzOs&amp;s=sFKFBAwrUGsHBL-aJtbQE7lcIp4piSa0kz-mx0PEbR4&amp;e=" xr:uid="{320B681C-F103-4058-B8E2-518FF78252CD}"/>
+    <hyperlink ref="H13" r:id="rId3" tooltip="Persistent link using digital object identifier" xr:uid="{B3E006C3-DDB9-480A-9D90-5884D6F5F9E8}"/>
+    <hyperlink ref="H12" r:id="rId4" xr:uid="{737771D8-B96A-49B6-86D2-864FF1155855}"/>
+    <hyperlink ref="H11" r:id="rId5" xr:uid="{63C37621-088F-42CB-A35E-1ECFDE9D82C3}"/>
+    <hyperlink ref="D18" r:id="rId6" xr:uid="{18AE47F8-0B31-409D-88A0-14B43BA66492}"/>
+    <hyperlink ref="D19" r:id="rId7" xr:uid="{BD971C0B-0989-4A61-909C-C1F9A507336B}"/>
+  </hyperlinks>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId8"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9B6BC44C-C965-493C-907E-B5E15FE8A950}">
   <dimension ref="A1:M14"/>
   <sheetViews>
@@ -3261,7 +3634,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5A029AF6-CB84-4D91-9DA5-CC90BF5892BA}">
   <dimension ref="A1:P30"/>
   <sheetViews>
@@ -3505,669 +3878,350 @@
       </c>
     </row>
     <row r="18" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A18" s="29" t="s">
+      <c r="A18" s="27" t="s">
         <v>299</v>
       </c>
-      <c r="B18" s="29"/>
-      <c r="C18" s="29"/>
-      <c r="D18" s="29"/>
-      <c r="E18" s="29"/>
-      <c r="F18" s="29"/>
-      <c r="G18" s="29"/>
-      <c r="H18" s="29"/>
-      <c r="I18" s="29"/>
-      <c r="J18" s="29"/>
-      <c r="K18" s="29"/>
-      <c r="L18" s="29"/>
+      <c r="B18" s="27"/>
+      <c r="C18" s="27"/>
+      <c r="D18" s="27"/>
+      <c r="E18" s="27"/>
+      <c r="F18" s="27"/>
+      <c r="G18" s="27"/>
+      <c r="H18" s="27"/>
+      <c r="I18" s="27"/>
+      <c r="J18" s="27"/>
+      <c r="K18" s="27"/>
+      <c r="L18" s="27"/>
     </row>
     <row r="19" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A19" s="29" t="s">
+      <c r="A19" s="27" t="s">
         <v>300</v>
       </c>
-      <c r="B19" s="29">
+      <c r="B19" s="27">
         <v>52.2</v>
       </c>
-      <c r="C19" s="29" t="s">
+      <c r="C19" s="27" t="s">
         <v>113</v>
       </c>
-      <c r="D19" s="29">
+      <c r="D19" s="27">
         <f>B19/$H$2</f>
         <v>187.9049676025918</v>
       </c>
-      <c r="E19" s="29" t="s">
+      <c r="E19" s="27" t="s">
         <v>114</v>
       </c>
-      <c r="F19" s="29">
+      <c r="F19" s="27">
         <f>D19*L2/1000</f>
         <v>939.52483801295898</v>
       </c>
-      <c r="G19" s="29"/>
-      <c r="H19" s="29"/>
-      <c r="I19" s="29"/>
-      <c r="J19" s="29"/>
-      <c r="K19" s="29"/>
-      <c r="L19" s="29"/>
+      <c r="G19" s="27"/>
+      <c r="H19" s="27"/>
+      <c r="I19" s="27"/>
+      <c r="J19" s="27"/>
+      <c r="K19" s="27"/>
+      <c r="L19" s="27"/>
     </row>
     <row r="20" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A20" s="29" t="s">
+      <c r="A20" s="27" t="s">
         <v>301</v>
       </c>
-      <c r="B20" s="29">
+      <c r="B20" s="27">
         <v>46.7</v>
       </c>
-      <c r="C20" s="29" t="s">
+      <c r="C20" s="27" t="s">
         <v>113</v>
       </c>
-      <c r="D20" s="29">
+      <c r="D20" s="27">
         <f t="shared" ref="D20:D21" si="2">B20/$H$2</f>
         <v>168.10655147588196</v>
       </c>
-      <c r="E20" s="29" t="s">
+      <c r="E20" s="27" t="s">
         <v>114</v>
       </c>
-      <c r="F20" s="29">
+      <c r="F20" s="27">
         <f>D20*L3/1000</f>
         <v>3362.131029517639</v>
       </c>
-      <c r="G20" s="29"/>
-      <c r="H20" s="29"/>
-      <c r="I20" s="29"/>
-      <c r="J20" s="29"/>
-      <c r="K20" s="29"/>
-      <c r="L20" s="29"/>
+      <c r="G20" s="27"/>
+      <c r="H20" s="27"/>
+      <c r="I20" s="27"/>
+      <c r="J20" s="27"/>
+      <c r="K20" s="27"/>
+      <c r="L20" s="27"/>
     </row>
     <row r="21" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A21" s="29" t="s">
+      <c r="A21" s="27" t="s">
         <v>302</v>
       </c>
-      <c r="B21" s="29">
+      <c r="B21" s="27">
         <v>41.6</v>
       </c>
-      <c r="C21" s="29" t="s">
+      <c r="C21" s="27" t="s">
         <v>113</v>
       </c>
-      <c r="D21" s="29">
+      <c r="D21" s="27">
         <f t="shared" si="2"/>
         <v>149.74802015838733</v>
       </c>
-      <c r="E21" s="29" t="s">
+      <c r="E21" s="27" t="s">
         <v>114</v>
       </c>
-      <c r="F21" s="29">
+      <c r="F21" s="27">
         <f>D21*L3/1000</f>
         <v>2994.9604031677463</v>
       </c>
-      <c r="G21" s="29"/>
-      <c r="H21" s="29"/>
-      <c r="I21" s="29"/>
-      <c r="J21" s="29"/>
-      <c r="K21" s="29"/>
-      <c r="L21" s="29"/>
+      <c r="G21" s="27"/>
+      <c r="H21" s="27"/>
+      <c r="I21" s="27"/>
+      <c r="J21" s="27"/>
+      <c r="K21" s="27"/>
+      <c r="L21" s="27"/>
     </row>
     <row r="22" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A22" s="29"/>
-      <c r="B22" s="29"/>
-      <c r="C22" s="29"/>
-      <c r="D22" s="29"/>
-      <c r="E22" s="29"/>
-      <c r="F22" s="29"/>
-      <c r="G22" s="29"/>
-      <c r="H22" s="29"/>
-      <c r="I22" s="29"/>
-      <c r="J22" s="29"/>
-      <c r="K22" s="29"/>
-      <c r="L22" s="29"/>
+      <c r="A22" s="27"/>
+      <c r="B22" s="27"/>
+      <c r="C22" s="27"/>
+      <c r="D22" s="27"/>
+      <c r="E22" s="27"/>
+      <c r="F22" s="27"/>
+      <c r="G22" s="27"/>
+      <c r="H22" s="27"/>
+      <c r="I22" s="27"/>
+      <c r="J22" s="27"/>
+      <c r="K22" s="27"/>
+      <c r="L22" s="27"/>
     </row>
     <row r="23" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A23" s="29" t="s">
+      <c r="A23" s="27" t="s">
         <v>304</v>
       </c>
-      <c r="B23" s="29"/>
-      <c r="C23" s="29"/>
-      <c r="D23" s="29"/>
-      <c r="E23" s="29"/>
-      <c r="F23" s="29"/>
-      <c r="G23" s="29"/>
-      <c r="H23" s="29"/>
-      <c r="I23" s="29"/>
-      <c r="J23" s="29"/>
-      <c r="K23" s="29"/>
-      <c r="L23" s="29"/>
+      <c r="B23" s="27"/>
+      <c r="C23" s="27"/>
+      <c r="D23" s="27"/>
+      <c r="E23" s="27"/>
+      <c r="F23" s="27"/>
+      <c r="G23" s="27"/>
+      <c r="H23" s="27"/>
+      <c r="I23" s="27"/>
+      <c r="J23" s="27"/>
+      <c r="K23" s="27"/>
+      <c r="L23" s="27"/>
     </row>
     <row r="24" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A24" s="29" t="s">
+      <c r="A24" s="27" t="s">
         <v>17</v>
       </c>
-      <c r="B24" s="29">
+      <c r="B24" s="27">
         <v>5881</v>
       </c>
-      <c r="C24" s="29" t="s">
+      <c r="C24" s="27" t="s">
         <v>305</v>
       </c>
-      <c r="D24" s="29">
+      <c r="D24" s="27">
         <f>B24*H2</f>
         <v>1633.7418</v>
       </c>
-      <c r="E24" s="29" t="s">
+      <c r="E24" s="27" t="s">
         <v>73</v>
       </c>
-      <c r="F24" s="29"/>
-      <c r="G24" s="29"/>
-      <c r="H24" s="29"/>
-      <c r="I24" s="29"/>
-      <c r="J24" s="29"/>
-      <c r="K24" s="29"/>
-      <c r="L24" s="29"/>
+      <c r="F24" s="27"/>
+      <c r="G24" s="27"/>
+      <c r="H24" s="27"/>
+      <c r="I24" s="27"/>
+      <c r="J24" s="27"/>
+      <c r="K24" s="27"/>
+      <c r="L24" s="27"/>
     </row>
     <row r="25" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A25" s="29" t="s">
+      <c r="A25" s="27" t="s">
         <v>92</v>
       </c>
-      <c r="B25" s="29"/>
-      <c r="C25" s="29"/>
-      <c r="D25" s="29"/>
-      <c r="E25" s="29"/>
-      <c r="F25" s="29"/>
-      <c r="G25" s="29"/>
-      <c r="H25" s="29"/>
-      <c r="I25" s="29"/>
-      <c r="J25" s="29"/>
-      <c r="K25" s="30"/>
-      <c r="L25" s="29" t="s">
+      <c r="B25" s="27"/>
+      <c r="C25" s="27"/>
+      <c r="D25" s="27"/>
+      <c r="E25" s="27"/>
+      <c r="F25" s="27"/>
+      <c r="G25" s="27"/>
+      <c r="H25" s="27"/>
+      <c r="I25" s="27"/>
+      <c r="J25" s="27"/>
+      <c r="K25" s="28"/>
+      <c r="L25" s="27" t="s">
         <v>318</v>
       </c>
     </row>
     <row r="26" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A26" s="29" t="s">
+      <c r="A26" s="27" t="s">
         <v>311</v>
       </c>
-      <c r="B26" s="29" t="s">
+      <c r="B26" s="27" t="s">
         <v>306</v>
       </c>
-      <c r="C26" s="29" t="s">
+      <c r="C26" s="27" t="s">
         <v>307</v>
       </c>
-      <c r="D26" s="29" t="s">
+      <c r="D26" s="27" t="s">
         <v>310</v>
       </c>
-      <c r="E26" s="29" t="s">
+      <c r="E26" s="27" t="s">
         <v>308</v>
       </c>
-      <c r="F26" s="29" t="s">
+      <c r="F26" s="27" t="s">
         <v>309</v>
       </c>
-      <c r="G26" s="29"/>
-      <c r="H26" s="29"/>
-      <c r="I26" s="29" t="s">
+      <c r="G26" s="27"/>
+      <c r="H26" s="27"/>
+      <c r="I26" s="27" t="s">
         <v>314</v>
       </c>
-      <c r="J26" s="29"/>
-      <c r="K26" s="29">
+      <c r="J26" s="27"/>
+      <c r="K26" s="27">
         <f>4.08/(4.08+3.69+0.58)</f>
         <v>0.488622754491018</v>
       </c>
-      <c r="L26" s="29">
+      <c r="L26" s="27">
         <v>943</v>
       </c>
     </row>
     <row r="27" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A27" s="29" t="s">
+      <c r="A27" s="27" t="s">
         <v>312</v>
       </c>
-      <c r="B27" s="29">
+      <c r="B27" s="27">
         <f>6*H2</f>
         <v>1.6667999999999998</v>
       </c>
-      <c r="C27" s="29">
+      <c r="C27" s="27">
         <f>283*H2</f>
         <v>78.617400000000004</v>
       </c>
-      <c r="D27" s="29">
+      <c r="D27" s="27">
         <f>38*H2</f>
         <v>10.5564</v>
       </c>
-      <c r="E27" s="29">
+      <c r="E27" s="27">
         <f>1230*H2</f>
         <v>341.69400000000002</v>
       </c>
-      <c r="F27" s="29">
+      <c r="F27" s="27">
         <f>4323*H2</f>
         <v>1200.9294</v>
       </c>
-      <c r="G27" s="29" t="s">
+      <c r="G27" s="27" t="s">
         <v>73</v>
       </c>
-      <c r="H27" s="29"/>
-      <c r="I27" s="29" t="s">
+      <c r="H27" s="27"/>
+      <c r="I27" s="27" t="s">
         <v>315</v>
       </c>
-      <c r="J27" s="29"/>
-      <c r="K27" s="29">
+      <c r="J27" s="27"/>
+      <c r="K27" s="27">
         <f>3.69/(4.08+3.69+0.58)</f>
         <v>0.44191616766467068</v>
       </c>
-      <c r="L27" s="29">
+      <c r="L27" s="27">
         <v>599</v>
       </c>
     </row>
     <row r="28" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A28" s="29" t="s">
+      <c r="A28" s="27" t="s">
         <v>313</v>
       </c>
-      <c r="B28" s="29">
+      <c r="B28" s="27">
         <f>11.5</f>
         <v>11.5</v>
       </c>
-      <c r="C28" s="29">
+      <c r="C28" s="27">
         <v>24</v>
       </c>
-      <c r="D28" s="29">
+      <c r="D28" s="27">
         <v>230</v>
       </c>
-      <c r="E28" s="29">
+      <c r="E28" s="27">
         <v>777.43592814371266</v>
       </c>
-      <c r="F28" s="29">
+      <c r="F28" s="27">
         <v>12</v>
       </c>
-      <c r="G28" s="29" t="s">
+      <c r="G28" s="27" t="s">
         <v>114</v>
       </c>
-      <c r="H28" s="29"/>
-      <c r="I28" s="29" t="s">
+      <c r="H28" s="27"/>
+      <c r="I28" s="27" t="s">
         <v>316</v>
       </c>
-      <c r="J28" s="29"/>
-      <c r="K28" s="29">
+      <c r="J28" s="27"/>
+      <c r="K28" s="27">
         <f>0.58/(4.08+3.69+0.58)</f>
         <v>6.9461077844311381E-2</v>
       </c>
-      <c r="L28" s="29">
+      <c r="L28" s="27">
         <v>748</v>
       </c>
     </row>
     <row r="29" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A29" s="29" t="s">
+      <c r="A29" s="27" t="s">
         <v>318</v>
       </c>
-      <c r="B29" s="29">
+      <c r="B29" s="27">
         <f>B28*B27</f>
         <v>19.168199999999999</v>
       </c>
-      <c r="C29" s="29">
+      <c r="C29" s="27">
         <f t="shared" ref="C29:F29" si="3">C28*C27</f>
         <v>1886.8176000000001</v>
       </c>
-      <c r="D29" s="29">
+      <c r="D29" s="27">
         <f t="shared" si="3"/>
         <v>2427.9720000000002</v>
       </c>
-      <c r="E29" s="29">
+      <c r="E29" s="27">
         <f t="shared" si="3"/>
         <v>265645.19203113776</v>
       </c>
-      <c r="F29" s="29">
+      <c r="F29" s="27">
         <f t="shared" si="3"/>
         <v>14411.1528</v>
       </c>
-      <c r="G29" s="29" t="s">
+      <c r="G29" s="27" t="s">
         <v>319</v>
       </c>
-      <c r="H29" s="29"/>
-      <c r="I29" s="29" t="s">
+      <c r="H29" s="27"/>
+      <c r="I29" s="27" t="s">
         <v>317</v>
       </c>
-      <c r="J29" s="29"/>
-      <c r="K29" s="29"/>
-      <c r="L29" s="29">
+      <c r="J29" s="27"/>
+      <c r="K29" s="27"/>
+      <c r="L29" s="27">
         <f>(K26*L26)+(K27*L27)+(K28*L28)</f>
         <v>777.43592814371266</v>
       </c>
     </row>
     <row r="30" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A30" s="29" t="s">
+      <c r="A30" s="27" t="s">
         <v>17</v>
       </c>
-      <c r="B30" s="29"/>
-      <c r="C30" s="29"/>
-      <c r="D30" s="29"/>
-      <c r="E30" s="29"/>
-      <c r="F30" s="29">
+      <c r="B30" s="27"/>
+      <c r="C30" s="27"/>
+      <c r="D30" s="27"/>
+      <c r="E30" s="27"/>
+      <c r="F30" s="27">
         <f>SUM(B29:F29)/1000</f>
         <v>284.39030263113773</v>
       </c>
-      <c r="G30" s="29" t="s">
+      <c r="G30" s="27" t="s">
         <v>72</v>
       </c>
-      <c r="H30" s="29"/>
-      <c r="I30" s="29"/>
-      <c r="J30" s="29"/>
-      <c r="K30" s="29"/>
-      <c r="L30" s="29"/>
+      <c r="H30" s="27"/>
+      <c r="I30" s="27"/>
+      <c r="J30" s="27"/>
+      <c r="K30" s="27"/>
+      <c r="L30" s="27"/>
     </row>
   </sheetData>
   <hyperlinks>
     <hyperlink ref="A1" r:id="rId1" tooltip="Persistent link using digital object identifier" xr:uid="{02408BA4-1641-4ED4-B210-4315E996BE1B}"/>
     <hyperlink ref="P9" r:id="rId2" xr:uid="{83FB7102-FA60-4FF6-B48E-F6D3561360A3}"/>
-  </hyperlinks>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2E6C6BEB-6091-4743-A766-86BDD24D0263}">
-  <dimension ref="A1:J29"/>
-  <sheetViews>
-    <sheetView zoomScale="175" zoomScaleNormal="175" workbookViewId="0">
-      <selection activeCell="C10" sqref="C10"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
-  <cols>
-    <col min="1" max="1" width="17.6640625" customWidth="1"/>
-    <col min="2" max="2" width="10.44140625" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A1" t="s">
-        <v>220</v>
-      </c>
-      <c r="B1">
-        <v>377970</v>
-      </c>
-      <c r="C1" t="s">
-        <v>221</v>
-      </c>
-    </row>
-    <row r="2" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A2" t="s">
-        <v>222</v>
-      </c>
-      <c r="B2">
-        <v>251000</v>
-      </c>
-      <c r="C2" t="s">
-        <v>221</v>
-      </c>
-    </row>
-    <row r="3" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A3" t="s">
-        <v>223</v>
-      </c>
-      <c r="B3">
-        <v>7.5</v>
-      </c>
-      <c r="C3" t="s">
-        <v>224</v>
-      </c>
-      <c r="I3">
-        <v>4.0468600000000002E-3</v>
-      </c>
-      <c r="J3" t="s">
-        <v>225</v>
-      </c>
-    </row>
-    <row r="4" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="B4">
-        <f>B3*I3*1000</f>
-        <v>30.351450000000003</v>
-      </c>
-      <c r="C4" t="s">
-        <v>226</v>
-      </c>
-      <c r="I4" s="16">
-        <v>9.2902999999999995E-8</v>
-      </c>
-      <c r="J4" t="s">
-        <v>248</v>
-      </c>
-    </row>
-    <row r="5" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A5" t="s">
-        <v>227</v>
-      </c>
-      <c r="B5">
-        <f>300*B4</f>
-        <v>9105.4350000000013</v>
-      </c>
-      <c r="C5" t="s">
-        <v>221</v>
-      </c>
-      <c r="D5">
-        <f>B5*100/B2</f>
-        <v>3.6276633466135464</v>
-      </c>
-      <c r="E5" t="s">
-        <v>234</v>
-      </c>
-    </row>
-    <row r="6" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A6" t="s">
-        <v>246</v>
-      </c>
-      <c r="B6">
-        <f>1.5/20</f>
-        <v>7.4999999999999997E-2</v>
-      </c>
-      <c r="C6" t="s">
-        <v>259</v>
-      </c>
-      <c r="D6" s="16">
-        <f>B6*I3*1000</f>
-        <v>0.30351450000000002</v>
-      </c>
-      <c r="E6" t="s">
-        <v>249</v>
-      </c>
-      <c r="G6" s="12" t="s">
-        <v>260</v>
-      </c>
-    </row>
-    <row r="7" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="B7">
-        <v>0.04</v>
-      </c>
-      <c r="C7" t="s">
-        <v>259</v>
-      </c>
-      <c r="D7" s="16">
-        <f>B7*I3*1000</f>
-        <v>0.1618744</v>
-      </c>
-      <c r="E7" t="s">
-        <v>249</v>
-      </c>
-      <c r="G7" s="12" t="s">
-        <v>261</v>
-      </c>
-    </row>
-    <row r="8" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="B8">
-        <f>76800/60</f>
-        <v>1280</v>
-      </c>
-      <c r="C8" t="s">
-        <v>247</v>
-      </c>
-      <c r="D8" s="16">
-        <f>B8*I4*1000</f>
-        <v>0.11891583999999998</v>
-      </c>
-      <c r="E8" t="s">
-        <v>249</v>
-      </c>
-      <c r="G8" s="12" t="s">
-        <v>254</v>
-      </c>
-    </row>
-    <row r="9" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A9" t="s">
-        <v>245</v>
-      </c>
-      <c r="B9">
-        <f>D9*B2/100</f>
-        <v>7530</v>
-      </c>
-      <c r="C9" t="s">
-        <v>221</v>
-      </c>
-      <c r="D9">
-        <v>3</v>
-      </c>
-      <c r="E9" t="s">
-        <v>234</v>
-      </c>
-    </row>
-    <row r="10" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A10" t="s">
-        <v>241</v>
-      </c>
-      <c r="B10" s="16">
-        <f>B9/D6</f>
-        <v>24809.358366733712</v>
-      </c>
-      <c r="C10" t="s">
-        <v>133</v>
-      </c>
-    </row>
-    <row r="12" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A12" t="s">
-        <v>4</v>
-      </c>
-      <c r="B12">
-        <v>0.86</v>
-      </c>
-    </row>
-    <row r="13" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A13" t="s">
-        <v>250</v>
-      </c>
-      <c r="B13">
-        <v>0.8</v>
-      </c>
-    </row>
-    <row r="14" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A14" t="s">
-        <v>251</v>
-      </c>
-      <c r="B14">
-        <f>B13*B12</f>
-        <v>0.68800000000000006</v>
-      </c>
-    </row>
-    <row r="15" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A15" t="s">
-        <v>252</v>
-      </c>
-      <c r="B15">
-        <f>3500/(10*365.25)</f>
-        <v>0.95824777549623541</v>
-      </c>
-      <c r="C15" t="s">
-        <v>253</v>
-      </c>
-      <c r="H15" s="12" t="s">
-        <v>255</v>
-      </c>
-    </row>
-    <row r="17" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A17" t="s">
-        <v>256</v>
-      </c>
-      <c r="B17">
-        <v>4</v>
-      </c>
-      <c r="D17" s="12" t="s">
-        <v>255</v>
-      </c>
-    </row>
-    <row r="18" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A18" t="s">
-        <v>257</v>
-      </c>
-      <c r="B18">
-        <f>4/24</f>
-        <v>0.16666666666666666</v>
-      </c>
-    </row>
-    <row r="20" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A20" t="s">
-        <v>92</v>
-      </c>
-      <c r="C20" t="s">
-        <v>335</v>
-      </c>
-    </row>
-    <row r="22" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A22" t="s">
-        <v>157</v>
-      </c>
-      <c r="B22">
-        <v>61</v>
-      </c>
-      <c r="C22">
-        <v>106</v>
-      </c>
-      <c r="D22" t="s">
-        <v>336</v>
-      </c>
-    </row>
-    <row r="23" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="B23">
-        <f>4*B22</f>
-        <v>244</v>
-      </c>
-      <c r="C23">
-        <f>4*C22</f>
-        <v>424</v>
-      </c>
-      <c r="D23" t="s">
-        <v>337</v>
-      </c>
-      <c r="F23" t="s">
-        <v>338</v>
-      </c>
-    </row>
-    <row r="24" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="B24">
-        <f>B23*1000/(3500*0.8)</f>
-        <v>87.142857142857139</v>
-      </c>
-      <c r="C24">
-        <f>C23*1000/(3500*0.8)</f>
-        <v>151.42857142857142</v>
-      </c>
-      <c r="D24" t="s">
-        <v>158</v>
-      </c>
-    </row>
-    <row r="26" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="B26" t="s">
-        <v>339</v>
-      </c>
-    </row>
-    <row r="27" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="B27" t="s">
-        <v>340</v>
-      </c>
-    </row>
-    <row r="28" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="B28" t="s">
-        <v>341</v>
-      </c>
-    </row>
-    <row r="29" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="B29" t="s">
-        <v>342</v>
-      </c>
-    </row>
-  </sheetData>
-  <hyperlinks>
-    <hyperlink ref="G8" r:id="rId1" xr:uid="{FBA62C15-C46F-466D-88EE-057833A0FBBF}"/>
-    <hyperlink ref="H15" r:id="rId2" display="https://www.energy.gov/sites/prod/files/2019/07/f65/Storage Cost and Performance Characterization Report_Final.pdf" xr:uid="{CC1E61B7-8D26-483D-BD96-17B755561199}"/>
-    <hyperlink ref="D17" r:id="rId3" display="https://www.energy.gov/sites/prod/files/2019/07/f65/Storage Cost and Performance Characterization Report_Final.pdf" xr:uid="{21A611EC-C9B2-4050-A1CA-6AF325D4BE20}"/>
-    <hyperlink ref="G6" r:id="rId4" xr:uid="{B05A067C-8AEF-4EB3-866F-BAD051CBCD75}"/>
-    <hyperlink ref="G7" r:id="rId5" display="https://class.ece.uw.edu/500/2014aut-e/11-13-14 Pres (PSE Storage).pdf" xr:uid="{3D30F8E6-C466-4480-9055-FE94A828A64C}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -4540,10 +4594,10 @@
         <v>2025</v>
       </c>
       <c r="D3" s="18"/>
-      <c r="E3" s="26">
+      <c r="E3" s="29">
         <v>2040</v>
       </c>
-      <c r="F3" s="26"/>
+      <c r="F3" s="29"/>
       <c r="G3" t="s">
         <v>272</v>
       </c>
@@ -4907,7 +4961,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{403B81F9-D657-42BD-96F8-D40A873BAE34}">
   <dimension ref="A1:L24"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="O5" sqref="O5"/>
     </sheetView>
   </sheetViews>
@@ -5248,8 +5302,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{341C9435-D140-4ACE-89B8-673675A87D0E}">
   <dimension ref="A1:P44"/>
   <sheetViews>
-    <sheetView topLeftCell="A16" workbookViewId="0">
-      <selection activeCell="P40" sqref="P40"/>
+    <sheetView topLeftCell="A10" workbookViewId="0">
+      <selection activeCell="A38" sqref="A34:C38"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -5302,15 +5356,15 @@
       <c r="C3" t="s">
         <v>161</v>
       </c>
-      <c r="J3" s="26" t="s">
+      <c r="J3" s="29" t="s">
         <v>188</v>
       </c>
-      <c r="K3" s="26"/>
-      <c r="L3" s="26"/>
-      <c r="M3" s="26"/>
-      <c r="N3" s="26"/>
-      <c r="O3" s="26"/>
-      <c r="P3" s="26"/>
+      <c r="K3" s="29"/>
+      <c r="L3" s="29"/>
+      <c r="M3" s="29"/>
+      <c r="N3" s="29"/>
+      <c r="O3" s="29"/>
+      <c r="P3" s="29"/>
     </row>
     <row r="4" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
@@ -5800,15 +5854,15 @@
       <c r="C17" t="s">
         <v>214</v>
       </c>
-      <c r="J17" s="26" t="s">
+      <c r="J17" s="29" t="s">
         <v>193</v>
       </c>
-      <c r="K17" s="26"/>
-      <c r="L17" s="26"/>
-      <c r="M17" s="26"/>
-      <c r="N17" s="26"/>
-      <c r="O17" s="26"/>
-      <c r="P17" s="26"/>
+      <c r="K17" s="29"/>
+      <c r="L17" s="29"/>
+      <c r="M17" s="29"/>
+      <c r="N17" s="29"/>
+      <c r="O17" s="29"/>
+      <c r="P17" s="29"/>
     </row>
     <row r="18" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A18" s="2" t="s">
@@ -6270,15 +6324,15 @@
       <c r="E31">
         <v>0.7</v>
       </c>
-      <c r="J31" s="26" t="s">
+      <c r="J31" s="29" t="s">
         <v>194</v>
       </c>
-      <c r="K31" s="26"/>
-      <c r="L31" s="26"/>
-      <c r="M31" s="26"/>
-      <c r="N31" s="26"/>
-      <c r="O31" s="26"/>
-      <c r="P31" s="26"/>
+      <c r="K31" s="29"/>
+      <c r="L31" s="29"/>
+      <c r="M31" s="29"/>
+      <c r="N31" s="29"/>
+      <c r="O31" s="29"/>
+      <c r="P31" s="29"/>
     </row>
     <row r="32" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A32" s="2" t="s">
@@ -6925,10 +6979,10 @@
       <c r="G10" t="s">
         <v>91</v>
       </c>
-      <c r="J10" s="27" t="s">
+      <c r="J10" s="30" t="s">
         <v>80</v>
       </c>
-      <c r="K10" s="27"/>
+      <c r="K10" s="30"/>
       <c r="L10" s="11">
         <f>L9/G5</f>
         <v>122583.35123523093</v>
@@ -6938,10 +6992,10 @@
       </c>
     </row>
     <row r="11" spans="1:16" x14ac:dyDescent="0.3">
-      <c r="J11" s="27" t="s">
+      <c r="J11" s="30" t="s">
         <v>81</v>
       </c>
-      <c r="K11" s="27"/>
+      <c r="K11" s="30"/>
       <c r="L11" s="11">
         <f>M4*L10</f>
         <v>4086438.5967776584</v>
@@ -7649,7 +7703,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DB5DFEF8-915B-4056-B382-3EF1CD6D8429}">
   <dimension ref="A1:M39"/>
   <sheetViews>
-    <sheetView topLeftCell="A4" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+    <sheetView topLeftCell="A16" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
       <selection activeCell="A13" sqref="A13:C13"/>
     </sheetView>
   </sheetViews>
@@ -9009,190 +9063,320 @@
 </file>
 
 <file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BFB7227C-A1DE-45C0-910C-0F614B128A68}">
-  <dimension ref="A1:K19"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2E6C6BEB-6091-4743-A766-86BDD24D0263}">
+  <dimension ref="A1:J29"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="O21" sqref="O21"/>
+    <sheetView topLeftCell="A13" zoomScale="175" zoomScaleNormal="175" workbookViewId="0">
+      <selection activeCell="B24" sqref="B24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="15.21875" customWidth="1"/>
-    <col min="2" max="2" width="10.88671875" customWidth="1"/>
+    <col min="1" max="1" width="17.6640625" customWidth="1"/>
+    <col min="2" max="2" width="10.44140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="B1" t="s">
-        <v>281</v>
+    <row r="1" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A1" t="s">
+        <v>220</v>
+      </c>
+      <c r="B1">
+        <v>377970</v>
       </c>
       <c r="C1" t="s">
-        <v>114</v>
-      </c>
-      <c r="J1">
-        <v>33.335999999999999</v>
-      </c>
-      <c r="K1" t="s">
+        <v>221</v>
+      </c>
+    </row>
+    <row r="2" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A2" t="s">
+        <v>222</v>
+      </c>
+      <c r="B2">
+        <v>251000</v>
+      </c>
+      <c r="C2" t="s">
+        <v>221</v>
+      </c>
+    </row>
+    <row r="3" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A3" t="s">
+        <v>223</v>
+      </c>
+      <c r="B3">
+        <v>7.5</v>
+      </c>
+      <c r="C3" t="s">
+        <v>224</v>
+      </c>
+      <c r="I3">
+        <v>4.0468600000000002E-3</v>
+      </c>
+      <c r="J3" t="s">
+        <v>225</v>
+      </c>
+    </row>
+    <row r="4" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="B4">
+        <f>B3*I3*1000</f>
+        <v>30.351450000000003</v>
+      </c>
+      <c r="C4" t="s">
+        <v>226</v>
+      </c>
+      <c r="I4" s="16">
+        <v>9.2902999999999995E-8</v>
+      </c>
+      <c r="J4" t="s">
+        <v>248</v>
+      </c>
+    </row>
+    <row r="5" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A5" t="s">
+        <v>227</v>
+      </c>
+      <c r="B5">
+        <f>300*B4</f>
+        <v>9105.4350000000013</v>
+      </c>
+      <c r="C5" t="s">
+        <v>221</v>
+      </c>
+      <c r="D5">
+        <f>B5*100/B2</f>
+        <v>3.6276633466135464</v>
+      </c>
+      <c r="E5" t="s">
+        <v>234</v>
+      </c>
+    </row>
+    <row r="6" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A6" t="s">
+        <v>246</v>
+      </c>
+      <c r="B6">
+        <f>1.5/20</f>
+        <v>7.4999999999999997E-2</v>
+      </c>
+      <c r="C6" t="s">
+        <v>259</v>
+      </c>
+      <c r="D6" s="16">
+        <f>B6*I3*1000</f>
+        <v>0.30351450000000002</v>
+      </c>
+      <c r="E6" t="s">
+        <v>249</v>
+      </c>
+      <c r="G6" s="12" t="s">
+        <v>260</v>
+      </c>
+    </row>
+    <row r="7" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="B7">
+        <v>0.04</v>
+      </c>
+      <c r="C7" t="s">
+        <v>259</v>
+      </c>
+      <c r="D7" s="16">
+        <f>B7*I3*1000</f>
+        <v>0.1618744</v>
+      </c>
+      <c r="E7" t="s">
+        <v>249</v>
+      </c>
+      <c r="G7" s="12" t="s">
+        <v>261</v>
+      </c>
+    </row>
+    <row r="8" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="B8">
+        <f>76800/60</f>
+        <v>1280</v>
+      </c>
+      <c r="C8" t="s">
+        <v>247</v>
+      </c>
+      <c r="D8" s="16">
+        <f>B8*I4*1000</f>
+        <v>0.11891583999999998</v>
+      </c>
+      <c r="E8" t="s">
+        <v>249</v>
+      </c>
+      <c r="G8" s="12" t="s">
+        <v>254</v>
+      </c>
+    </row>
+    <row r="9" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A9" t="s">
+        <v>245</v>
+      </c>
+      <c r="B9">
+        <f>D9*B2/100</f>
+        <v>7530</v>
+      </c>
+      <c r="C9" t="s">
+        <v>221</v>
+      </c>
+      <c r="D9">
         <v>3</v>
       </c>
-    </row>
-    <row r="2" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A2">
-        <v>2017</v>
-      </c>
-      <c r="B2">
-        <f>29*1/100</f>
-        <v>0.28999999999999998</v>
-      </c>
-      <c r="C2">
-        <f>B2*1000/J1</f>
-        <v>8.6993040556755457</v>
-      </c>
-    </row>
-    <row r="3" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A3">
-        <v>2050</v>
-      </c>
-      <c r="B3">
-        <f>4*1/100</f>
-        <v>0.04</v>
-      </c>
-      <c r="C3">
-        <f>B3*1000/J1</f>
-        <v>1.1999040076793857</v>
-      </c>
-      <c r="D3" s="12" t="s">
-        <v>279</v>
-      </c>
-    </row>
-    <row r="5" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A5" t="s">
-        <v>284</v>
-      </c>
-      <c r="B5">
-        <f>3000*10</f>
-        <v>30000</v>
-      </c>
-      <c r="D5" t="s">
-        <v>329</v>
-      </c>
-    </row>
-    <row r="6" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A6" t="s">
-        <v>285</v>
-      </c>
-      <c r="B6">
-        <f>B5*C3</f>
-        <v>35997.120230381566</v>
-      </c>
-      <c r="C6" t="s">
-        <v>286</v>
-      </c>
-    </row>
-    <row r="7" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A7" t="s">
-        <v>287</v>
-      </c>
-      <c r="B7">
-        <f>B6/(8760*0.9*7)</f>
-        <v>0.6522635397256934</v>
-      </c>
-      <c r="C7" t="s">
-        <v>330</v>
-      </c>
-    </row>
-    <row r="8" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A8" t="s">
-        <v>287</v>
-      </c>
-      <c r="B8">
-        <f>B6/(8760*0.9*10)</f>
-        <v>0.45658447780798539</v>
-      </c>
-      <c r="C8" t="s">
-        <v>331</v>
-      </c>
-    </row>
-    <row r="9" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="D9" s="12" t="s">
-        <v>280</v>
-      </c>
-    </row>
-    <row r="11" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="H11" s="12" t="s">
-        <v>345</v>
-      </c>
-    </row>
-    <row r="12" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A12" s="20">
-        <v>2022</v>
-      </c>
-      <c r="B12" s="20">
-        <v>3800</v>
-      </c>
-      <c r="H12" s="12" t="s">
-        <v>344</v>
-      </c>
-    </row>
-    <row r="13" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A13" s="20">
-        <v>2030</v>
-      </c>
-      <c r="B13" s="20">
-        <v>1500</v>
-      </c>
-      <c r="H13" s="12" t="s">
-        <v>324</v>
-      </c>
-    </row>
-    <row r="14" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A14">
-        <v>2050</v>
+      <c r="E9" t="s">
+        <v>234</v>
+      </c>
+    </row>
+    <row r="10" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A10" t="s">
+        <v>241</v>
+      </c>
+      <c r="B10" s="16">
+        <f>B9/D6</f>
+        <v>24809.358366733712</v>
+      </c>
+      <c r="C10" t="s">
+        <v>133</v>
+      </c>
+    </row>
+    <row r="12" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A12" t="s">
+        <v>4</v>
+      </c>
+      <c r="B12">
+        <v>0.86</v>
+      </c>
+    </row>
+    <row r="13" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A13" t="s">
+        <v>250</v>
+      </c>
+      <c r="B13">
+        <v>0.8</v>
+      </c>
+    </row>
+    <row r="14" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A14" t="s">
+        <v>251</v>
       </c>
       <c r="B14">
-        <v>400</v>
-      </c>
-    </row>
-    <row r="17" spans="1:8" x14ac:dyDescent="0.3">
+        <f>B13*B12</f>
+        <v>0.68800000000000006</v>
+      </c>
+    </row>
+    <row r="15" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A15" t="s">
+        <v>252</v>
+      </c>
+      <c r="B15">
+        <f>3500/(10*365.25)</f>
+        <v>0.95824777549623541</v>
+      </c>
+      <c r="C15" t="s">
+        <v>253</v>
+      </c>
+      <c r="H15" s="12" t="s">
+        <v>255</v>
+      </c>
+    </row>
+    <row r="17" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A17" t="s">
+        <v>256</v>
+      </c>
+      <c r="B17">
         <v>4</v>
       </c>
-      <c r="B17">
-        <v>82</v>
-      </c>
-      <c r="C17" s="20"/>
-      <c r="D17" s="28" t="s">
-        <v>349</v>
-      </c>
-      <c r="H17" t="s">
-        <v>351</v>
-      </c>
-    </row>
-    <row r="18" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="C18" s="20"/>
-      <c r="D18" s="12" t="s">
-        <v>350</v>
-      </c>
-      <c r="H18" t="s">
-        <v>354</v>
-      </c>
-    </row>
-    <row r="19" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="D19" s="12" t="s">
-        <v>352</v>
+      <c r="D17" s="12" t="s">
+        <v>255</v>
+      </c>
+    </row>
+    <row r="18" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A18" t="s">
+        <v>257</v>
+      </c>
+      <c r="B18">
+        <f>4/24</f>
+        <v>0.16666666666666666</v>
+      </c>
+    </row>
+    <row r="20" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A20" t="s">
+        <v>92</v>
+      </c>
+      <c r="C20" t="s">
+        <v>335</v>
+      </c>
+    </row>
+    <row r="22" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A22" t="s">
+        <v>157</v>
+      </c>
+      <c r="B22">
+        <v>61</v>
+      </c>
+      <c r="C22">
+        <v>106</v>
+      </c>
+      <c r="D22" t="s">
+        <v>336</v>
+      </c>
+    </row>
+    <row r="23" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="B23">
+        <f>4*B22</f>
+        <v>244</v>
+      </c>
+      <c r="C23">
+        <f>4*C22</f>
+        <v>424</v>
+      </c>
+      <c r="D23" t="s">
+        <v>337</v>
+      </c>
+      <c r="F23" t="s">
+        <v>338</v>
+      </c>
+    </row>
+    <row r="24" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="B24">
+        <f>B23*1000/(3500*0.8)</f>
+        <v>87.142857142857139</v>
+      </c>
+      <c r="C24">
+        <f>C23*1000/(3500*0.8)</f>
+        <v>151.42857142857142</v>
+      </c>
+      <c r="D24" t="s">
+        <v>158</v>
+      </c>
+    </row>
+    <row r="26" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="B26" t="s">
+        <v>339</v>
+      </c>
+    </row>
+    <row r="27" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="B27" t="s">
+        <v>340</v>
+      </c>
+    </row>
+    <row r="28" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="B28" t="s">
+        <v>341</v>
+      </c>
+    </row>
+    <row r="29" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="B29" t="s">
+        <v>342</v>
       </c>
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="D3" r:id="rId1" xr:uid="{73261102-8930-4034-AFBD-8AF2404129E0}"/>
-    <hyperlink ref="D9" r:id="rId2" display="https://urldefense.proofpoint.com/v2/url?u=https-3A__doi.org_10.3390_environments5020024&amp;d=DwMFaQ&amp;c=OCIEmEwdEq_aNlsP4fF3gFqSN-E3mlr2t9JcDdfOZag&amp;r=79oVBkpSJ8jc8Mw2l8LuV83qCNXLl72NkphdMlliukM&amp;m=NGWcOQO2qa2PKM1ngjeYDCH3rElV-XSihhWPcRPvzOs&amp;s=sFKFBAwrUGsHBL-aJtbQE7lcIp4piSa0kz-mx0PEbR4&amp;e=" xr:uid="{320B681C-F103-4058-B8E2-518FF78252CD}"/>
-    <hyperlink ref="H13" r:id="rId3" tooltip="Persistent link using digital object identifier" xr:uid="{B3E006C3-DDB9-480A-9D90-5884D6F5F9E8}"/>
-    <hyperlink ref="H12" r:id="rId4" xr:uid="{737771D8-B96A-49B6-86D2-864FF1155855}"/>
-    <hyperlink ref="H11" r:id="rId5" xr:uid="{63C37621-088F-42CB-A35E-1ECFDE9D82C3}"/>
-    <hyperlink ref="D18" r:id="rId6" xr:uid="{18AE47F8-0B31-409D-88A0-14B43BA66492}"/>
-    <hyperlink ref="D19" r:id="rId7" xr:uid="{BD971C0B-0989-4A61-909C-C1F9A507336B}"/>
+    <hyperlink ref="G8" r:id="rId1" xr:uid="{FBA62C15-C46F-466D-88EE-057833A0FBBF}"/>
+    <hyperlink ref="H15" r:id="rId2" display="https://www.energy.gov/sites/prod/files/2019/07/f65/Storage Cost and Performance Characterization Report_Final.pdf" xr:uid="{CC1E61B7-8D26-483D-BD96-17B755561199}"/>
+    <hyperlink ref="D17" r:id="rId3" display="https://www.energy.gov/sites/prod/files/2019/07/f65/Storage Cost and Performance Characterization Report_Final.pdf" xr:uid="{21A611EC-C9B2-4050-A1CA-6AF325D4BE20}"/>
+    <hyperlink ref="G6" r:id="rId4" xr:uid="{B05A067C-8AEF-4EB3-866F-BAD051CBCD75}"/>
+    <hyperlink ref="G7" r:id="rId5" display="https://class.ece.uw.edu/500/2014aut-e/11-13-14 Pres (PSE Storage).pdf" xr:uid="{3D30F8E6-C466-4480-9055-FE94A828A64C}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId8"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
added intro and litreview draft
Former-commit-id: 9e8d3fb3816dc710a72af07e4eefa25d914aceb5
Former-commit-id: 65e2ca89214491e667fb2548c45b9cb86e03f1ff
</commit_message>
<xml_diff>
--- a/data/tech-economic-data.xlsx
+++ b/data/tech-economic-data.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\github\i2cner\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{88371D5E-61CC-4AB5-BE31-95A64361A5F6}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F5950392-763F-4B3A-9576-BF21698557BA}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{ECBC9880-2B97-44EA-9887-629A306A84A1}"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{ECBC9880-2B97-44EA-9887-629A306A84A1}"/>
   </bookViews>
   <sheets>
     <sheet name="CCS_Costs_Early" sheetId="14" r:id="rId1"/>
@@ -29,6 +29,8 @@
     <sheet name="PEMFC" sheetId="19" r:id="rId14"/>
     <sheet name="EIA_LCOE_WND_SOLAR" sheetId="11" r:id="rId15"/>
     <sheet name="Photoconversion" sheetId="16" r:id="rId16"/>
+    <sheet name="Fossil fuel price" sheetId="22" r:id="rId17"/>
+    <sheet name="Cap limits" sheetId="26" r:id="rId18"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -46,7 +48,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="762" uniqueCount="387">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="805" uniqueCount="408">
   <si>
     <t>H2 Method</t>
   </si>
@@ -1179,34 +1181,97 @@
     <t>Life Cycle Emissions</t>
   </si>
   <si>
-    <t>CCS PC</t>
-  </si>
-  <si>
     <t>Total Emi</t>
   </si>
   <si>
     <t>Direct Emi</t>
   </si>
   <si>
-    <t>CCS Gas CC</t>
-  </si>
-  <si>
     <t>https://www.energy.gov/sites/prod/files/2014/03/f12/27637.pdf</t>
   </si>
   <si>
     <t>Steam reforming+CCS</t>
   </si>
   <si>
-    <t>PC</t>
-  </si>
-  <si>
-    <t>Gas CC</t>
-  </si>
-  <si>
     <t>CO2 Cap</t>
   </si>
   <si>
     <t>Emi build</t>
+  </si>
+  <si>
+    <t>ELC/LNG</t>
+  </si>
+  <si>
+    <t>ELC use</t>
+  </si>
+  <si>
+    <t>1 MBTU</t>
+  </si>
+  <si>
+    <t>$/MBTU</t>
+  </si>
+  <si>
+    <t>1$</t>
+  </si>
+  <si>
+    <t>https://www.fepc.or.jp/english/library/electricity_eview_japan/__icsFiles/afieldfile/2020/03/11/2019ERJ_full.pdf</t>
+  </si>
+  <si>
+    <t>Coal JPN</t>
+  </si>
+  <si>
+    <t>Gas CC JPN</t>
+  </si>
+  <si>
+    <t>CCS PC IPCC</t>
+  </si>
+  <si>
+    <t>CCS Gas CC IPCC</t>
+  </si>
+  <si>
+    <t>Potential</t>
+  </si>
+  <si>
+    <t>Source: Kato</t>
+  </si>
+  <si>
+    <t>Given</t>
+  </si>
+  <si>
+    <t>Max</t>
+  </si>
+  <si>
+    <t>CCS Gas PC JPN</t>
+  </si>
+  <si>
+    <t>CCS Gas CC JPN</t>
+  </si>
+  <si>
+    <t>Coal IPCC</t>
+  </si>
+  <si>
+    <t>Gas CC IPCC</t>
+  </si>
+  <si>
+    <t>Offshore Fixed</t>
+  </si>
+  <si>
+    <t>Offshore Floating</t>
+  </si>
+  <si>
+    <t>https://www.nrel.gov/docs/fy01osti/27637.pdf</t>
+  </si>
+  <si>
+    <t>Total cap cost</t>
+  </si>
+  <si>
+    <t>Eur/kw</t>
+  </si>
+  <si>
+    <t>Opex</t>
+  </si>
+  <si>
+    <t>Eur/kw/y</t>
   </si>
 </sst>
 </file>
@@ -1217,7 +1282,7 @@
     <numFmt numFmtId="164" formatCode="0.000E+00"/>
     <numFmt numFmtId="165" formatCode="0.00000000E+00"/>
   </numFmts>
-  <fonts count="16" x14ac:knownFonts="1">
+  <fonts count="15" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -1318,12 +1383,6 @@
     <font>
       <sz val="8"/>
       <color rgb="FF0C7DBB"/>
-      <name val="Arial"/>
-      <family val="2"/>
-    </font>
-    <font>
-      <sz val="8"/>
-      <color rgb="FF006FCA"/>
       <name val="Arial"/>
       <family val="2"/>
     </font>
@@ -1433,13 +1492,13 @@
     <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="11" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="3">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -1756,10 +1815,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DA3B25EB-4023-477D-80C4-74718858ACC8}">
-  <dimension ref="A1:P50"/>
+  <dimension ref="A1:P54"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A31" workbookViewId="0">
-      <selection activeCell="B47" sqref="B47"/>
+    <sheetView tabSelected="1" topLeftCell="A22" workbookViewId="0">
+      <selection activeCell="J50" sqref="J50"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1812,15 +1871,15 @@
       <c r="C3" t="s">
         <v>161</v>
       </c>
-      <c r="J3" s="29" t="s">
+      <c r="J3" s="30" t="s">
         <v>188</v>
       </c>
-      <c r="K3" s="29"/>
-      <c r="L3" s="29"/>
-      <c r="M3" s="29"/>
-      <c r="N3" s="29"/>
-      <c r="O3" s="29"/>
-      <c r="P3" s="29"/>
+      <c r="K3" s="30"/>
+      <c r="L3" s="30"/>
+      <c r="M3" s="30"/>
+      <c r="N3" s="30"/>
+      <c r="O3" s="30"/>
+      <c r="P3" s="30"/>
     </row>
     <row r="4" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
@@ -2310,15 +2369,15 @@
       <c r="C17" t="s">
         <v>214</v>
       </c>
-      <c r="J17" s="29" t="s">
+      <c r="J17" s="30" t="s">
         <v>193</v>
       </c>
-      <c r="K17" s="29"/>
-      <c r="L17" s="29"/>
-      <c r="M17" s="29"/>
-      <c r="N17" s="29"/>
-      <c r="O17" s="29"/>
-      <c r="P17" s="29"/>
+      <c r="K17" s="30"/>
+      <c r="L17" s="30"/>
+      <c r="M17" s="30"/>
+      <c r="N17" s="30"/>
+      <c r="O17" s="30"/>
+      <c r="P17" s="30"/>
     </row>
     <row r="18" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A18" s="2" t="s">
@@ -2780,15 +2839,15 @@
       <c r="E31">
         <v>0.7</v>
       </c>
-      <c r="J31" s="29" t="s">
+      <c r="J31" s="30" t="s">
         <v>194</v>
       </c>
-      <c r="K31" s="29"/>
-      <c r="L31" s="29"/>
-      <c r="M31" s="29"/>
-      <c r="N31" s="29"/>
-      <c r="O31" s="29"/>
-      <c r="P31" s="29"/>
+      <c r="K31" s="30"/>
+      <c r="L31" s="30"/>
+      <c r="M31" s="30"/>
+      <c r="N31" s="30"/>
+      <c r="O31" s="30"/>
+      <c r="P31" s="30"/>
     </row>
     <row r="32" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A32" s="2" t="s">
@@ -2827,23 +2886,23 @@
       </c>
       <c r="K33" s="3">
         <f t="shared" ref="K33:K44" si="12">$B$37*J33</f>
-        <v>1.8722199999999996E-4</v>
+        <v>2.0999999999999998E-4</v>
       </c>
       <c r="L33" s="3">
         <f t="shared" ref="L33:L44" si="13">K33*$B$12</f>
-        <v>0.13637801476977224</v>
+        <v>0.15297018032951348</v>
       </c>
       <c r="N33" s="3">
         <f t="shared" ref="N33:N44" si="14">$E$31-L33</f>
-        <v>0.56362198523022777</v>
+        <v>0.54702981967048647</v>
       </c>
       <c r="O33" s="3">
         <f t="shared" ref="O33:O44" si="15">K33*$B$21</f>
-        <v>2.4488637599999998E-2</v>
+        <v>2.7467999999999999E-2</v>
       </c>
       <c r="P33" s="3">
         <f>$D$31+O33</f>
-        <v>6.5328945111999312E-2</v>
+        <v>6.8308307511999317E-2</v>
       </c>
     </row>
     <row r="34" spans="1:16" x14ac:dyDescent="0.3">
@@ -2855,24 +2914,24 @@
       </c>
       <c r="K34" s="3">
         <f t="shared" si="12"/>
-        <v>2.2734099999999996E-4</v>
+        <v>2.5499999999999996E-4</v>
       </c>
       <c r="L34" s="3">
         <f>K34*$B$12</f>
-        <v>0.16560187507758059</v>
+        <v>0.18574950468583779</v>
       </c>
       <c r="M34" s="3"/>
       <c r="N34" s="3">
         <f>$E$31-L34</f>
-        <v>0.53439812492241934</v>
+        <v>0.51425049531416223</v>
       </c>
       <c r="O34" s="3">
         <f>K34*$B$21</f>
-        <v>2.9736202799999997E-2</v>
+        <v>3.3353999999999995E-2</v>
       </c>
       <c r="P34" s="3">
         <f t="shared" ref="P34:P44" si="16">$D$31+O34</f>
-        <v>7.057651031199931E-2</v>
+        <v>7.4194307511999305E-2</v>
       </c>
     </row>
     <row r="35" spans="1:16" x14ac:dyDescent="0.3">
@@ -2891,24 +2950,24 @@
       </c>
       <c r="K35" s="3">
         <f t="shared" si="12"/>
-        <v>2.3001559999999996E-4</v>
+        <v>2.5799999999999998E-4</v>
       </c>
       <c r="L35" s="3">
         <f t="shared" si="13"/>
-        <v>0.16755013243143446</v>
+        <v>0.18793479297625942</v>
       </c>
       <c r="M35" s="3"/>
       <c r="N35" s="3">
         <f t="shared" si="14"/>
-        <v>0.53244986756856549</v>
+        <v>0.51206520702374059</v>
       </c>
       <c r="O35" s="3">
         <f t="shared" si="15"/>
-        <v>3.0086040479999996E-2</v>
+        <v>3.3746400000000003E-2</v>
       </c>
       <c r="P35" s="3">
         <f t="shared" si="16"/>
-        <v>7.0926347991999303E-2</v>
+        <v>7.4586707511999306E-2</v>
       </c>
     </row>
     <row r="36" spans="1:16" x14ac:dyDescent="0.3">
@@ -2927,24 +2986,24 @@
       </c>
       <c r="K36" s="3">
         <f t="shared" si="12"/>
-        <v>2.3269019999999996E-4</v>
+        <v>2.61E-4</v>
       </c>
       <c r="L36" s="3">
         <f t="shared" si="13"/>
-        <v>0.16949838978528836</v>
+        <v>0.19012008126668106</v>
       </c>
       <c r="M36" s="3"/>
       <c r="N36" s="3">
         <f t="shared" si="14"/>
-        <v>0.53050161021471154</v>
+        <v>0.50987991873331895</v>
       </c>
       <c r="O36" s="3">
         <f t="shared" si="15"/>
-        <v>3.0435878159999995E-2</v>
+        <v>3.4138800000000004E-2</v>
       </c>
       <c r="P36" s="3">
         <f t="shared" si="16"/>
-        <v>7.1276185671999309E-2</v>
+        <v>7.4979107511999321E-2</v>
       </c>
     </row>
     <row r="37" spans="1:16" x14ac:dyDescent="0.3">
@@ -2952,38 +3011,38 @@
         <v>111</v>
       </c>
       <c r="B37" s="21">
-        <f>267.46/1000000</f>
-        <v>2.6745999999999996E-4</v>
+        <f>C53/1000000</f>
+        <v>2.9999999999999997E-4</v>
       </c>
       <c r="C37" t="s">
         <v>62</v>
       </c>
       <c r="D37" t="s">
-        <v>381</v>
+        <v>379</v>
       </c>
       <c r="J37" s="3">
         <v>0.88</v>
       </c>
       <c r="K37" s="3">
         <f t="shared" si="12"/>
-        <v>2.3536479999999998E-4</v>
+        <v>2.6399999999999997E-4</v>
       </c>
       <c r="L37" s="3">
         <f t="shared" si="13"/>
-        <v>0.17144664713914226</v>
+        <v>0.19230536955710267</v>
       </c>
       <c r="M37" s="3"/>
       <c r="N37" s="3">
         <f t="shared" si="14"/>
-        <v>0.52855335286085769</v>
+        <v>0.50769463044289731</v>
       </c>
       <c r="O37" s="3">
         <f t="shared" si="15"/>
-        <v>3.0785715839999998E-2</v>
+        <v>3.4531199999999998E-2</v>
       </c>
       <c r="P37" s="3">
         <f t="shared" si="16"/>
-        <v>7.1626023351999302E-2</v>
+        <v>7.5371507511999308E-2</v>
       </c>
     </row>
     <row r="38" spans="1:16" x14ac:dyDescent="0.3">
@@ -2992,24 +3051,24 @@
       </c>
       <c r="K38" s="3">
         <f t="shared" si="12"/>
-        <v>2.3803939999999998E-4</v>
+        <v>2.6699999999999998E-4</v>
       </c>
       <c r="L38" s="3">
         <f t="shared" si="13"/>
-        <v>0.17339490449299616</v>
+        <v>0.19449065784752431</v>
       </c>
       <c r="M38" s="3"/>
       <c r="N38" s="3">
         <f t="shared" si="14"/>
-        <v>0.52660509550700385</v>
+        <v>0.50550934215247567</v>
       </c>
       <c r="O38" s="3">
         <f t="shared" si="15"/>
-        <v>3.1135553520000001E-2</v>
+        <v>3.4923599999999999E-2</v>
       </c>
       <c r="P38" s="3">
         <f t="shared" si="16"/>
-        <v>7.1975861031999308E-2</v>
+        <v>7.5763907511999309E-2</v>
       </c>
     </row>
     <row r="39" spans="1:16" x14ac:dyDescent="0.3">
@@ -3018,24 +3077,24 @@
       </c>
       <c r="K39" s="3">
         <f t="shared" si="12"/>
-        <v>2.4071399999999997E-4</v>
+        <v>2.7E-4</v>
       </c>
       <c r="L39" s="3">
         <f t="shared" si="13"/>
-        <v>0.17534316184685003</v>
+        <v>0.19667594613794592</v>
       </c>
       <c r="M39" s="3"/>
       <c r="N39" s="3">
         <f t="shared" si="14"/>
-        <v>0.5246568381531499</v>
+        <v>0.50332405386205403</v>
       </c>
       <c r="O39" s="3">
         <f t="shared" si="15"/>
-        <v>3.1485391199999997E-2</v>
+        <v>3.5316E-2</v>
       </c>
       <c r="P39" s="3">
         <f t="shared" si="16"/>
-        <v>7.2325698711999314E-2</v>
+        <v>7.615630751199931E-2</v>
       </c>
     </row>
     <row r="40" spans="1:16" x14ac:dyDescent="0.3">
@@ -3047,24 +3106,24 @@
       </c>
       <c r="K40" s="3">
         <f t="shared" si="12"/>
-        <v>2.4338859999999997E-4</v>
+        <v>2.7299999999999997E-4</v>
       </c>
       <c r="L40" s="3">
         <f t="shared" si="13"/>
-        <v>0.17729141920070393</v>
+        <v>0.19886123442836753</v>
       </c>
       <c r="M40" s="3"/>
       <c r="N40" s="3">
         <f t="shared" si="14"/>
-        <v>0.52270858079929605</v>
+        <v>0.50113876557163239</v>
       </c>
       <c r="O40" s="3">
         <f t="shared" si="15"/>
-        <v>3.1835228879999997E-2</v>
+        <v>3.5708400000000001E-2</v>
       </c>
       <c r="P40" s="3">
         <f t="shared" si="16"/>
-        <v>7.2675536391999307E-2</v>
+        <v>7.6548707511999312E-2</v>
       </c>
     </row>
     <row r="41" spans="1:16" x14ac:dyDescent="0.3">
@@ -3076,53 +3135,50 @@
       </c>
       <c r="K41" s="3">
         <f t="shared" si="12"/>
-        <v>2.4606319999999999E-4</v>
+        <v>2.7599999999999999E-4</v>
       </c>
       <c r="L41" s="3">
         <f t="shared" si="13"/>
-        <v>0.17923967655455783</v>
+        <v>0.20104652271878917</v>
       </c>
       <c r="M41" s="3"/>
       <c r="N41" s="3">
         <f t="shared" si="14"/>
-        <v>0.5207603234454421</v>
+        <v>0.49895347728121076</v>
       </c>
       <c r="O41" s="3">
         <f t="shared" si="15"/>
-        <v>3.2185066560000003E-2</v>
+        <v>3.6100800000000002E-2</v>
       </c>
       <c r="P41" s="3">
         <f t="shared" si="16"/>
-        <v>7.3025374071999313E-2</v>
+        <v>7.6941107511999313E-2</v>
       </c>
     </row>
     <row r="42" spans="1:16" x14ac:dyDescent="0.3">
-      <c r="A42" s="31" t="s">
-        <v>375</v>
-      </c>
       <c r="J42" s="3">
         <v>0.93</v>
       </c>
       <c r="K42" s="3">
         <f t="shared" si="12"/>
-        <v>2.4873779999999996E-4</v>
+        <v>2.7900000000000001E-4</v>
       </c>
       <c r="L42" s="3">
         <f t="shared" si="13"/>
-        <v>0.1811879339084117</v>
+        <v>0.20323181100921081</v>
       </c>
       <c r="M42" s="3"/>
       <c r="N42" s="3">
         <f t="shared" si="14"/>
-        <v>0.51881206609158825</v>
+        <v>0.49676818899078912</v>
       </c>
       <c r="O42" s="3">
         <f t="shared" si="15"/>
-        <v>3.2534904239999995E-2</v>
+        <v>3.6493200000000003E-2</v>
       </c>
       <c r="P42" s="3">
         <f t="shared" si="16"/>
-        <v>7.3375211751999306E-2</v>
+        <v>7.7333507511999314E-2</v>
       </c>
     </row>
     <row r="43" spans="1:16" x14ac:dyDescent="0.3">
@@ -3134,24 +3190,24 @@
       </c>
       <c r="K43" s="3">
         <f t="shared" si="12"/>
-        <v>2.5141239999999993E-4</v>
+        <v>2.8199999999999997E-4</v>
       </c>
       <c r="L43" s="3">
         <f t="shared" si="13"/>
-        <v>0.18313619126226557</v>
+        <v>0.20541709929963239</v>
       </c>
       <c r="M43" s="3"/>
       <c r="N43" s="3">
         <f t="shared" si="14"/>
-        <v>0.51686380873773441</v>
+        <v>0.49458290070036759</v>
       </c>
       <c r="O43" s="3">
         <f t="shared" si="15"/>
-        <v>3.2884741919999995E-2</v>
+        <v>3.6885599999999998E-2</v>
       </c>
       <c r="P43" s="3">
         <f t="shared" si="16"/>
-        <v>7.3725049431999312E-2</v>
+        <v>7.7725907511999315E-2</v>
       </c>
     </row>
     <row r="44" spans="1:16" x14ac:dyDescent="0.3">
@@ -3159,45 +3215,45 @@
         <v>376</v>
       </c>
       <c r="B44" t="s">
+        <v>377</v>
+      </c>
+      <c r="C44" t="s">
         <v>378</v>
       </c>
-      <c r="C44" t="s">
-        <v>379</v>
-      </c>
       <c r="D44" t="s">
-        <v>386</v>
+        <v>382</v>
       </c>
       <c r="E44" t="s">
-        <v>385</v>
+        <v>381</v>
       </c>
       <c r="J44" s="3">
         <v>0.95</v>
       </c>
       <c r="K44" s="3">
         <f t="shared" si="12"/>
-        <v>2.5408699999999995E-4</v>
+        <v>2.8499999999999999E-4</v>
       </c>
       <c r="L44" s="3">
         <f t="shared" si="13"/>
-        <v>0.18508444861611947</v>
+        <v>0.20760238759005403</v>
       </c>
       <c r="M44" s="3"/>
       <c r="N44" s="3">
         <f t="shared" si="14"/>
-        <v>0.51491555138388045</v>
+        <v>0.49239761240994595</v>
       </c>
       <c r="O44" s="3">
         <f t="shared" si="15"/>
-        <v>3.3234579599999994E-2</v>
+        <v>3.7277999999999999E-2</v>
       </c>
       <c r="P44" s="3">
         <f t="shared" si="16"/>
-        <v>7.4074887111999305E-2</v>
+        <v>7.8118307511999302E-2</v>
       </c>
     </row>
     <row r="45" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A45" t="s">
-        <v>383</v>
+        <v>399</v>
       </c>
       <c r="B45">
         <v>820</v>
@@ -3206,16 +3262,16 @@
         <v>760</v>
       </c>
       <c r="D45">
-        <f>B45-C45</f>
+        <f t="shared" ref="D45:D50" si="17">B45-C45</f>
         <v>60</v>
       </c>
-      <c r="E45">
-        <v>0</v>
+      <c r="F45" s="12" t="s">
+        <v>388</v>
       </c>
     </row>
     <row r="46" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A46" t="s">
-        <v>384</v>
+        <v>400</v>
       </c>
       <c r="B46">
         <v>490</v>
@@ -3224,92 +3280,158 @@
         <v>370</v>
       </c>
       <c r="D46">
-        <f>B46-C46</f>
+        <f t="shared" si="17"/>
         <v>120</v>
-      </c>
-      <c r="E46">
-        <v>0</v>
       </c>
     </row>
     <row r="47" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A47" t="s">
-        <v>377</v>
+        <v>389</v>
       </c>
       <c r="B47">
-        <v>220</v>
+        <v>943</v>
       </c>
       <c r="C47">
-        <f>0.1*760</f>
-        <v>76</v>
+        <v>864</v>
       </c>
       <c r="D47">
-        <f>B47-C47</f>
-        <v>144</v>
+        <f t="shared" si="17"/>
+        <v>79</v>
       </c>
       <c r="E47">
-        <f>C45-C47</f>
-        <v>684</v>
+        <v>0</v>
+      </c>
+      <c r="F47" s="12" t="s">
+        <v>375</v>
       </c>
     </row>
     <row r="48" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A48" t="s">
-        <v>380</v>
+        <v>390</v>
       </c>
       <c r="B48">
-        <v>170</v>
+        <v>599</v>
       </c>
       <c r="C48">
-        <f>0.1*370</f>
-        <v>37</v>
+        <v>476</v>
       </c>
       <c r="D48">
-        <f>B48-C48</f>
-        <v>133</v>
+        <f t="shared" si="17"/>
+        <v>123</v>
       </c>
       <c r="E48">
-        <f>C46-C48</f>
-        <v>333</v>
+        <v>0</v>
       </c>
     </row>
     <row r="49" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A49" t="s">
-        <v>13</v>
+        <v>391</v>
       </c>
       <c r="B49">
-        <f>11888/33.336</f>
-        <v>356.61147108231341</v>
+        <v>190</v>
       </c>
       <c r="C49">
-        <f>B49*0.75</f>
-        <v>267.45860331173503</v>
+        <v>76</v>
       </c>
       <c r="D49">
-        <f>0.25*B49</f>
-        <v>89.152867770578354</v>
-      </c>
-      <c r="E49">
-        <v>0</v>
+        <f t="shared" si="17"/>
+        <v>114</v>
       </c>
     </row>
     <row r="50" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A50" t="s">
-        <v>382</v>
+        <v>392</v>
       </c>
       <c r="B50">
-        <f>C50+D50</f>
-        <v>179.04867610591151</v>
+        <v>94</v>
       </c>
       <c r="C50">
-        <f>0.3*C49</f>
-        <v>80.23758099352051</v>
+        <v>37</v>
       </c>
       <c r="D50">
-        <f>D48*D49/D46</f>
-        <v>98.811095112391016</v>
-      </c>
-      <c r="E50">
-        <f>C49-C50</f>
-        <v>187.22102231821452</v>
+        <f t="shared" si="17"/>
+        <v>57</v>
+      </c>
+    </row>
+    <row r="51" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A51" t="s">
+        <v>397</v>
+      </c>
+      <c r="B51">
+        <f>SUM(C51:D51)</f>
+        <v>236.5</v>
+      </c>
+      <c r="C51">
+        <v>86.4</v>
+      </c>
+      <c r="D51">
+        <f>(D47/D45)*D49</f>
+        <v>150.1</v>
+      </c>
+      <c r="E51">
+        <f>C51/0.1</f>
+        <v>864</v>
+      </c>
+    </row>
+    <row r="52" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A52" t="s">
+        <v>398</v>
+      </c>
+      <c r="B52">
+        <f>SUM(C52:D52)</f>
+        <v>106.02500000000001</v>
+      </c>
+      <c r="C52">
+        <v>47.6</v>
+      </c>
+      <c r="D52">
+        <f>(D48/D46)*D50</f>
+        <v>58.424999999999997</v>
+      </c>
+      <c r="E52">
+        <f>C52/0.1</f>
+        <v>476</v>
+      </c>
+    </row>
+    <row r="53" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A53" t="s">
+        <v>13</v>
+      </c>
+      <c r="B53">
+        <f>400</f>
+        <v>400</v>
+      </c>
+      <c r="C53">
+        <f>B53*0.75</f>
+        <v>300</v>
+      </c>
+      <c r="D53">
+        <f>0.25*B53</f>
+        <v>100</v>
+      </c>
+      <c r="E53">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="54" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A54" t="s">
+        <v>380</v>
+      </c>
+      <c r="B54">
+        <f>C54+D54</f>
+        <v>136.34146341463415</v>
+      </c>
+      <c r="C54">
+        <f>0.3*C53</f>
+        <v>90</v>
+      </c>
+      <c r="D54">
+        <f>D50*D53/D48</f>
+        <v>46.341463414634148</v>
+      </c>
+      <c r="E54">
+        <f>C53-C54</f>
+        <v>210</v>
       </c>
     </row>
   </sheetData>
@@ -3321,9 +3443,11 @@
   <hyperlinks>
     <hyperlink ref="A40" r:id="rId1" xr:uid="{10A2F329-F7D4-428D-8810-C82B420F96A6}"/>
     <hyperlink ref="A41" r:id="rId2" xr:uid="{39C6E003-BA83-483B-8994-724B3428E1E4}"/>
+    <hyperlink ref="F45" r:id="rId3" xr:uid="{0C77527A-EB26-4897-B8C5-45140E80D9A5}"/>
+    <hyperlink ref="F47" r:id="rId4" xr:uid="{D1E6EA12-4F3B-4CCA-8CA5-BD992BEB908D}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId3"/>
+  <pageSetup orientation="portrait" r:id="rId5"/>
 </worksheet>
 </file>
 
@@ -4565,7 +4689,7 @@
   <dimension ref="A1:R26"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A26" sqref="A26:D26"/>
+      <selection activeCell="F20" sqref="F20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -4594,10 +4718,10 @@
         <v>2025</v>
       </c>
       <c r="D3" s="18"/>
-      <c r="E3" s="29">
+      <c r="E3" s="30">
         <v>2040</v>
       </c>
-      <c r="F3" s="29"/>
+      <c r="F3" s="30"/>
       <c r="G3" t="s">
         <v>272</v>
       </c>
@@ -5298,6 +5422,345 @@
 </worksheet>
 </file>
 
+<file path=xl/worksheets/sheet17.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5AAD7D94-F8EE-45E7-8B7E-34AF298F6BD9}">
+  <dimension ref="A1:G7"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="I29" sqref="I29"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="12.77734375" customWidth="1"/>
+    <col min="2" max="2" width="12" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="10.88671875" customWidth="1"/>
+    <col min="5" max="5" width="10.6640625" customWidth="1"/>
+    <col min="7" max="7" width="10.88671875" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A1" t="s">
+        <v>385</v>
+      </c>
+      <c r="B1">
+        <f>0.000293071</f>
+        <v>2.93071E-4</v>
+      </c>
+      <c r="C1" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A2" t="s">
+        <v>387</v>
+      </c>
+      <c r="B2">
+        <v>1000000</v>
+      </c>
+      <c r="C2" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="B4">
+        <v>2017</v>
+      </c>
+      <c r="D4">
+        <v>2050</v>
+      </c>
+      <c r="F4">
+        <v>2100</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="B5" t="s">
+        <v>386</v>
+      </c>
+      <c r="C5" t="s">
+        <v>34</v>
+      </c>
+      <c r="D5" t="s">
+        <v>386</v>
+      </c>
+      <c r="E5" t="s">
+        <v>34</v>
+      </c>
+      <c r="F5" t="s">
+        <v>386</v>
+      </c>
+      <c r="G5" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A6" t="s">
+        <v>39</v>
+      </c>
+      <c r="B6">
+        <f>10/B2</f>
+        <v>1.0000000000000001E-5</v>
+      </c>
+      <c r="C6">
+        <f>B6/B1</f>
+        <v>3.4121424501230083E-2</v>
+      </c>
+      <c r="F6">
+        <f>40/B2</f>
+        <v>4.0000000000000003E-5</v>
+      </c>
+      <c r="G6">
+        <f>F6/B1</f>
+        <v>0.13648569800492033</v>
+      </c>
+    </row>
+    <row r="7" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A7" t="s">
+        <v>214</v>
+      </c>
+      <c r="B7">
+        <f>12/B2</f>
+        <v>1.2E-5</v>
+      </c>
+      <c r="C7">
+        <f>B7/B1</f>
+        <v>4.0945709401476092E-2</v>
+      </c>
+      <c r="F7">
+        <f>45/B2</f>
+        <v>4.5000000000000003E-5</v>
+      </c>
+      <c r="G7">
+        <f>F7/B1</f>
+        <v>0.15354641025553536</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet18.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A3ADF0EE-DD27-4477-ABAB-E77A2AEA500F}">
+  <dimension ref="A1:G23"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="Z11" sqref="Z11"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetData>
+    <row r="1" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A1" t="s">
+        <v>162</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="D2" t="s">
+        <v>395</v>
+      </c>
+      <c r="E2" t="s">
+        <v>396</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A3" t="s">
+        <v>393</v>
+      </c>
+      <c r="C3">
+        <v>2020</v>
+      </c>
+      <c r="D3" s="29">
+        <f>10.2</f>
+        <v>10.199999999999999</v>
+      </c>
+      <c r="E3">
+        <f>D3*E4/D4</f>
+        <v>24.157894736842099</v>
+      </c>
+      <c r="G3" t="s">
+        <v>394</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A4">
+        <v>180</v>
+      </c>
+      <c r="C4">
+        <v>2030</v>
+      </c>
+      <c r="D4" s="29">
+        <f>26.6</f>
+        <v>26.6</v>
+      </c>
+      <c r="E4">
+        <f>D4*E5/D5</f>
+        <v>63</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="C5">
+        <v>2040</v>
+      </c>
+      <c r="D5">
+        <v>38</v>
+      </c>
+      <c r="E5">
+        <f>D5*E6/D6</f>
+        <v>90</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="C6">
+        <v>2100</v>
+      </c>
+      <c r="D6" s="29">
+        <v>76</v>
+      </c>
+      <c r="E6">
+        <v>180</v>
+      </c>
+    </row>
+    <row r="8" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A8" t="s">
+        <v>401</v>
+      </c>
+    </row>
+    <row r="10" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A10" t="s">
+        <v>393</v>
+      </c>
+      <c r="D10" t="s">
+        <v>395</v>
+      </c>
+      <c r="E10" t="s">
+        <v>396</v>
+      </c>
+    </row>
+    <row r="11" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A11">
+        <v>130</v>
+      </c>
+      <c r="C11">
+        <v>2030</v>
+      </c>
+      <c r="D11" s="29">
+        <v>5.8</v>
+      </c>
+      <c r="E11">
+        <f>D11*E12/D12</f>
+        <v>19.842105263157897</v>
+      </c>
+    </row>
+    <row r="12" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="C12">
+        <v>2040</v>
+      </c>
+      <c r="D12" s="29">
+        <v>15</v>
+      </c>
+      <c r="E12">
+        <f>D12*E13/D13</f>
+        <v>51.315789473684212</v>
+      </c>
+    </row>
+    <row r="13" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="C13">
+        <v>2050</v>
+      </c>
+      <c r="D13" s="29">
+        <v>19</v>
+      </c>
+      <c r="E13">
+        <f>D13*E14/D14</f>
+        <v>65</v>
+      </c>
+    </row>
+    <row r="14" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="C14">
+        <v>2100</v>
+      </c>
+      <c r="D14" s="29">
+        <f>2*D13</f>
+        <v>38</v>
+      </c>
+      <c r="E14">
+        <v>130</v>
+      </c>
+    </row>
+    <row r="17" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A17" t="s">
+        <v>402</v>
+      </c>
+    </row>
+    <row r="19" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A19" t="s">
+        <v>393</v>
+      </c>
+      <c r="D19" t="s">
+        <v>395</v>
+      </c>
+      <c r="E19" t="s">
+        <v>396</v>
+      </c>
+    </row>
+    <row r="20" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A20">
+        <v>260</v>
+      </c>
+      <c r="C20">
+        <v>2030</v>
+      </c>
+      <c r="D20" s="29">
+        <v>3.8</v>
+      </c>
+      <c r="E20">
+        <f>D20*E21/D21</f>
+        <v>27.444444444444446</v>
+      </c>
+    </row>
+    <row r="21" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="C21">
+        <v>2040</v>
+      </c>
+      <c r="D21" s="29">
+        <v>12.9</v>
+      </c>
+      <c r="E21">
+        <f>D21*E22/D22</f>
+        <v>93.166666666666671</v>
+      </c>
+    </row>
+    <row r="22" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="C22">
+        <v>2050</v>
+      </c>
+      <c r="D22" s="29">
+        <v>18</v>
+      </c>
+      <c r="E22">
+        <f>D22*E23/D23</f>
+        <v>130</v>
+      </c>
+    </row>
+    <row r="23" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="C23">
+        <v>2100</v>
+      </c>
+      <c r="D23">
+        <f>2*D22</f>
+        <v>36</v>
+      </c>
+      <c r="E23">
+        <f>A20</f>
+        <v>260</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{341C9435-D140-4ACE-89B8-673675A87D0E}">
   <dimension ref="A1:P44"/>
@@ -5356,15 +5819,15 @@
       <c r="C3" t="s">
         <v>161</v>
       </c>
-      <c r="J3" s="29" t="s">
+      <c r="J3" s="30" t="s">
         <v>188</v>
       </c>
-      <c r="K3" s="29"/>
-      <c r="L3" s="29"/>
-      <c r="M3" s="29"/>
-      <c r="N3" s="29"/>
-      <c r="O3" s="29"/>
-      <c r="P3" s="29"/>
+      <c r="K3" s="30"/>
+      <c r="L3" s="30"/>
+      <c r="M3" s="30"/>
+      <c r="N3" s="30"/>
+      <c r="O3" s="30"/>
+      <c r="P3" s="30"/>
     </row>
     <row r="4" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
@@ -5854,15 +6317,15 @@
       <c r="C17" t="s">
         <v>214</v>
       </c>
-      <c r="J17" s="29" t="s">
+      <c r="J17" s="30" t="s">
         <v>193</v>
       </c>
-      <c r="K17" s="29"/>
-      <c r="L17" s="29"/>
-      <c r="M17" s="29"/>
-      <c r="N17" s="29"/>
-      <c r="O17" s="29"/>
-      <c r="P17" s="29"/>
+      <c r="K17" s="30"/>
+      <c r="L17" s="30"/>
+      <c r="M17" s="30"/>
+      <c r="N17" s="30"/>
+      <c r="O17" s="30"/>
+      <c r="P17" s="30"/>
     </row>
     <row r="18" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A18" s="2" t="s">
@@ -6324,15 +6787,15 @@
       <c r="E31">
         <v>0.7</v>
       </c>
-      <c r="J31" s="29" t="s">
+      <c r="J31" s="30" t="s">
         <v>194</v>
       </c>
-      <c r="K31" s="29"/>
-      <c r="L31" s="29"/>
-      <c r="M31" s="29"/>
-      <c r="N31" s="29"/>
-      <c r="O31" s="29"/>
-      <c r="P31" s="29"/>
+      <c r="K31" s="30"/>
+      <c r="L31" s="30"/>
+      <c r="M31" s="30"/>
+      <c r="N31" s="30"/>
+      <c r="O31" s="30"/>
+      <c r="P31" s="30"/>
     </row>
     <row r="32" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A32" s="2" t="s">
@@ -6979,10 +7442,10 @@
       <c r="G10" t="s">
         <v>91</v>
       </c>
-      <c r="J10" s="30" t="s">
+      <c r="J10" s="31" t="s">
         <v>80</v>
       </c>
-      <c r="K10" s="30"/>
+      <c r="K10" s="31"/>
       <c r="L10" s="11">
         <f>L9/G5</f>
         <v>122583.35123523093</v>
@@ -6992,10 +7455,10 @@
       </c>
     </row>
     <row r="11" spans="1:16" x14ac:dyDescent="0.3">
-      <c r="J11" s="30" t="s">
+      <c r="J11" s="31" t="s">
         <v>81</v>
       </c>
-      <c r="K11" s="30"/>
+      <c r="K11" s="31"/>
       <c r="L11" s="11">
         <f>M4*L10</f>
         <v>4086438.5967776584</v>
@@ -7703,8 +8166,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DB5DFEF8-915B-4056-B382-3EF1CD6D8429}">
   <dimension ref="A1:M39"/>
   <sheetViews>
-    <sheetView topLeftCell="A16" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="A13" sqref="A13:C13"/>
+    <sheetView topLeftCell="A4" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <selection activeCell="B8" sqref="B8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -7818,16 +8281,36 @@
       <c r="C6" t="s">
         <v>3</v>
       </c>
+      <c r="G6" t="s">
+        <v>118</v>
+      </c>
+      <c r="H6">
+        <v>450</v>
+      </c>
+      <c r="I6" t="s">
+        <v>405</v>
+      </c>
     </row>
     <row r="7" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A7" s="14" t="s">
-        <v>109</v>
+        <v>404</v>
       </c>
       <c r="B7" s="14">
+        <f>133.815</f>
         <v>133.815</v>
       </c>
       <c r="C7" s="14" t="s">
         <v>119</v>
+      </c>
+      <c r="G7" t="s">
+        <v>406</v>
+      </c>
+      <c r="H7">
+        <f>0.05*H6</f>
+        <v>22.5</v>
+      </c>
+      <c r="I7" t="s">
+        <v>407</v>
       </c>
     </row>
     <row r="8" spans="1:13" x14ac:dyDescent="0.3">
@@ -7840,6 +8323,13 @@
       <c r="C8" t="s">
         <v>127</v>
       </c>
+      <c r="G8" t="s">
+        <v>17</v>
+      </c>
+      <c r="H8">
+        <f>H6+(H7*B14)</f>
+        <v>900</v>
+      </c>
     </row>
     <row r="9" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
@@ -7847,7 +8337,7 @@
       </c>
       <c r="B9">
         <f>(133815+(B14*70004))*1000</f>
-        <v>2233935000</v>
+        <v>1533895000</v>
       </c>
       <c r="C9" t="s">
         <v>140</v>
@@ -7859,7 +8349,7 @@
       </c>
       <c r="B10">
         <f>B9/B8</f>
-        <v>50656122.448979594</v>
+        <v>34782199.54648526</v>
       </c>
       <c r="C10" t="s">
         <v>138</v>
@@ -7871,7 +8361,7 @@
       </c>
       <c r="B11">
         <f>B10/(B14*1000)</f>
-        <v>1688.5374149659865</v>
+        <v>1739.1099773242629</v>
       </c>
       <c r="C11" t="s">
         <v>117</v>
@@ -7883,7 +8373,7 @@
       </c>
       <c r="B12">
         <f>B11/8760</f>
-        <v>0.19275541266735005</v>
+        <v>0.19852853622423092</v>
       </c>
       <c r="C12" t="s">
         <v>133</v>
@@ -7895,7 +8385,7 @@
       </c>
       <c r="B13" s="15">
         <f>B7*1.1/B12</f>
-        <v>763.64392554841572</v>
+        <v>741.43749205780068</v>
       </c>
       <c r="C13" s="15" t="s">
         <v>134</v>
@@ -7906,10 +8396,13 @@
         <v>35</v>
       </c>
       <c r="B14">
-        <v>30</v>
+        <v>20</v>
       </c>
       <c r="C14" t="s">
         <v>137</v>
+      </c>
+      <c r="D14" s="12" t="s">
+        <v>403</v>
       </c>
     </row>
     <row r="17" spans="1:11" x14ac:dyDescent="0.3">
@@ -7956,7 +8449,7 @@
       </c>
       <c r="D18">
         <f>B18*B14*365*24*3600/1000000000</f>
-        <v>22.705919999999999</v>
+        <v>15.137280000000001</v>
       </c>
     </row>
     <row r="21" spans="1:11" x14ac:dyDescent="0.3">
@@ -8074,7 +8567,7 @@
       </c>
       <c r="F26" s="15">
         <f>D26/B11</f>
-        <v>4.084030751199931E-2</v>
+        <v>3.9652689117928845E-2</v>
       </c>
       <c r="G26" t="s">
         <v>34</v>
@@ -8105,7 +8598,7 @@
       </c>
       <c r="F29" s="15">
         <f>D29/B12</f>
-        <v>6.2146114779525812</v>
+        <v>6.0338932769192164</v>
       </c>
       <c r="G29" t="s">
         <v>134</v>
@@ -8116,13 +8609,56 @@
         <v>154</v>
       </c>
     </row>
-    <row r="37" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A32" s="2" t="s">
+        <v>383</v>
+      </c>
+    </row>
+    <row r="33" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A33" t="s">
+        <v>359</v>
+      </c>
+      <c r="B33">
+        <v>30</v>
+      </c>
+      <c r="C33" t="s">
+        <v>127</v>
+      </c>
+    </row>
+    <row r="34" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A34" t="s">
+        <v>384</v>
+      </c>
+      <c r="B34">
+        <v>1064000</v>
+      </c>
+      <c r="C34" t="s">
+        <v>125</v>
+      </c>
+      <c r="D34">
+        <f>B34/(B33*1000)</f>
+        <v>35.466666666666669</v>
+      </c>
+      <c r="E34" t="s">
+        <v>117</v>
+      </c>
+    </row>
+    <row r="35" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A35" t="s">
+        <v>383</v>
+      </c>
+      <c r="B35" s="15">
+        <f>D34/(F22+D34)</f>
+        <v>1.1356177322866581E-2</v>
+      </c>
+    </row>
+    <row r="37" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A37" s="2"/>
     </row>
-    <row r="38" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="38" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A38" s="2"/>
     </row>
-    <row r="39" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="39" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A39" s="23"/>
       <c r="B39" s="22"/>
       <c r="C39" s="22"/>
@@ -8131,9 +8667,10 @@
   </sheetData>
   <hyperlinks>
     <hyperlink ref="M1" r:id="rId1" xr:uid="{E2B26766-48C9-476C-9577-B9DD82383664}"/>
+    <hyperlink ref="D14" r:id="rId2" xr:uid="{C435BC4A-77B0-4536-9CEB-EFCBE8814B4A}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId2"/>
+  <pageSetup orientation="portrait" r:id="rId3"/>
 </worksheet>
 </file>
 
@@ -8142,7 +8679,7 @@
   <dimension ref="A1:Q35"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="M22" sqref="M22"/>
+      <selection activeCell="O18" sqref="O18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -8434,7 +8971,7 @@
       </c>
       <c r="O12">
         <f>(133815+(O17*70004))*1000</f>
-        <v>2233935000</v>
+        <v>1533895000</v>
       </c>
       <c r="P12" t="s">
         <v>140</v>
@@ -8462,7 +8999,7 @@
       </c>
       <c r="O13">
         <f>O12/O11</f>
-        <v>39191842.105263159</v>
+        <v>26910438.596491229</v>
       </c>
       <c r="P13" t="s">
         <v>138</v>
@@ -8484,7 +9021,7 @@
       </c>
       <c r="O14">
         <f>O13/(O17*1000)</f>
-        <v>1306.3947368421052</v>
+        <v>1345.5219298245615</v>
       </c>
       <c r="P14" t="s">
         <v>117</v>
@@ -8497,7 +9034,7 @@
       </c>
       <c r="O15">
         <f>O14/8760</f>
-        <v>0.14913181927421293</v>
+        <v>0.15359839381558921</v>
       </c>
       <c r="P15" t="s">
         <v>133</v>
@@ -8518,7 +9055,7 @@
       </c>
       <c r="O16" s="15">
         <f>O10*1.1/O15</f>
-        <v>1194.9160203855529</v>
+        <v>1160.1683817992757</v>
       </c>
       <c r="P16" s="15" t="s">
         <v>134</v>
@@ -8537,7 +9074,7 @@
         <v>35</v>
       </c>
       <c r="O17">
-        <v>30</v>
+        <v>20</v>
       </c>
       <c r="P17" t="s">
         <v>137</v>
@@ -8586,7 +9123,7 @@
       </c>
       <c r="F20" s="15">
         <f>D20/O14</f>
-        <v>5.5138531441766954E-2</v>
+        <v>5.3535126909540154E-2</v>
       </c>
       <c r="G20" t="s">
         <v>34</v>
@@ -8617,7 +9154,7 @@
       </c>
       <c r="F23" s="15">
         <f>D23/O15</f>
-        <v>8.0324910259251059</v>
+        <v>7.7989096776506859</v>
       </c>
       <c r="G23" t="s">
         <v>134</v>
@@ -8665,7 +9202,7 @@
   <dimension ref="A1:P31"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="J1" sqref="J1:K1"/>
+      <selection activeCell="J40" sqref="J40"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>

</xml_diff>

<commit_message>
added litreview, alkaline ec emissions
Former-commit-id: 81773bfdbeecdc359b7a7412964d263f0e91909e
Former-commit-id: 0f7abe6bc99effe150dff7bfb589ed72662fb65a
</commit_message>
<xml_diff>
--- a/data/tech-economic-data.xlsx
+++ b/data/tech-economic-data.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\github\i2cner\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F5950392-763F-4B3A-9576-BF21698557BA}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3F19CD19-5D95-4B5A-894A-6F0C07CA95BC}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{ECBC9880-2B97-44EA-9887-629A306A84A1}"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" firstSheet="4" activeTab="10" xr2:uid="{ECBC9880-2B97-44EA-9887-629A306A84A1}"/>
   </bookViews>
   <sheets>
     <sheet name="CCS_Costs_Early" sheetId="14" r:id="rId1"/>
@@ -1817,8 +1817,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DA3B25EB-4023-477D-80C4-74718858ACC8}">
   <dimension ref="A1:P54"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A22" workbookViewId="0">
-      <selection activeCell="J50" sqref="J50"/>
+    <sheetView topLeftCell="A22" workbookViewId="0">
+      <selection activeCell="E51" sqref="E51"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -3337,6 +3337,10 @@
         <f t="shared" si="17"/>
         <v>114</v>
       </c>
+      <c r="E49">
+        <f>0.9*C45</f>
+        <v>684</v>
+      </c>
     </row>
     <row r="50" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A50" t="s">
@@ -3351,6 +3355,10 @@
       <c r="D50">
         <f t="shared" si="17"/>
         <v>57</v>
+      </c>
+      <c r="E50">
+        <f>0.9*(C50/0.1)</f>
+        <v>333</v>
       </c>
     </row>
     <row r="51" spans="1:5" x14ac:dyDescent="0.3">
@@ -3644,8 +3652,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9B6BC44C-C965-493C-907E-B5E15FE8A950}">
   <dimension ref="A1:M14"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="L1" sqref="L1:M1"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C3" sqref="C3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -9603,7 +9611,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2E6C6BEB-6091-4743-A766-86BDD24D0263}">
   <dimension ref="A1:J29"/>
   <sheetViews>
-    <sheetView topLeftCell="A13" zoomScale="175" zoomScaleNormal="175" workbookViewId="0">
+    <sheetView topLeftCell="A10" zoomScale="175" zoomScaleNormal="175" workbookViewId="0">
       <selection activeCell="B24" sqref="B24"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
added pws capacity factor
Former-commit-id: ef1132612ec949e6d38c329589843b014e6f8087
Former-commit-id: 23dd5676499da8d401ff9bfab0308be51139a606
</commit_message>
<xml_diff>
--- a/data/tech-economic-data.xlsx
+++ b/data/tech-economic-data.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21929"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22527"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\github\i2cner\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3F19CD19-5D95-4B5A-894A-6F0C07CA95BC}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FDAE0CDF-10F6-49B5-B5E5-CCAFD454E86B}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" firstSheet="4" activeTab="10" xr2:uid="{ECBC9880-2B97-44EA-9887-629A306A84A1}"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" firstSheet="11" activeTab="15" xr2:uid="{ECBC9880-2B97-44EA-9887-629A306A84A1}"/>
   </bookViews>
   <sheets>
     <sheet name="CCS_Costs_Early" sheetId="14" r:id="rId1"/>
@@ -40,7 +40,9 @@
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
       <xcalcf:calcFeatures>
         <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
         <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
       </xcalcf:calcFeatures>
     </ext>
   </extLst>
@@ -48,7 +50,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="805" uniqueCount="408">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="810" uniqueCount="412">
   <si>
     <t>H2 Method</t>
   </si>
@@ -1142,12 +1144,6 @@
     <t>EUR/a</t>
   </si>
   <si>
-    <t>Correction factors</t>
-  </si>
-  <si>
-    <t>CF1</t>
-  </si>
-  <si>
     <t>Reported H2 Cost</t>
   </si>
   <si>
@@ -1272,6 +1268,24 @@
   </si>
   <si>
     <t>Eur/kw/y</t>
+  </si>
+  <si>
+    <t>analogous to avg annual capacity factor</t>
+  </si>
+  <si>
+    <t>added to match $/kg-H2 cost from paper</t>
+  </si>
+  <si>
+    <t>Theo max cap</t>
+  </si>
+  <si>
+    <t>Correction factor</t>
+  </si>
+  <si>
+    <t>True CF</t>
+  </si>
+  <si>
+    <t>during day time</t>
   </si>
 </sst>
 </file>
@@ -3018,7 +3032,7 @@
         <v>62</v>
       </c>
       <c r="D37" t="s">
-        <v>379</v>
+        <v>377</v>
       </c>
       <c r="J37" s="3">
         <v>0.88</v>
@@ -3212,19 +3226,19 @@
     </row>
     <row r="44" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A44" t="s">
+        <v>374</v>
+      </c>
+      <c r="B44" t="s">
+        <v>375</v>
+      </c>
+      <c r="C44" t="s">
         <v>376</v>
       </c>
-      <c r="B44" t="s">
-        <v>377</v>
-      </c>
-      <c r="C44" t="s">
-        <v>378</v>
-      </c>
       <c r="D44" t="s">
-        <v>382</v>
+        <v>380</v>
       </c>
       <c r="E44" t="s">
-        <v>381</v>
+        <v>379</v>
       </c>
       <c r="J44" s="3">
         <v>0.95</v>
@@ -3253,7 +3267,7 @@
     </row>
     <row r="45" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A45" t="s">
-        <v>399</v>
+        <v>397</v>
       </c>
       <c r="B45">
         <v>820</v>
@@ -3266,12 +3280,12 @@
         <v>60</v>
       </c>
       <c r="F45" s="12" t="s">
-        <v>388</v>
+        <v>386</v>
       </c>
     </row>
     <row r="46" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A46" t="s">
-        <v>400</v>
+        <v>398</v>
       </c>
       <c r="B46">
         <v>490</v>
@@ -3286,7 +3300,7 @@
     </row>
     <row r="47" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A47" t="s">
-        <v>389</v>
+        <v>387</v>
       </c>
       <c r="B47">
         <v>943</v>
@@ -3302,12 +3316,12 @@
         <v>0</v>
       </c>
       <c r="F47" s="12" t="s">
-        <v>375</v>
+        <v>373</v>
       </c>
     </row>
     <row r="48" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A48" t="s">
-        <v>390</v>
+        <v>388</v>
       </c>
       <c r="B48">
         <v>599</v>
@@ -3325,7 +3339,7 @@
     </row>
     <row r="49" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A49" t="s">
-        <v>391</v>
+        <v>389</v>
       </c>
       <c r="B49">
         <v>190</v>
@@ -3344,7 +3358,7 @@
     </row>
     <row r="50" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A50" t="s">
-        <v>392</v>
+        <v>390</v>
       </c>
       <c r="B50">
         <v>94</v>
@@ -3363,7 +3377,7 @@
     </row>
     <row r="51" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A51" t="s">
-        <v>397</v>
+        <v>395</v>
       </c>
       <c r="B51">
         <f>SUM(C51:D51)</f>
@@ -3383,7 +3397,7 @@
     </row>
     <row r="52" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A52" t="s">
-        <v>398</v>
+        <v>396</v>
       </c>
       <c r="B52">
         <f>SUM(C52:D52)</f>
@@ -3423,7 +3437,7 @@
     </row>
     <row r="54" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A54" t="s">
-        <v>380</v>
+        <v>378</v>
       </c>
       <c r="B54">
         <f>C54+D54</f>
@@ -3652,8 +3666,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9B6BC44C-C965-493C-907E-B5E15FE8A950}">
   <dimension ref="A1:M14"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C3" sqref="C3"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="L31" sqref="L31"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -3771,7 +3785,7 @@
   <dimension ref="A1:P30"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="G16" sqref="G16"/>
+      <selection activeCell="B13" sqref="B13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -3950,14 +3964,14 @@
         <v>2050</v>
       </c>
       <c r="K12">
-        <v>1000</v>
+        <v>1250</v>
       </c>
       <c r="L12" t="s">
         <v>322</v>
       </c>
       <c r="M12">
         <f t="shared" si="1"/>
-        <v>1110</v>
+        <v>1387.5000000000002</v>
       </c>
       <c r="N12" t="s">
         <v>323</v>
@@ -5091,19 +5105,20 @@
 
 <file path=xl/worksheets/sheet16.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{403B81F9-D657-42BD-96F8-D40A873BAE34}">
-  <dimension ref="A1:L24"/>
+  <dimension ref="A1:L27"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="O5" sqref="O5"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D11" sqref="D11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="17.5546875" customWidth="1"/>
     <col min="2" max="2" width="13.88671875" customWidth="1"/>
+    <col min="3" max="3" width="11" customWidth="1"/>
     <col min="4" max="4" width="10" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="12" bestFit="1" customWidth="1"/>
-    <col min="10" max="11" width="11" bestFit="1" customWidth="1"/>
+    <col min="9" max="10" width="12" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="11" bestFit="1" customWidth="1"/>
     <col min="12" max="12" width="12" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
@@ -5189,122 +5204,123 @@
         <v>234</v>
       </c>
     </row>
-    <row r="8" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="B8" t="s">
-        <v>365</v>
-      </c>
-    </row>
     <row r="9" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
-        <v>364</v>
+        <v>409</v>
       </c>
       <c r="B9">
         <v>0.21</v>
       </c>
+      <c r="D9" t="s">
+        <v>406</v>
+      </c>
+      <c r="H9" t="s">
+        <v>407</v>
+      </c>
     </row>
     <row r="10" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
-        <v>161</v>
+        <v>107</v>
       </c>
       <c r="B10">
-        <v>0.9</v>
+        <v>1</v>
+      </c>
+      <c r="D10" t="s">
+        <v>411</v>
       </c>
     </row>
     <row r="11" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
-        <v>35</v>
+        <v>410</v>
       </c>
       <c r="B11">
-        <v>20</v>
-      </c>
-      <c r="C11" t="s">
-        <v>137</v>
+        <f>B10*B9</f>
+        <v>0.21</v>
       </c>
     </row>
     <row r="12" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
+        <v>35</v>
+      </c>
+      <c r="B12">
+        <v>20</v>
+      </c>
+      <c r="C12" t="s">
+        <v>137</v>
+      </c>
+    </row>
+    <row r="13" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A13" t="s">
         <v>228</v>
       </c>
-      <c r="B12">
+      <c r="B13">
         <v>1000</v>
       </c>
-      <c r="C12" t="s">
+      <c r="C13" t="s">
         <v>229</v>
       </c>
-      <c r="D12">
-        <f>365.25*B12*B10*B9</f>
-        <v>69032.25</v>
-      </c>
-      <c r="E12" t="s">
+      <c r="D13">
+        <f>365.25*B13*B10*B9</f>
+        <v>76702.5</v>
+      </c>
+      <c r="E13" t="s">
         <v>230</v>
       </c>
-      <c r="F12">
-        <f>D12*B11</f>
-        <v>1380645</v>
-      </c>
-      <c r="G12" t="s">
+      <c r="F13">
+        <f>D13*B12</f>
+        <v>1534050</v>
+      </c>
+      <c r="G13" t="s">
         <v>231</v>
       </c>
     </row>
-    <row r="13" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="B13">
-        <f>33.33*D12/1000000</f>
-        <v>2.3008448925000002</v>
-      </c>
-      <c r="C13" t="s">
+    <row r="14" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="B14">
+        <f>33.33*D13/1000000</f>
+        <v>2.5564943249999996</v>
+      </c>
+      <c r="C14" t="s">
         <v>239</v>
       </c>
-      <c r="D13">
-        <f>B13*B11</f>
-        <v>46.016897850000007</v>
-      </c>
-      <c r="E13" t="s">
+      <c r="D14">
+        <f>B14*B12</f>
+        <v>51.129886499999991</v>
+      </c>
+      <c r="E14" t="s">
         <v>240</v>
       </c>
     </row>
-    <row r="14" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A14" t="s">
+    <row r="15" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A15" t="s">
+        <v>408</v>
+      </c>
+      <c r="B15">
+        <f>B13*365.25*33.33/(8760*1000000)</f>
+        <v>1.389701198630137E-3</v>
+      </c>
+      <c r="C15" t="s">
+        <v>133</v>
+      </c>
+    </row>
+    <row r="16" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A16" t="s">
         <v>232</v>
       </c>
-      <c r="B14">
+      <c r="B16">
         <f>222881/1000000</f>
         <v>0.222881</v>
       </c>
-      <c r="C14" t="s">
+      <c r="C16" t="s">
         <v>233</v>
-      </c>
-    </row>
-    <row r="15" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A15" t="s">
-        <v>235</v>
-      </c>
-      <c r="B15">
-        <f>B13/(8760*B10)</f>
-        <v>2.918372517123288E-4</v>
-      </c>
-      <c r="C15" t="s">
-        <v>133</v>
-      </c>
-    </row>
-    <row r="16" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A16" t="s">
-        <v>236</v>
-      </c>
-      <c r="B16">
-        <f>B14/B15</f>
-        <v>763.71675888621417</v>
-      </c>
-      <c r="C16" t="s">
-        <v>226</v>
       </c>
     </row>
     <row r="17" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A17" t="s">
-        <v>241</v>
+        <v>235</v>
       </c>
       <c r="B17">
-        <f>B6/B16</f>
-        <v>16.432793773312781</v>
+        <f>1000*365.25*33.33/(8760*1000000)</f>
+        <v>1.389701198630137E-3</v>
       </c>
       <c r="C17" t="s">
         <v>133</v>
@@ -5312,118 +5328,142 @@
     </row>
     <row r="18" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A18" t="s">
+        <v>236</v>
+      </c>
+      <c r="B18">
+        <f>B16/B17</f>
+        <v>160.38051936610498</v>
+      </c>
+      <c r="C18" t="s">
+        <v>226</v>
+      </c>
+    </row>
+    <row r="19" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A19" t="s">
+        <v>241</v>
+      </c>
+      <c r="B19">
+        <f>B6/B18</f>
+        <v>78.251398920537056</v>
+      </c>
+      <c r="C19" t="s">
+        <v>133</v>
+      </c>
+    </row>
+    <row r="20" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A20" t="s">
         <v>86</v>
       </c>
-      <c r="B18">
+      <c r="B20">
         <f>4.291722</f>
         <v>4.291722</v>
       </c>
-      <c r="C18" t="s">
+      <c r="C20" t="s">
         <v>51</v>
       </c>
-      <c r="I18" t="s">
-        <v>373</v>
-      </c>
-    </row>
-    <row r="19" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A19" t="s">
-        <v>118</v>
-      </c>
-      <c r="B19">
-        <f>B18/B15</f>
-        <v>14705.874506488488</v>
-      </c>
-      <c r="C19" t="s">
-        <v>134</v>
-      </c>
-      <c r="I19" t="s">
-        <v>370</v>
-      </c>
-      <c r="J19" t="s">
-        <v>372</v>
-      </c>
-      <c r="K19" t="s">
+      <c r="I20" t="s">
         <v>371</v>
-      </c>
-      <c r="L19" t="s">
-        <v>243</v>
-      </c>
-    </row>
-    <row r="20" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A20" t="s">
-        <v>238</v>
-      </c>
-      <c r="B20">
-        <f>(B18*1000000)/F12</f>
-        <v>3.1084905967862846</v>
-      </c>
-      <c r="C20" t="s">
-        <v>110</v>
-      </c>
-      <c r="E20" t="s">
-        <v>242</v>
-      </c>
-      <c r="F20">
-        <v>3</v>
-      </c>
-      <c r="G20" t="s">
-        <v>243</v>
-      </c>
-      <c r="I20">
-        <f>(B19+(B22*B11))*1000000</f>
-        <v>19607832675.317982</v>
-      </c>
-      <c r="J20">
-        <f>B11*8760*B10*1000000</f>
-        <v>157680000000</v>
-      </c>
-      <c r="K20">
-        <f>J20/33.33</f>
-        <v>4730873087.3087311</v>
-      </c>
-      <c r="L20">
-        <f>I20/K20</f>
-        <v>4.1446541290483783</v>
       </c>
     </row>
     <row r="21" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A21" t="s">
+        <v>118</v>
+      </c>
+      <c r="B21">
+        <f>B20/B17</f>
+        <v>3088.2336463625829</v>
+      </c>
+      <c r="C21" t="s">
+        <v>134</v>
+      </c>
+      <c r="I21" t="s">
+        <v>368</v>
+      </c>
+      <c r="J21" t="s">
+        <v>370</v>
+      </c>
+      <c r="K21" t="s">
+        <v>369</v>
+      </c>
+      <c r="L21" t="s">
+        <v>243</v>
+      </c>
+    </row>
+    <row r="22" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A22" t="s">
+        <v>238</v>
+      </c>
+      <c r="B22">
+        <f>(B20*1000000)/F13</f>
+        <v>2.7976415371076562</v>
+      </c>
+      <c r="C22" t="s">
+        <v>110</v>
+      </c>
+      <c r="E22" t="s">
+        <v>242</v>
+      </c>
+      <c r="F22">
+        <v>3</v>
+      </c>
+      <c r="G22" t="s">
+        <v>243</v>
+      </c>
+      <c r="I22">
+        <f>(B21+(B24*B12))*1000000</f>
+        <v>4117644861.8167777</v>
+      </c>
+      <c r="J22">
+        <f>B12*8760*B10*B9*1000000</f>
+        <v>36792000000</v>
+      </c>
+      <c r="K22">
+        <f>J22/33.33</f>
+        <v>1103870387.0387039</v>
+      </c>
+      <c r="L22">
+        <f>I22/K22</f>
+        <v>3.7301887161435419</v>
+      </c>
+    </row>
+    <row r="23" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A23" t="s">
         <v>146</v>
       </c>
-      <c r="B21">
-        <f>F12*F21/(1000000*B11*B15)</f>
-        <v>236.54365436543651</v>
-      </c>
-      <c r="C21" t="s">
+      <c r="B23">
+        <f>F13*F23/(1000000*B12*B17)</f>
+        <v>55.193519351935194</v>
+      </c>
+      <c r="C23" t="s">
         <v>244</v>
       </c>
-      <c r="E21" t="s">
+      <c r="E23" t="s">
         <v>242</v>
       </c>
-      <c r="F21">
+      <c r="F23">
         <v>1</v>
       </c>
-      <c r="G21" t="s">
+      <c r="G23" t="s">
         <v>243</v>
       </c>
     </row>
-    <row r="22" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="B22">
-        <f>B19/(3*B11)</f>
-        <v>245.0979084414748</v>
-      </c>
-    </row>
-    <row r="23" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A23" s="12" t="s">
+    <row r="24" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="B24">
+        <f>B21/(3*B12)</f>
+        <v>51.470560772709717</v>
+      </c>
+    </row>
+    <row r="26" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A26" s="12" t="s">
         <v>258</v>
       </c>
     </row>
-    <row r="24" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="B24" s="12"/>
+    <row r="27" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="B27" s="12"/>
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="A23" r:id="rId1" location="!divAbstract" display="https://pubs.rsc.org/en/content/articlelanding/2013/ee/c3ee40831k - !divAbstract" xr:uid="{92883294-6EE4-4414-BC11-4CB1313D14CB}"/>
+    <hyperlink ref="A26" r:id="rId1" location="!divAbstract" display="https://pubs.rsc.org/en/content/articlelanding/2013/ee/c3ee40831k - !divAbstract" xr:uid="{92883294-6EE4-4414-BC11-4CB1313D14CB}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId2"/>
@@ -5449,7 +5489,7 @@
   <sheetData>
     <row r="1" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
-        <v>385</v>
+        <v>383</v>
       </c>
       <c r="B1">
         <f>0.000293071</f>
@@ -5461,7 +5501,7 @@
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
-        <v>387</v>
+        <v>385</v>
       </c>
       <c r="B2">
         <v>1000000</v>
@@ -5483,19 +5523,19 @@
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.3">
       <c r="B5" t="s">
-        <v>386</v>
+        <v>384</v>
       </c>
       <c r="C5" t="s">
         <v>34</v>
       </c>
       <c r="D5" t="s">
-        <v>386</v>
+        <v>384</v>
       </c>
       <c r="E5" t="s">
         <v>34</v>
       </c>
       <c r="F5" t="s">
-        <v>386</v>
+        <v>384</v>
       </c>
       <c r="G5" t="s">
         <v>34</v>
@@ -5565,15 +5605,15 @@
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.3">
       <c r="D2" t="s">
-        <v>395</v>
+        <v>393</v>
       </c>
       <c r="E2" t="s">
-        <v>396</v>
+        <v>394</v>
       </c>
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
-        <v>393</v>
+        <v>391</v>
       </c>
       <c r="C3">
         <v>2020</v>
@@ -5587,7 +5627,7 @@
         <v>24.157894736842099</v>
       </c>
       <c r="G3" t="s">
-        <v>394</v>
+        <v>392</v>
       </c>
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.3">
@@ -5631,18 +5671,18 @@
     </row>
     <row r="8" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
-        <v>401</v>
+        <v>399</v>
       </c>
     </row>
     <row r="10" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
+        <v>391</v>
+      </c>
+      <c r="D10" t="s">
         <v>393</v>
       </c>
-      <c r="D10" t="s">
-        <v>395</v>
-      </c>
       <c r="E10" t="s">
-        <v>396</v>
+        <v>394</v>
       </c>
     </row>
     <row r="11" spans="1:7" x14ac:dyDescent="0.3">
@@ -5698,18 +5738,18 @@
     </row>
     <row r="17" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A17" t="s">
-        <v>402</v>
+        <v>400</v>
       </c>
     </row>
     <row r="19" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A19" t="s">
+        <v>391</v>
+      </c>
+      <c r="D19" t="s">
         <v>393</v>
       </c>
-      <c r="D19" t="s">
-        <v>395</v>
-      </c>
       <c r="E19" t="s">
-        <v>396</v>
+        <v>394</v>
       </c>
     </row>
     <row r="20" spans="1:5" x14ac:dyDescent="0.3">
@@ -8277,7 +8317,7 @@
         <v>3</v>
       </c>
       <c r="D5" t="s">
-        <v>374</v>
+        <v>372</v>
       </c>
     </row>
     <row r="6" spans="1:13" x14ac:dyDescent="0.3">
@@ -8296,12 +8336,12 @@
         <v>450</v>
       </c>
       <c r="I6" t="s">
-        <v>405</v>
+        <v>403</v>
       </c>
     </row>
     <row r="7" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A7" s="14" t="s">
-        <v>404</v>
+        <v>402</v>
       </c>
       <c r="B7" s="14">
         <f>133.815</f>
@@ -8311,19 +8351,19 @@
         <v>119</v>
       </c>
       <c r="G7" t="s">
-        <v>406</v>
+        <v>404</v>
       </c>
       <c r="H7">
         <f>0.05*H6</f>
         <v>22.5</v>
       </c>
       <c r="I7" t="s">
-        <v>407</v>
+        <v>405</v>
       </c>
     </row>
     <row r="8" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
-        <v>366</v>
+        <v>364</v>
       </c>
       <c r="B8">
         <v>44.1</v>
@@ -8410,7 +8450,7 @@
         <v>137</v>
       </c>
       <c r="D14" s="12" t="s">
-        <v>403</v>
+        <v>401</v>
       </c>
     </row>
     <row r="17" spans="1:11" x14ac:dyDescent="0.3">
@@ -8619,7 +8659,7 @@
     </row>
     <row r="32" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A32" s="2" t="s">
-        <v>383</v>
+        <v>381</v>
       </c>
     </row>
     <row r="33" spans="1:5" x14ac:dyDescent="0.3">
@@ -8635,7 +8675,7 @@
     </row>
     <row r="34" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A34" t="s">
-        <v>384</v>
+        <v>382</v>
       </c>
       <c r="B34">
         <v>1064000</v>
@@ -8653,7 +8693,7 @@
     </row>
     <row r="35" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A35" t="s">
-        <v>383</v>
+        <v>381</v>
       </c>
       <c r="B35" s="15">
         <f>D34/(F22+D34)</f>
@@ -8867,7 +8907,7 @@
         <v>3</v>
       </c>
       <c r="Q8" t="s">
-        <v>374</v>
+        <v>372</v>
       </c>
     </row>
     <row r="9" spans="1:17" x14ac:dyDescent="0.3">
@@ -8964,7 +9004,7 @@
         <v>22</v>
       </c>
       <c r="N11" t="s">
-        <v>366</v>
+        <v>364</v>
       </c>
       <c r="O11">
         <v>57</v>
@@ -9399,7 +9439,7 @@
         <v>148</v>
       </c>
       <c r="B13" t="s">
-        <v>367</v>
+        <v>365</v>
       </c>
     </row>
     <row r="14" spans="1:16" x14ac:dyDescent="0.3">
@@ -9566,7 +9606,7 @@
     </row>
     <row r="29" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A29" s="2" t="s">
-        <v>368</v>
+        <v>366</v>
       </c>
       <c r="B29">
         <f>B27/(B28*1000)</f>
@@ -9585,7 +9625,7 @@
     </row>
     <row r="30" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A30" s="2" t="s">
-        <v>369</v>
+        <v>367</v>
       </c>
       <c r="B30">
         <f>D29/(8760*0.9)</f>
@@ -9611,7 +9651,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2E6C6BEB-6091-4743-A766-86BDD24D0263}">
   <dimension ref="A1:J29"/>
   <sheetViews>
-    <sheetView topLeftCell="A10" zoomScale="175" zoomScaleNormal="175" workbookViewId="0">
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
       <selection activeCell="B24" sqref="B24"/>
     </sheetView>
   </sheetViews>

</xml_diff>